<commit_message>
Updated the test cases to include write to excel utility
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
+++ b/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
@@ -1,25 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\auto\sahi_pro\userdata\scripts\Sahi_Project\svmx\test_lab\test_cases\optimax\op_excleData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11115" windowHeight="4650" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="User_Details" sheetId="1" r:id="rId1"/>
     <sheet name="Dispatch_Process" sheetId="4" r:id="rId2"/>
-    <sheet name="RS_6299_RS_6300" sheetId="2" r:id="rId3"/>
-    <sheet name="RS_6665" sheetId="3" r:id="rId4"/>
+    <sheet name="MTTS" sheetId="5" r:id="rId3"/>
+    <sheet name="Territory" sheetId="6" r:id="rId4"/>
+    <sheet name="RS_6299_RS_6300" sheetId="2" r:id="rId5"/>
+    <sheet name="RS_6665" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:K13"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="75">
   <si>
     <t>UserName</t>
   </si>
@@ -234,12 +232,31 @@
   </si>
   <si>
     <t>AM load testing</t>
+  </si>
+  <si>
+    <t>MTTS Name</t>
+  </si>
+  <si>
+    <t>MTTSRule_Wed Oct 04 2017 14:13:01 GMT+0530 (IST)</t>
+  </si>
+  <si>
+    <t>MTTSRule_Wed Oct 04 2017 14:17:09 GMT+0530 (IST)</t>
+  </si>
+  <si>
+    <t>MTTSRule_Wed Oct 04 2017 14:24:25 GMT+0530 (IST)</t>
+  </si>
+  <si>
+    <t>Territory Name</t>
+  </si>
+  <si>
+    <t>TerritoryRule_Wed Oct 04 2017 14:41:41 GMT+0530 (IST)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -612,9 +629,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="26.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -652,15 +669,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -692,6 +709,71 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="47.85546875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:1" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="false"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -701,9 +783,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="30.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -745,7 +827,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L19"/>
   <sheetViews>
@@ -755,13 +837,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="4" width="24.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="25.28515625" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" customWidth="1"/>
-    <col min="12" max="12" width="30.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="2" max="4" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="30.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated the automation sheet for datacreation
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
+++ b/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
@@ -3,21 +3,26 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\auto\sahi_pro\userdata\scripts\Sahi_Project\svmx\test_lab\test_cases\optimax\op_excleData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11115" windowHeight="4650" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11115" windowHeight="4650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="User_Details" sheetId="1" r:id="rId1"/>
-    <sheet name="Dispatch_Process" sheetId="4" r:id="rId2"/>
-    <sheet name="MTTS" sheetId="5" r:id="rId3"/>
-    <sheet name="TerritoryRule" sheetId="6" r:id="rId4"/>
-    <sheet name="RS_6299_RS_6300" sheetId="2" r:id="rId5"/>
-    <sheet name="RS_6665" sheetId="3" r:id="rId6"/>
+    <sheet name="BusinessHours" sheetId="7" r:id="rId2"/>
+    <sheet name="Dispatch_Process" sheetId="4" r:id="rId3"/>
+    <sheet name="MTTS" sheetId="5" r:id="rId4"/>
+    <sheet name="TerritoryRule" sheetId="6" r:id="rId5"/>
+    <sheet name="RS_6299_RS_6300" sheetId="2" r:id="rId6"/>
+    <sheet name="RS_6665" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:K13"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="95">
   <si>
     <t>UserName</t>
   </si>
@@ -244,14 +249,79 @@
   </si>
   <si>
     <t>TerritoryRule_Thu Oct 05 2017 12:13:54 GMT+0530 (IST)</t>
+  </si>
+  <si>
+    <t>FridayEndTime</t>
+  </si>
+  <si>
+    <t>FridayStartTime</t>
+  </si>
+  <si>
+    <t>IsActive</t>
+  </si>
+  <si>
+    <t>MondayEndTime</t>
+  </si>
+  <si>
+    <t>MondayStartTime</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>SaturdayEndTime</t>
+  </si>
+  <si>
+    <t>SaturdayStartTime</t>
+  </si>
+  <si>
+    <t>SundayEndTime</t>
+  </si>
+  <si>
+    <t>SundayStartTime</t>
+  </si>
+  <si>
+    <t>ThursdayEndTime</t>
+  </si>
+  <si>
+    <t>ThursdayStartTime</t>
+  </si>
+  <si>
+    <t>TimeZoneSidKey</t>
+  </si>
+  <si>
+    <t>TuesdayEndTime</t>
+  </si>
+  <si>
+    <t>TuesdayStartTime</t>
+  </si>
+  <si>
+    <t>WednesdayEndTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WednesdayStartTime </t>
+  </si>
+  <si>
+    <t>PST -7 BH - CA</t>
+  </si>
+  <si>
+    <t>America/Los_Angeles</t>
+  </si>
+  <si>
+    <t>09:00:00.000Z</t>
+  </si>
+  <si>
+    <t>18:00:00.000Z</t>
+  </si>
+  <si>
+    <t>Id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,6 +341,12 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -295,11 +371,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -623,9 +700,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="34.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="26.5703125" collapsed="true"/>
+    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -661,6 +738,144 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" customWidth="1"/>
+    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.42578125" customWidth="1"/>
+    <col min="17" max="17" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M1" t="s">
+        <v>73</v>
+      </c>
+      <c r="N1" t="s">
+        <v>80</v>
+      </c>
+      <c r="O1" t="s">
+        <v>79</v>
+      </c>
+      <c r="P1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>81</v>
+      </c>
+      <c r="R1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -669,9 +884,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -702,15 +917,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="1" max="1" width="47" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -718,35 +935,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>71</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -755,6 +946,32 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="50" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -764,9 +981,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="30.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -808,7 +1025,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L19"/>
   <sheetViews>
@@ -818,13 +1035,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="2" max="4" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="1" max="1" width="23" customWidth="1" collapsed="1"/>
+    <col min="2" max="4" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="34.42578125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="30.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
RS_6321 and RS_6322 completed
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
+++ b/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
@@ -4,22 +4,23 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11115" windowHeight="4650" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11115" windowHeight="4650" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="User_Details" sheetId="1" r:id="rId1"/>
     <sheet name="BusinessHours" sheetId="7" r:id="rId2"/>
     <sheet name="Territory" sheetId="8" r:id="rId3"/>
-    <sheet name="Dispatch_Process" sheetId="4" r:id="rId4"/>
-    <sheet name="MTTS" sheetId="5" r:id="rId5"/>
-    <sheet name="TerritoryRule" sheetId="6" r:id="rId6"/>
-    <sheet name="RS_6299_RS_6300" sheetId="2" r:id="rId7"/>
-    <sheet name="RS_6665" sheetId="3" r:id="rId8"/>
+    <sheet name="ChildTerritory" sheetId="9" r:id="rId4"/>
+    <sheet name="Dispatch_Process" sheetId="4" r:id="rId5"/>
+    <sheet name="MTTS" sheetId="5" r:id="rId6"/>
+    <sheet name="TerritoryRule" sheetId="6" r:id="rId7"/>
+    <sheet name="RS_6299_RS_6300" sheetId="2" r:id="rId8"/>
+    <sheet name="RS_6665" sheetId="3" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
   <oleSize ref="A1:K13"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="105">
   <si>
     <t>UserName</t>
   </si>
@@ -333,13 +334,21 @@
   </si>
   <si>
     <t>AutomationTerritory_Fri Oct 06 2017 14:12:08 GMT+0530 (IST)</t>
+  </si>
+  <si>
+    <t>AutomationChildTerritory_Fri Oct 06 2017 14:48:56 GMT+0530 (IST)</t>
+  </si>
+  <si>
+    <t>Child Territory Name</t>
+  </si>
+  <si>
+    <t>AutomationChildTerritory_Fri Oct 06 2017 14:45:08 GMT+0530 (IST)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -719,9 +728,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="34.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="26.5703125" collapsed="true"/>
+    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -763,23 +772,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -903,13 +912,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -917,14 +926,19 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -933,6 +947,32 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="60.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -942,9 +982,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -975,7 +1015,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
@@ -985,7 +1025,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="47.0" collapsed="true"/>
+    <col min="1" max="1" width="47" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -1013,7 +1053,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1021,7 +1061,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="50.0" collapsed="true"/>
+    <col min="1" max="1" width="50" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -1039,7 +1079,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1049,9 +1089,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="30.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1093,7 +1133,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L19"/>
   <sheetViews>
@@ -1103,13 +1143,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="2" max="4" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="1" max="1" width="23" customWidth="1" collapsed="1"/>
+    <col min="2" max="4" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="34.42578125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="30.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Validating Product and Skill Violation
Validating Product and Skill Violation
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
+++ b/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\auto\sahi_pro\userdata\scripts\Sahi_Project\svmx\test_lab\test_cases\optimax\op_excleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11115" windowHeight="4650" firstSheet="8" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11115" windowHeight="4650" firstSheet="11" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="User_Details" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,11 @@
     <sheet name="SVMXC__Service_Group__c" sheetId="11" r:id="rId11"/>
     <sheet name="SVMXC__Service_Group_Members__c" sheetId="12" r:id="rId12"/>
     <sheet name="SVMXC__Skill__c" sheetId="13" r:id="rId13"/>
+    <sheet name="Installed_Product" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="389">
   <si>
     <t>UserName</t>
   </si>
@@ -1196,62 +1197,19 @@
     <t>01m3B0000004DHPQA2</t>
   </si>
   <si>
-    <t>a2N3B000000GtgWUAS</t>
-  </si>
-  <si>
-    <t>a1y3B000000Hh7PQAS</t>
-  </si>
-  <si>
-    <t>a2N3B000000GtgbUAC</t>
-  </si>
-  <si>
-    <t>a1y3B000000Hh7UQAS</t>
-  </si>
-  <si>
-    <t>a2N3B000000GtggUAC</t>
-  </si>
-  <si>
-    <t>a1y3B000000Hh7ZQAS</t>
-  </si>
-  <si>
-    <t>a2N3B000000GtgvUAC</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>a2N3B000000Gth0UAC</t>
-  </si>
-  <si>
-    <t>a1y3B000000Hh7jQAC</t>
-  </si>
-  <si>
-    <t>a2N3B000000Gth5UAC</t>
-  </si>
-  <si>
-    <t>a2N3B000000GthAUAS</t>
-  </si>
-  <si>
-    <t>a1y3B000000Hh7tQAC</t>
-  </si>
-  <si>
-    <t>a2N3B000000GthFUAS</t>
-  </si>
-  <si>
-    <t>a1y3B000000Hh7yQAC</t>
-  </si>
-  <si>
     <t>a2N3B000000GthKUAS</t>
   </si>
   <si>
     <t>a1y3B000000Hh83QAC</t>
+  </si>
+  <si>
+    <t>a0N3B0000014s9d</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1631,9 +1589,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="34.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="26.5703125" collapsed="true"/>
+    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1677,9 +1635,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1734,7 +1692,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>401</v>
+        <v>386</v>
       </c>
     </row>
   </sheetData>
@@ -1771,7 +1729,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>402</v>
+        <v>387</v>
       </c>
     </row>
   </sheetData>
@@ -1783,23 +1741,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="29.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="60.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="25.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="27.85546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="60.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="25.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="27.85546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="26.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -5394,6 +5352,31 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>388</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R2"/>
@@ -5404,24 +5387,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -5546,7 +5529,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="60.5703125" collapsed="true"/>
+    <col min="1" max="1" width="60.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -5582,7 +5565,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="60.5703125" collapsed="true"/>
+    <col min="1" max="1" width="60.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -5610,9 +5593,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="96.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="1" max="1" width="96" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -5653,7 +5636,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="47.0" collapsed="true"/>
+    <col min="1" max="1" width="47" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -5689,7 +5672,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="50.0" collapsed="true"/>
+    <col min="1" max="1" width="50" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -5717,9 +5700,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="30.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -5771,13 +5754,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="2" max="4" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="1" max="1" width="23" customWidth="1" collapsed="1"/>
+    <col min="2" max="4" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="34.42578125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="30.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated excel sheet, data creating & excel file
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
+++ b/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11115" windowHeight="4650" firstSheet="13" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11115" windowHeight="4650" firstSheet="14" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="User_Details" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="232">
   <si>
     <t>UserName</t>
   </si>
@@ -637,154 +637,106 @@
     <t>SVMXC__Skill__c</t>
   </si>
   <si>
-    <t>0013B00000I0wVhQAJ</t>
-  </si>
-  <si>
-    <t>a2N3B000000GvuwUAC</t>
-  </si>
-  <si>
-    <t>a1y3B000000HhkmQAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4iDQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4iEQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4iFQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4iGQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4iHQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4iIQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4iJQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4iKQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4iLQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4iMQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4iNQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4iOQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4iPQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4iQQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4iRQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4iSQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4iTQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4iUQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4iVQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4iWQAS</t>
-  </si>
-  <si>
-    <t>a2D3B000002LX6fUAG</t>
-  </si>
-  <si>
-    <t>a2D3B000002LX6gUAG</t>
-  </si>
-  <si>
-    <t>0013B00000I0wVmQAJ</t>
-  </si>
-  <si>
-    <t>a2N3B000000Gvv1UAC</t>
-  </si>
-  <si>
-    <t>a1y3B000000HhkrQAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4iXQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4iYQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4iZQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4iaQAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4ibQAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4icQAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4idQAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4ieQAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4ifQAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4igQAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4ihQAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4iiQAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4ijQAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4ikQAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4ilQAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4imQAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4inQAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4ioQAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4ipQAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4iqQAC</t>
-  </si>
-  <si>
-    <t>a2D3B000002LX6kUAG</t>
-  </si>
-  <si>
-    <t>a2D3B000002LX6lUAG</t>
+    <t>0013B00000I1pJbQAJ</t>
+  </si>
+  <si>
+    <t>a2N3B000000Gw1hUAC</t>
+  </si>
+  <si>
+    <t>a1y3B000000HhlpQAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4oFQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4oGQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4oHQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4oIQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4oJQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4oKQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4oLQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4oMQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4oNQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4oOQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4oPQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4oQQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4oRQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4oSQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4oTQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4oUQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4oVQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4oWQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4oXQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4oYQAS</t>
+  </si>
+  <si>
+    <t>a2D3B000002LX7sUAG</t>
+  </si>
+  <si>
+    <t>a2D3B000002LX7tUAG</t>
+  </si>
+  <si>
+    <t>a1x3B0000002sNIQAY</t>
+  </si>
+  <si>
+    <t>a1x3B0000002sNJQAY</t>
+  </si>
+  <si>
+    <t>a1x3B0000002sNKQAY</t>
+  </si>
+  <si>
+    <t>a1x3B0000002sNLQAY</t>
+  </si>
+  <si>
+    <t>a1x3B0000002sNMQAY</t>
+  </si>
+  <si>
+    <t>a1x3B0000002sNNQAY</t>
+  </si>
+  <si>
+    <t>0013B00000I1pMQQAZ</t>
+  </si>
+  <si>
+    <t>a2N3B000000Gw1rUAC</t>
+  </si>
+  <si>
+    <t>a1y3B000000HhluQAC</t>
   </si>
 </sst>
 </file>
@@ -1282,7 +1234,7 @@
         <v>175</v>
       </c>
       <c r="I2" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -1419,16 +1371,16 @@
         <v>114</v>
       </c>
       <c r="I2" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="J2" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="K2" t="s">
         <v>175</v>
       </c>
       <c r="L2" t="s">
-        <v>226</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1457,16 +1409,16 @@
         <v>114</v>
       </c>
       <c r="I3" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="J3" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="K3" t="s">
         <v>175</v>
       </c>
       <c r="L3" t="s">
-        <v>227</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1495,16 +1447,16 @@
         <v>114</v>
       </c>
       <c r="I4" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="J4" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="K4" t="s">
         <v>175</v>
       </c>
       <c r="L4" t="s">
-        <v>228</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1533,16 +1485,16 @@
         <v>114</v>
       </c>
       <c r="I5" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="J5" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="K5" t="s">
         <v>175</v>
       </c>
       <c r="L5" t="s">
-        <v>229</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1571,16 +1523,16 @@
         <v>114</v>
       </c>
       <c r="I6" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="J6" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="K6" t="s">
         <v>175</v>
       </c>
       <c r="L6" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1609,16 +1561,16 @@
         <v>114</v>
       </c>
       <c r="I7" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="J7" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="K7" t="s">
         <v>175</v>
       </c>
       <c r="L7" t="s">
-        <v>231</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1647,16 +1599,16 @@
         <v>114</v>
       </c>
       <c r="I8" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="J8" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="K8" t="s">
         <v>175</v>
       </c>
       <c r="L8" t="s">
-        <v>232</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1685,16 +1637,16 @@
         <v>114</v>
       </c>
       <c r="I9" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="J9" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="K9" t="s">
         <v>175</v>
       </c>
       <c r="L9" t="s">
-        <v>233</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1723,16 +1675,16 @@
         <v>114</v>
       </c>
       <c r="I10" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="J10" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="K10" t="s">
         <v>175</v>
       </c>
       <c r="L10" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1761,16 +1713,16 @@
         <v>114</v>
       </c>
       <c r="I11" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="J11" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="K11" t="s">
         <v>175</v>
       </c>
       <c r="L11" t="s">
-        <v>235</v>
+        <v>210</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1799,16 +1751,16 @@
         <v>114</v>
       </c>
       <c r="I12" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="J12" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="K12" t="s">
         <v>175</v>
       </c>
       <c r="L12" t="s">
-        <v>236</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1837,16 +1789,16 @@
         <v>114</v>
       </c>
       <c r="I13" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="J13" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="K13" t="s">
         <v>175</v>
       </c>
       <c r="L13" t="s">
-        <v>237</v>
+        <v>212</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1875,16 +1827,16 @@
         <v>114</v>
       </c>
       <c r="I14" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="J14" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="K14" t="s">
         <v>175</v>
       </c>
       <c r="L14" t="s">
-        <v>238</v>
+        <v>213</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1913,16 +1865,16 @@
         <v>114</v>
       </c>
       <c r="I15" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="J15" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="K15" t="s">
         <v>175</v>
       </c>
       <c r="L15" t="s">
-        <v>239</v>
+        <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1951,16 +1903,16 @@
         <v>114</v>
       </c>
       <c r="I16" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="J16" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="K16" t="s">
         <v>175</v>
       </c>
       <c r="L16" t="s">
-        <v>240</v>
+        <v>215</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1989,16 +1941,16 @@
         <v>114</v>
       </c>
       <c r="I17" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="J17" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="K17" t="s">
         <v>175</v>
       </c>
       <c r="L17" t="s">
-        <v>241</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -2027,16 +1979,16 @@
         <v>114</v>
       </c>
       <c r="I18" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="J18" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="K18" t="s">
         <v>175</v>
       </c>
       <c r="L18" t="s">
-        <v>242</v>
+        <v>217</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -2065,16 +2017,16 @@
         <v>114</v>
       </c>
       <c r="I19" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="J19" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="K19" t="s">
         <v>175</v>
       </c>
       <c r="L19" t="s">
-        <v>243</v>
+        <v>218</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2103,16 +2055,16 @@
         <v>114</v>
       </c>
       <c r="I20" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="J20" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="K20" t="s">
         <v>175</v>
       </c>
       <c r="L20" t="s">
-        <v>244</v>
+        <v>219</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -2141,16 +2093,16 @@
         <v>114</v>
       </c>
       <c r="I21" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="J21" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="K21" t="s">
         <v>175</v>
       </c>
       <c r="L21" t="s">
-        <v>245</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -2184,7 +2136,7 @@
         <v>186</v>
       </c>
       <c r="B2" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -2196,7 +2148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
@@ -2231,7 +2183,7 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>246</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2245,7 +2197,7 @@
         <v>174</v>
       </c>
       <c r="D3" t="s">
-        <v>247</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -2317,9 +2269,11 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2328,7 +2282,7 @@
     <col min="3" max="3" bestFit="true" customWidth="true" width="27.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>188</v>
       </c>
@@ -2338,50 +2292,53 @@
       <c r="C1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>193</v>
@@ -2395,10 +2352,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2406,10 +2363,11 @@
     <col min="1" max="1" customWidth="true" width="22.0" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>196</v>
       </c>
@@ -2422,74 +2380,110 @@
       <c r="D1" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>226</v>
+        <v>201</v>
       </c>
       <c r="C2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+      <c r="D2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>227</v>
+        <v>202</v>
       </c>
       <c r="C3" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+      <c r="D3" t="s">
+        <v>221</v>
+      </c>
+      <c r="E3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>228</v>
+        <v>203</v>
       </c>
       <c r="C4" t="s">
+        <v>231</v>
+      </c>
+      <c r="D4" t="s">
+        <v>221</v>
+      </c>
+      <c r="E4" t="s">
         <v>225</v>
       </c>
-      <c r="D4" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>229</v>
+        <v>204</v>
       </c>
       <c r="C5" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+      <c r="D5" t="s">
+        <v>222</v>
+      </c>
+      <c r="E5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="C6" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+      <c r="D6" t="s">
+        <v>222</v>
+      </c>
+      <c r="E6" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10</v>
       </c>
       <c r="B7" t="s">
+        <v>206</v>
+      </c>
+      <c r="C7" t="s">
         <v>231</v>
       </c>
-      <c r="C7" t="s">
-        <v>225</v>
+      <c r="D7" t="s">
+        <v>222</v>
+      </c>
+      <c r="E7" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chreating new sheet in automation excel
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
+++ b/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\auto\sahi_pro\userdata\scripts\Sahi_Project\svmx\test_lab\test_cases\optimax\op_excleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11115" windowHeight="4650" firstSheet="14" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11115" windowHeight="4650" firstSheet="15" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="User_Details" sheetId="1" r:id="rId1"/>
@@ -30,10 +30,11 @@
     <sheet name="Installed_Product" sheetId="16" r:id="rId16"/>
     <sheet name="SVMXC__Resource_Preference__c" sheetId="18" r:id="rId17"/>
     <sheet name="SVMXC__Service_Group_Skills__c" sheetId="19" r:id="rId18"/>
+    <sheet name="RS_6694" sheetId="20" r:id="rId19"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="237">
   <si>
     <t>UserName</t>
   </si>
@@ -637,113 +638,127 @@
     <t>SVMXC__Skill__c</t>
   </si>
   <si>
-    <t>0013B00000I1pJbQAJ</t>
-  </si>
-  <si>
-    <t>a2N3B000000Gw1hUAC</t>
-  </si>
-  <si>
-    <t>a1y3B000000HhlpQAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4oFQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4oGQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4oHQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4oIQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4oJQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4oKQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4oLQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4oMQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4oNQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4oOQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4oPQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4oQQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4oRQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4oSQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4oTQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4oUQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4oVQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4oWQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4oXQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4oYQAS</t>
-  </si>
-  <si>
-    <t>a2D3B000002LX7sUAG</t>
-  </si>
-  <si>
-    <t>a2D3B000002LX7tUAG</t>
-  </si>
-  <si>
-    <t>a1x3B0000002sNIQAY</t>
-  </si>
-  <si>
-    <t>a1x3B0000002sNJQAY</t>
-  </si>
-  <si>
-    <t>a1x3B0000002sNKQAY</t>
-  </si>
-  <si>
-    <t>a1x3B0000002sNLQAY</t>
-  </si>
-  <si>
-    <t>a1x3B0000002sNMQAY</t>
-  </si>
-  <si>
-    <t>a1x3B0000002sNNQAY</t>
-  </si>
-  <si>
-    <t>0013B00000I1pMQQAZ</t>
-  </si>
-  <si>
-    <t>a2N3B000000Gw1rUAC</t>
-  </si>
-  <si>
-    <t>a1y3B000000HhluQAC</t>
+    <t>a2N3B000000GzViUAK</t>
+  </si>
+  <si>
+    <t>0013B00000I4z82QAB</t>
+  </si>
+  <si>
+    <t>a2N3B000000GzW7UAK</t>
+  </si>
+  <si>
+    <t>a1y3B000000HhmyQAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4u3QAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4u4QAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4u5QAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4u6QAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4u7QAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4u8QAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4u9QAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4uAQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4uBQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4uCQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4uDQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4uEQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4uFQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4uGQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4uHQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4uIQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4uJQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4uKQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4uLQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M4uMQAS</t>
+  </si>
+  <si>
+    <t>a2D3B000002LX9AUAW</t>
+  </si>
+  <si>
+    <t>a2D3B000002LX9BUAW</t>
+  </si>
+  <si>
+    <t>a1x3B0000002sRqQAI</t>
+  </si>
+  <si>
+    <t>a1x3B0000002sRrQAI</t>
+  </si>
+  <si>
+    <t>a1x3B0000002sRsQAI</t>
+  </si>
+  <si>
+    <t>a1x3B0000002sRtQAI</t>
+  </si>
+  <si>
+    <t>a1x3B0000002sRuQAI</t>
+  </si>
+  <si>
+    <t>a1x3B0000002sRvQAI</t>
+  </si>
+  <si>
+    <t>a133B000000OIxzQAG</t>
+  </si>
+  <si>
+    <t>a133B000000OIy0QAG</t>
+  </si>
+  <si>
+    <t>a133B000000OIy1QAG</t>
+  </si>
+  <si>
+    <t>a133B000000OIy2QAG</t>
+  </si>
+  <si>
+    <t>a133B000000OIy3QAG</t>
+  </si>
+  <si>
+    <t>a133B000000OIy4QAG</t>
+  </si>
+  <si>
+    <t>Work Order for 6694</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1130,9 +1145,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="34.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="26.5703125" collapsed="true"/>
+    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1173,10 +1188,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="35.140625" collapsed="true"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="35.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1205,7 +1220,7 @@
         <v>103</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>88</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1234,7 +1249,7 @@
         <v>175</v>
       </c>
       <c r="I2" t="s">
-        <v>230</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -1294,17 +1309,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="29.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="60.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="25.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="27.85546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="60.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="25.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="27.85546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="26.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -1371,16 +1386,16 @@
         <v>114</v>
       </c>
       <c r="I2" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="J2" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="K2" t="s">
         <v>175</v>
       </c>
       <c r="L2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1409,16 +1424,16 @@
         <v>114</v>
       </c>
       <c r="I3" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="J3" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="K3" t="s">
         <v>175</v>
       </c>
       <c r="L3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1447,16 +1462,16 @@
         <v>114</v>
       </c>
       <c r="I4" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="J4" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="K4" t="s">
         <v>175</v>
       </c>
       <c r="L4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1485,16 +1500,16 @@
         <v>114</v>
       </c>
       <c r="I5" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="J5" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="K5" t="s">
         <v>175</v>
       </c>
       <c r="L5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1523,16 +1538,16 @@
         <v>114</v>
       </c>
       <c r="I6" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="J6" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="K6" t="s">
         <v>175</v>
       </c>
       <c r="L6" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1561,16 +1576,16 @@
         <v>114</v>
       </c>
       <c r="I7" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="J7" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="K7" t="s">
         <v>175</v>
       </c>
       <c r="L7" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1599,16 +1614,16 @@
         <v>114</v>
       </c>
       <c r="I8" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="J8" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="K8" t="s">
         <v>175</v>
       </c>
       <c r="L8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1637,16 +1652,16 @@
         <v>114</v>
       </c>
       <c r="I9" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="J9" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="K9" t="s">
         <v>175</v>
       </c>
       <c r="L9" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1675,16 +1690,16 @@
         <v>114</v>
       </c>
       <c r="I10" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="J10" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="K10" t="s">
         <v>175</v>
       </c>
       <c r="L10" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1713,16 +1728,16 @@
         <v>114</v>
       </c>
       <c r="I11" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="J11" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="K11" t="s">
         <v>175</v>
       </c>
       <c r="L11" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1751,16 +1766,16 @@
         <v>114</v>
       </c>
       <c r="I12" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="J12" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="K12" t="s">
         <v>175</v>
       </c>
       <c r="L12" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1789,16 +1804,16 @@
         <v>114</v>
       </c>
       <c r="I13" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="J13" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="K13" t="s">
         <v>175</v>
       </c>
       <c r="L13" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1827,16 +1842,16 @@
         <v>114</v>
       </c>
       <c r="I14" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="J14" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="K14" t="s">
         <v>175</v>
       </c>
       <c r="L14" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1865,16 +1880,16 @@
         <v>114</v>
       </c>
       <c r="I15" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="J15" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="K15" t="s">
         <v>175</v>
       </c>
       <c r="L15" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1903,16 +1918,16 @@
         <v>114</v>
       </c>
       <c r="I16" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="J16" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="K16" t="s">
         <v>175</v>
       </c>
       <c r="L16" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1941,16 +1956,16 @@
         <v>114</v>
       </c>
       <c r="I17" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="J17" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="K17" t="s">
         <v>175</v>
       </c>
       <c r="L17" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1979,16 +1994,16 @@
         <v>114</v>
       </c>
       <c r="I18" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="J18" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="K18" t="s">
         <v>175</v>
       </c>
       <c r="L18" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -2017,16 +2032,16 @@
         <v>114</v>
       </c>
       <c r="I19" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="J19" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="K19" t="s">
         <v>175</v>
       </c>
       <c r="L19" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2055,16 +2070,16 @@
         <v>114</v>
       </c>
       <c r="I20" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="J20" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="K20" t="s">
         <v>175</v>
       </c>
       <c r="L20" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -2093,16 +2108,16 @@
         <v>114</v>
       </c>
       <c r="I21" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="J21" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="K21" t="s">
         <v>175</v>
       </c>
       <c r="L21" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -2120,7 +2135,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -2136,7 +2151,7 @@
         <v>186</v>
       </c>
       <c r="B2" t="s">
-        <v>229</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -2154,8 +2169,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2183,7 +2198,7 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2197,7 +2212,7 @@
         <v>174</v>
       </c>
       <c r="D3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -2216,7 +2231,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -2249,7 +2264,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -2271,15 +2286,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2298,50 +2314,86 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>229</v>
+        <v>199</v>
+      </c>
+      <c r="B2" t="s">
+        <v>202</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>191</v>
       </c>
+      <c r="D2" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>229</v>
+        <v>199</v>
+      </c>
+      <c r="B3" t="s">
+        <v>203</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>191</v>
       </c>
+      <c r="D3" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>229</v>
+        <v>199</v>
+      </c>
+      <c r="B4" t="s">
+        <v>204</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>192</v>
       </c>
+      <c r="D4" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>229</v>
+        <v>199</v>
+      </c>
+      <c r="B5" t="s">
+        <v>205</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>192</v>
       </c>
+      <c r="D5" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>229</v>
+        <v>199</v>
+      </c>
+      <c r="B6" t="s">
+        <v>206</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>193</v>
       </c>
+      <c r="D6" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>229</v>
+        <v>199</v>
+      </c>
+      <c r="B7" t="s">
+        <v>207</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>193</v>
+      </c>
+      <c r="D7" t="s">
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -2360,11 +2412,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="1" max="1" width="22" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2389,16 +2441,16 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C2" t="s">
         <v>201</v>
       </c>
-      <c r="C2" t="s">
-        <v>231</v>
-      </c>
       <c r="D2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2406,16 +2458,16 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C3" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="D3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2423,16 +2475,16 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C4" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="D4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E4" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2440,16 +2492,16 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C5" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="D5" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E5" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2457,16 +2509,16 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C6" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="D6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E6" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2474,16 +2526,197 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C7" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="D7" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E7" t="s">
-        <v>228</v>
+        <v>229</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2">
+        <v>2900</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2">
+        <v>2400</v>
+      </c>
+      <c r="L2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3">
+        <v>1083</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3">
+        <v>3000</v>
+      </c>
+      <c r="L3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4">
+        <v>1340</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4">
+        <v>3000</v>
+      </c>
+      <c r="L4" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -2501,24 +2734,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -2643,7 +2876,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="60.5703125" collapsed="true"/>
+    <col min="1" max="1" width="60.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -2684,7 +2917,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="60.5703125" collapsed="true"/>
+    <col min="1" max="1" width="60.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -2712,9 +2945,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="96.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="1" max="1" width="96" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2755,7 +2988,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="47.0" collapsed="true"/>
+    <col min="1" max="1" width="47" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -2791,7 +3024,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="50.0" collapsed="true"/>
+    <col min="1" max="1" width="50" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -2817,8 +3050,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2873,19 +3106,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection sqref="A1:L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="2" max="4" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="1" max="1" width="23" customWidth="1" collapsed="1"/>
+    <col min="2" max="4" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="34.42578125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="30.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated MTTS test cases to use the new Rule Sheet
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
+++ b/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\auto\sahi_pro\userdata\scripts\Sahi_Project\svmx\test_lab\test_cases\optimax\op_excleData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11115" windowHeight="4650" firstSheet="15" activeTab="18"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="5640" firstSheet="16" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="User_Details" sheetId="1" r:id="rId1"/>
@@ -31,10 +26,12 @@
     <sheet name="SVMXC__Resource_Preference__c" sheetId="18" r:id="rId17"/>
     <sheet name="SVMXC__Service_Group_Skills__c" sheetId="19" r:id="rId18"/>
     <sheet name="RS_6694" sheetId="20" r:id="rId19"/>
+    <sheet name="Rules" sheetId="21" r:id="rId20"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:S16"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -42,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="242">
   <si>
     <t>UserName</t>
   </si>
@@ -753,12 +750,28 @@
   </si>
   <si>
     <t>Work Order for 6694</t>
+  </si>
+  <si>
+    <t>MTTS</t>
+  </si>
+  <si>
+    <t>Skill Match Rule</t>
+  </si>
+  <si>
+    <t>Territory Match Rule</t>
+  </si>
+  <si>
+    <t>Eligibility Rule</t>
+  </si>
+  <si>
+    <t>MTTSRule_Mon Oct 23 2017 12:39:19 GMT+0530 (IST)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1145,9 +1158,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="26.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1188,10 +1201,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="35.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="35.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1309,17 +1322,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="60.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="25.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="27.85546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="26.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="29.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="60.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="26.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -2135,7 +2148,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -2169,8 +2182,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2231,7 +2244,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -2264,7 +2277,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -2292,10 +2305,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="20.42578125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2412,11 +2425,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2547,24 +2560,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.0" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.140625" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="26.7109375" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="26.42578125" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="17.85546875" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="25.28515625" collapsed="false"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="34.42578125" collapsed="false"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="45.7109375" collapsed="false"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="36.42578125" collapsed="false"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="30.7109375" collapsed="false"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="19.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -2734,24 +2747,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -2863,6 +2876,40 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -2876,7 +2923,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="60.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="60.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -2917,7 +2964,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="60.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="60.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -2945,9 +2992,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="96" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="96.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2988,7 +3035,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="47.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -3024,7 +3071,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="50.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -3050,8 +3097,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3112,13 +3159,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" customWidth="1" collapsed="1"/>
-    <col min="2" max="4" width="24.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="34.42578125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="30.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="2" max="4" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="30.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated Skill Match test cases to use the new Rule Sheet
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
+++ b/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="243">
   <si>
     <t>UserName</t>
   </si>
@@ -765,6 +765,9 @@
   </si>
   <si>
     <t>MTTSRule_Mon Oct 23 2017 12:39:19 GMT+0530 (IST)</t>
+  </si>
+  <si>
+    <t>SkillMatchRule_Mon Oct 23 2017 13:01:16 GMT+0530 (IST)</t>
   </si>
 </sst>
 </file>
@@ -2308,7 +2311,7 @@
     <col min="1" max="1" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="27.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="20.42578125" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2566,18 +2569,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="23.0" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.140625" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="26.7109375" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="26.42578125" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="17.85546875" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="25.28515625" collapsed="false"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="34.42578125" collapsed="false"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="45.7109375" collapsed="false"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="36.42578125" collapsed="false"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="30.7109375" collapsed="false"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="19.0" collapsed="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="45.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="36.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -2907,6 +2910,9 @@
       <c r="A2" t="s">
         <v>241</v>
       </c>
+      <c r="B2" t="s">
+        <v>242</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Territory Match Rule test cases to use the new rule sheet
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
+++ b/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="244">
   <si>
     <t>UserName</t>
   </si>
@@ -768,6 +768,9 @@
   </si>
   <si>
     <t>SkillMatchRule_Mon Oct 23 2017 13:01:16 GMT+0530 (IST)</t>
+  </si>
+  <si>
+    <t>TerritoryRule_Mon Oct 23 2017 14:07:00 GMT+0530 (IST)</t>
   </si>
 </sst>
 </file>
@@ -2913,6 +2916,9 @@
       <c r="B2" t="s">
         <v>242</v>
       </c>
+      <c r="C2" t="s">
+        <v>243</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Eligibility Rule to use the new Rule sheet
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
+++ b/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="5640" firstSheet="16" activeTab="19"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="5640" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="User_Details" sheetId="1" r:id="rId1"/>
@@ -12,26 +12,23 @@
     <sheet name="Territory" sheetId="8" r:id="rId3"/>
     <sheet name="ChildTerritory" sheetId="9" r:id="rId4"/>
     <sheet name="Dispatch_Process" sheetId="4" r:id="rId5"/>
-    <sheet name="MTTS" sheetId="5" r:id="rId6"/>
-    <sheet name="TerritoryRule" sheetId="6" r:id="rId7"/>
-    <sheet name="RS_6299_RS_6300" sheetId="2" r:id="rId8"/>
-    <sheet name="RS_6665" sheetId="3" r:id="rId9"/>
-    <sheet name="SVMXC__Territory__c" sheetId="10" r:id="rId10"/>
-    <sheet name="SVMXC__Service_Group__c" sheetId="11" r:id="rId11"/>
-    <sheet name="SVMXC__Service_Group_Members__c" sheetId="12" r:id="rId12"/>
-    <sheet name="Account" sheetId="17" r:id="rId13"/>
-    <sheet name="SVMXC__Skill__c" sheetId="13" r:id="rId14"/>
-    <sheet name="SkillRule" sheetId="14" r:id="rId15"/>
-    <sheet name="Installed_Product" sheetId="16" r:id="rId16"/>
-    <sheet name="SVMXC__Resource_Preference__c" sheetId="18" r:id="rId17"/>
-    <sheet name="SVMXC__Service_Group_Skills__c" sheetId="19" r:id="rId18"/>
-    <sheet name="RS_6694" sheetId="20" r:id="rId19"/>
-    <sheet name="Rules" sheetId="21" r:id="rId20"/>
+    <sheet name="RS_6299_RS_6300" sheetId="2" r:id="rId6"/>
+    <sheet name="RS_6665" sheetId="3" r:id="rId7"/>
+    <sheet name="SVMXC__Territory__c" sheetId="10" r:id="rId8"/>
+    <sheet name="SVMXC__Service_Group__c" sheetId="11" r:id="rId9"/>
+    <sheet name="SVMXC__Service_Group_Members__c" sheetId="12" r:id="rId10"/>
+    <sheet name="Account" sheetId="17" r:id="rId11"/>
+    <sheet name="SVMXC__Skill__c" sheetId="13" r:id="rId12"/>
+    <sheet name="Installed_Product" sheetId="16" r:id="rId13"/>
+    <sheet name="SVMXC__Resource_Preference__c" sheetId="18" r:id="rId14"/>
+    <sheet name="SVMXC__Service_Group_Skills__c" sheetId="19" r:id="rId15"/>
+    <sheet name="RS_6694" sheetId="20" r:id="rId16"/>
+    <sheet name="Rules" sheetId="21" r:id="rId17"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:S16"/>
+  <oleSize ref="A1:G16"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -39,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="236">
   <si>
     <t>UserName</t>
   </si>
@@ -230,18 +227,6 @@
     <t>Territory ID</t>
   </si>
   <si>
-    <t>MTTS Name</t>
-  </si>
-  <si>
-    <t>Territory Rule Name</t>
-  </si>
-  <si>
-    <t>MTTSRule_Thu Oct 05 2017 12:09:28 GMT+0530 (IST)</t>
-  </si>
-  <si>
-    <t>TerritoryRule_Thu Oct 05 2017 12:13:54 GMT+0530 (IST)</t>
-  </si>
-  <si>
     <t>FridayEndTime</t>
   </si>
   <si>
@@ -308,12 +293,6 @@
     <t>Id</t>
   </si>
   <si>
-    <t>MTTSRule_Fri Oct 06 2017 11:15:12 GMT+0530 (IST)</t>
-  </si>
-  <si>
-    <t>MTTSRule_Fri Oct 06 2017 11:26:59 GMT+0530 (IST)</t>
-  </si>
-  <si>
     <t>Territory Name</t>
   </si>
   <si>
@@ -569,15 +548,6 @@
     <t>01m3B0000004DHPQA2</t>
   </si>
   <si>
-    <t>Skill Rule Name</t>
-  </si>
-  <si>
-    <t>SkillMatchRule_Wed Oct 11 2017 15:52:02 GMT+0530 (IST)</t>
-  </si>
-  <si>
-    <t>SkillMatchRule_Wed Oct 11 2017 15:57:44 GMT+0530 (IST)</t>
-  </si>
-  <si>
     <t>govendhan@svmx-cct5.org.cct5part1</t>
   </si>
   <si>
@@ -771,13 +741,15 @@
   </si>
   <si>
     <t>TerritoryRule_Mon Oct 23 2017 14:07:00 GMT+0530 (IST)</t>
+  </si>
+  <si>
+    <t>TechEligibilityRule_Mon Oct 23 2017 14:51:34 GMT+0530 (IST)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1164,9 +1136,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="34.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="26.5703125" collapsed="true"/>
+    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1182,10 +1154,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -1198,127 +1170,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="35.140625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>172</v>
-      </c>
-      <c r="B2" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>40</v>
-      </c>
-      <c r="D2">
-        <v>1000</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>60</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>175</v>
-      </c>
-      <c r="I2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L21"/>
   <sheetViews>
@@ -1328,28 +1179,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="29.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="60.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="25.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="27.85546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="60.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="25.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="27.85546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="26.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D1" t="s">
         <v>15</v>
@@ -1358,7 +1209,7 @@
         <v>16</v>
       </c>
       <c r="F1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G1" t="s">
         <v>12</v>
@@ -1367,21 +1218,21 @@
         <v>14</v>
       </c>
       <c r="I1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="K1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="L1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -1390,36 +1241,36 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G2">
         <v>90001</v>
       </c>
       <c r="H2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I2" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="J2" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="K2" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="L2" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -1428,36 +1279,36 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E3" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G3">
         <v>90274</v>
       </c>
       <c r="H3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I3" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="J3" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="K3" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="L3" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -1466,36 +1317,36 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E4" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F4" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G4">
         <v>90305</v>
       </c>
       <c r="H4" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I4" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="J4" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="K4" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="L4" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -1504,36 +1355,36 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E5" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F5" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G5">
         <v>90363</v>
       </c>
       <c r="H5" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I5" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="J5" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="K5" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="L5" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
@@ -1542,36 +1393,36 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="E6" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F6" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G6">
         <v>90402</v>
       </c>
       <c r="H6" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I6" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="J6" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="K6" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="L6" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -1580,36 +1431,36 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="E7" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G7">
         <v>90606</v>
       </c>
       <c r="H7" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I7" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="J7" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="K7" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="L7" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
@@ -1618,36 +1469,36 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="E8" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="F8" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G8">
         <v>90620</v>
       </c>
       <c r="H8" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I8" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="J8" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="K8" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="L8" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
@@ -1656,36 +1507,36 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E9" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="F9" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G9">
         <v>90630</v>
       </c>
       <c r="H9" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I9" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="J9" t="s">
+        <v>191</v>
+      </c>
+      <c r="K9" t="s">
+        <v>169</v>
+      </c>
+      <c r="L9" t="s">
         <v>200</v>
-      </c>
-      <c r="K9" t="s">
-        <v>175</v>
-      </c>
-      <c r="L9" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
@@ -1694,36 +1545,36 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="E10" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="F10" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G10">
         <v>90631</v>
       </c>
       <c r="H10" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I10" t="s">
+        <v>192</v>
+      </c>
+      <c r="J10" t="s">
+        <v>191</v>
+      </c>
+      <c r="K10" t="s">
+        <v>169</v>
+      </c>
+      <c r="L10" t="s">
         <v>201</v>
-      </c>
-      <c r="J10" t="s">
-        <v>200</v>
-      </c>
-      <c r="K10" t="s">
-        <v>175</v>
-      </c>
-      <c r="L10" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
@@ -1732,36 +1583,36 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E11" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="F11" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G11">
         <v>90713</v>
       </c>
       <c r="H11" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I11" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="J11" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="K11" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="L11" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B12" t="b">
         <v>1</v>
@@ -1770,36 +1621,36 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="E12" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F12" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G12">
         <v>91344</v>
       </c>
       <c r="H12" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I12" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="J12" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="K12" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="L12" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B13" t="b">
         <v>1</v>
@@ -1808,36 +1659,36 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="E13" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="F13" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G13">
         <v>91606</v>
       </c>
       <c r="H13" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I13" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="J13" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="K13" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="L13" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B14" t="b">
         <v>1</v>
@@ -1846,36 +1697,36 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="E14" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="F14" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G14">
         <v>91803</v>
       </c>
       <c r="H14" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I14" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="J14" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="K14" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="L14" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B15" t="b">
         <v>1</v>
@@ -1884,36 +1735,36 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="E15" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="F15" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G15">
         <v>92009</v>
       </c>
       <c r="H15" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I15" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="J15" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="K15" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="L15" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B16" t="b">
         <v>1</v>
@@ -1922,36 +1773,36 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="E16" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="F16" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G16">
         <v>92105</v>
       </c>
       <c r="H16" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I16" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="J16" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="K16" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="L16" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
@@ -1960,36 +1811,36 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E17" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="F17" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G17">
         <v>92284</v>
       </c>
       <c r="H17" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I17" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="J17" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="K17" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="L17" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B18" t="b">
         <v>1</v>
@@ -1998,36 +1849,36 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="E18" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="F18" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G18">
         <v>92595</v>
       </c>
       <c r="H18" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I18" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="J18" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="K18" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="L18" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B19" t="b">
         <v>1</v>
@@ -2036,36 +1887,36 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="E19" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F19" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G19">
         <v>92780</v>
       </c>
       <c r="H19" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I19" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="J19" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="K19" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="L19" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B20" t="b">
         <v>1</v>
@@ -2074,36 +1925,36 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="E20" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="F20" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G20">
         <v>93108</v>
       </c>
       <c r="H20" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I20" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="J20" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="K20" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="L20" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B21" t="b">
         <v>1</v>
@@ -2112,31 +1963,31 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="E21" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F21" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G21">
         <v>93720</v>
       </c>
       <c r="H21" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I21" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="J21" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="K21" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="L21" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -2144,7 +1995,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2154,23 +2005,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="B2" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -2178,7 +2029,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -2188,27 +2039,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -2217,21 +2068,21 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="D3" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -2240,40 +2091,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -2283,17 +2101,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -2301,7 +2119,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -2311,108 +2129,108 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="27.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="B1" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="C1" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="D1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="B2" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="D2" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="B3" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="D3" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="B4" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="D4" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="B5" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="D5" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="B6" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D6" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="B7" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D7" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -2421,7 +2239,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
@@ -2431,28 +2249,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="1" max="1" width="22" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="B1" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="C1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D1" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="E1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2460,16 +2278,16 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="C2" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="D2" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="E2" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2477,16 +2295,16 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="C3" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="D3" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="E3" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2494,16 +2312,16 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="C4" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="D4" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="E4" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2511,16 +2329,16 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="C5" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="D5" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="E5" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2528,16 +2346,16 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="C6" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="D6" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="E6" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2545,16 +2363,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="C7" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="D7" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="E7" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -2562,7 +2380,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
@@ -2572,18 +2390,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="45.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="36.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="30.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="25.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="45.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="36.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="30.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="19" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -2659,7 +2477,7 @@
         <v>2400</v>
       </c>
       <c r="L2" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2697,7 +2515,7 @@
         <v>3000</v>
       </c>
       <c r="L3" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2735,7 +2553,53 @@
         <v>3000</v>
       </c>
       <c r="L4" t="s">
-        <v>236</v>
+        <v>227</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="55.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D2" t="s">
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -2753,175 +2617,135 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N1" t="s">
+        <v>63</v>
+      </c>
+      <c r="O1" t="s">
+        <v>70</v>
+      </c>
+      <c r="P1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q1" t="s">
         <v>72</v>
       </c>
-      <c r="C1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="R1" t="s">
         <v>71</v>
-      </c>
-      <c r="F1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G1" t="s">
-        <v>81</v>
-      </c>
-      <c r="H1" t="s">
-        <v>80</v>
-      </c>
-      <c r="I1" t="s">
-        <v>83</v>
-      </c>
-      <c r="J1" t="s">
-        <v>82</v>
-      </c>
-      <c r="K1" t="s">
-        <v>78</v>
-      </c>
-      <c r="L1" t="s">
-        <v>77</v>
-      </c>
-      <c r="M1" t="s">
-        <v>68</v>
-      </c>
-      <c r="N1" t="s">
-        <v>67</v>
-      </c>
-      <c r="O1" t="s">
-        <v>74</v>
-      </c>
-      <c r="P1" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>76</v>
-      </c>
-      <c r="R1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C2" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>237</v>
-      </c>
-      <c r="B1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C1" t="s">
-        <v>239</v>
-      </c>
-      <c r="D1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>241</v>
-      </c>
-      <c r="B2" t="s">
-        <v>242</v>
-      </c>
-      <c r="C2" t="s">
-        <v>243</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -2935,32 +2759,32 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="60.5703125" collapsed="true"/>
+    <col min="1" max="1" width="60.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2976,17 +2800,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="60.5703125" collapsed="true"/>
+    <col min="1" max="1" width="60.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -3004,9 +2828,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="96.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="1" max="1" width="96" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -3022,10 +2846,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="B2" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="C2" t="s">
         <v>59</v>
@@ -3039,78 +2863,14 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="47.0" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="50.0" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3161,7 +2921,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L19"/>
   <sheetViews>
@@ -3171,13 +2931,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="2" max="4" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="1" max="1" width="23" customWidth="1" collapsed="1"/>
+    <col min="2" max="4" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="34.42578125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="30.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -3861,4 +3621,125 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="35.140625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>40</v>
+      </c>
+      <c r="D2">
+        <v>1000</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>60</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>169</v>
+      </c>
+      <c r="I2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Territory and Dispatch Process test cases to use the new rule sheet
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
+++ b/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
@@ -4,29 +4,27 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="5640" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="5640" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="User_Details" sheetId="1" r:id="rId1"/>
     <sheet name="BusinessHours" sheetId="7" r:id="rId2"/>
-    <sheet name="Territory" sheetId="8" r:id="rId3"/>
-    <sheet name="ChildTerritory" sheetId="9" r:id="rId4"/>
-    <sheet name="Dispatch_Process" sheetId="4" r:id="rId5"/>
-    <sheet name="RS_6299_RS_6300" sheetId="2" r:id="rId6"/>
-    <sheet name="RS_6665" sheetId="3" r:id="rId7"/>
-    <sheet name="SVMXC__Territory__c" sheetId="10" r:id="rId8"/>
-    <sheet name="SVMXC__Service_Group__c" sheetId="11" r:id="rId9"/>
-    <sheet name="SVMXC__Service_Group_Members__c" sheetId="12" r:id="rId10"/>
-    <sheet name="Account" sheetId="17" r:id="rId11"/>
-    <sheet name="SVMXC__Skill__c" sheetId="13" r:id="rId12"/>
-    <sheet name="Installed_Product" sheetId="16" r:id="rId13"/>
-    <sheet name="SVMXC__Resource_Preference__c" sheetId="18" r:id="rId14"/>
-    <sheet name="SVMXC__Service_Group_Skills__c" sheetId="19" r:id="rId15"/>
-    <sheet name="RS_6694" sheetId="20" r:id="rId16"/>
-    <sheet name="Rules" sheetId="21" r:id="rId17"/>
+    <sheet name="Dispatch_Process" sheetId="4" r:id="rId3"/>
+    <sheet name="RS_6299_RS_6300" sheetId="2" r:id="rId4"/>
+    <sheet name="RS_6665" sheetId="3" r:id="rId5"/>
+    <sheet name="SVMXC__Territory__c" sheetId="10" r:id="rId6"/>
+    <sheet name="SVMXC__Service_Group__c" sheetId="11" r:id="rId7"/>
+    <sheet name="SVMXC__Service_Group_Members__c" sheetId="12" r:id="rId8"/>
+    <sheet name="Account" sheetId="17" r:id="rId9"/>
+    <sheet name="SVMXC__Skill__c" sheetId="13" r:id="rId10"/>
+    <sheet name="Installed_Product" sheetId="16" r:id="rId11"/>
+    <sheet name="SVMXC__Resource_Preference__c" sheetId="18" r:id="rId12"/>
+    <sheet name="SVMXC__Service_Group_Skills__c" sheetId="19" r:id="rId13"/>
+    <sheet name="RS_6694" sheetId="20" r:id="rId14"/>
+    <sheet name="Rules" sheetId="21" r:id="rId15"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:G16"/>
+  <oleSize ref="A1:H16"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="233">
   <si>
     <t>UserName</t>
   </si>
@@ -293,24 +291,6 @@
     <t>Id</t>
   </si>
   <si>
-    <t>Territory Name</t>
-  </si>
-  <si>
-    <t>AutomationTerritory_Fri Oct 06 2017 14:10:03 GMT+0530 (IST)</t>
-  </si>
-  <si>
-    <t>AutomationTerritory_Fri Oct 06 2017 14:12:08 GMT+0530 (IST)</t>
-  </si>
-  <si>
-    <t>AutomationChildTerritory_Fri Oct 06 2017 14:48:56 GMT+0530 (IST)</t>
-  </si>
-  <si>
-    <t>Child Territory Name</t>
-  </si>
-  <si>
-    <t>AutomationChildTerritory_Fri Oct 06 2017 14:45:08 GMT+0530 (IST)</t>
-  </si>
-  <si>
     <t>SVMXC__Active__c</t>
   </si>
   <si>
@@ -560,9 +540,6 @@
     <t>a1j3B0000008e6u</t>
   </si>
   <si>
-    <t>AutomationTerritory_Fri Oct 13 2017 16:48:15 GMT+0530 (IST)</t>
-  </si>
-  <si>
     <t>a0N3B0000014s9d</t>
   </si>
   <si>
@@ -744,6 +721,18 @@
   </si>
   <si>
     <t>TechEligibilityRule_Mon Oct 23 2017 14:51:34 GMT+0530 (IST)</t>
+  </si>
+  <si>
+    <t>Territory</t>
+  </si>
+  <si>
+    <t>Child Territory</t>
+  </si>
+  <si>
+    <t>AutomationTerritory_Mon Oct 23 2017 14:58:18 GMT+0530 (IST)</t>
+  </si>
+  <si>
+    <t>AutomationChildTerritory_Mon Oct 23 2017 15:09:26 GMT+0530 (IST)</t>
   </si>
 </sst>
 </file>
@@ -1154,10 +1143,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -1170,866 +1159,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L21"/>
-  <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="60.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="25.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="27.85546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="26.28515625" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" t="s">
-        <v>101</v>
-      </c>
-      <c r="J1" t="s">
-        <v>102</v>
-      </c>
-      <c r="K1" t="s">
-        <v>103</v>
-      </c>
-      <c r="L1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G2">
-        <v>90001</v>
-      </c>
-      <c r="H2" t="s">
-        <v>108</v>
-      </c>
-      <c r="I2" t="s">
-        <v>192</v>
-      </c>
-      <c r="J2" t="s">
-        <v>191</v>
-      </c>
-      <c r="K2" t="s">
-        <v>169</v>
-      </c>
-      <c r="L2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E3" t="s">
-        <v>111</v>
-      </c>
-      <c r="F3" t="s">
-        <v>107</v>
-      </c>
-      <c r="G3">
-        <v>90274</v>
-      </c>
-      <c r="H3" t="s">
-        <v>108</v>
-      </c>
-      <c r="I3" t="s">
-        <v>192</v>
-      </c>
-      <c r="J3" t="s">
-        <v>191</v>
-      </c>
-      <c r="K3" t="s">
-        <v>169</v>
-      </c>
-      <c r="L3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B4" t="b">
-        <v>1</v>
-      </c>
-      <c r="C4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>113</v>
-      </c>
-      <c r="E4" t="s">
-        <v>114</v>
-      </c>
-      <c r="F4" t="s">
-        <v>107</v>
-      </c>
-      <c r="G4">
-        <v>90305</v>
-      </c>
-      <c r="H4" t="s">
-        <v>108</v>
-      </c>
-      <c r="I4" t="s">
-        <v>192</v>
-      </c>
-      <c r="J4" t="s">
-        <v>191</v>
-      </c>
-      <c r="K4" t="s">
-        <v>169</v>
-      </c>
-      <c r="L4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>116</v>
-      </c>
-      <c r="E5" t="s">
-        <v>117</v>
-      </c>
-      <c r="F5" t="s">
-        <v>107</v>
-      </c>
-      <c r="G5">
-        <v>90363</v>
-      </c>
-      <c r="H5" t="s">
-        <v>108</v>
-      </c>
-      <c r="I5" t="s">
-        <v>192</v>
-      </c>
-      <c r="J5" t="s">
-        <v>191</v>
-      </c>
-      <c r="K5" t="s">
-        <v>169</v>
-      </c>
-      <c r="L5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>119</v>
-      </c>
-      <c r="E6" t="s">
-        <v>120</v>
-      </c>
-      <c r="F6" t="s">
-        <v>107</v>
-      </c>
-      <c r="G6">
-        <v>90402</v>
-      </c>
-      <c r="H6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I6" t="s">
-        <v>192</v>
-      </c>
-      <c r="J6" t="s">
-        <v>191</v>
-      </c>
-      <c r="K6" t="s">
-        <v>169</v>
-      </c>
-      <c r="L6" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>121</v>
-      </c>
-      <c r="B7" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>122</v>
-      </c>
-      <c r="E7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F7" t="s">
-        <v>107</v>
-      </c>
-      <c r="G7">
-        <v>90606</v>
-      </c>
-      <c r="H7" t="s">
-        <v>108</v>
-      </c>
-      <c r="I7" t="s">
-        <v>192</v>
-      </c>
-      <c r="J7" t="s">
-        <v>191</v>
-      </c>
-      <c r="K7" t="s">
-        <v>169</v>
-      </c>
-      <c r="L7" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>124</v>
-      </c>
-      <c r="B8" t="b">
-        <v>1</v>
-      </c>
-      <c r="C8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>125</v>
-      </c>
-      <c r="E8" t="s">
-        <v>126</v>
-      </c>
-      <c r="F8" t="s">
-        <v>107</v>
-      </c>
-      <c r="G8">
-        <v>90620</v>
-      </c>
-      <c r="H8" t="s">
-        <v>108</v>
-      </c>
-      <c r="I8" t="s">
-        <v>192</v>
-      </c>
-      <c r="J8" t="s">
-        <v>191</v>
-      </c>
-      <c r="K8" t="s">
-        <v>169</v>
-      </c>
-      <c r="L8" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>127</v>
-      </c>
-      <c r="B9" t="b">
-        <v>1</v>
-      </c>
-      <c r="C9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>128</v>
-      </c>
-      <c r="E9" t="s">
-        <v>129</v>
-      </c>
-      <c r="F9" t="s">
-        <v>107</v>
-      </c>
-      <c r="G9">
-        <v>90630</v>
-      </c>
-      <c r="H9" t="s">
-        <v>108</v>
-      </c>
-      <c r="I9" t="s">
-        <v>192</v>
-      </c>
-      <c r="J9" t="s">
-        <v>191</v>
-      </c>
-      <c r="K9" t="s">
-        <v>169</v>
-      </c>
-      <c r="L9" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>130</v>
-      </c>
-      <c r="B10" t="b">
-        <v>1</v>
-      </c>
-      <c r="C10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>131</v>
-      </c>
-      <c r="E10" t="s">
-        <v>132</v>
-      </c>
-      <c r="F10" t="s">
-        <v>107</v>
-      </c>
-      <c r="G10">
-        <v>90631</v>
-      </c>
-      <c r="H10" t="s">
-        <v>108</v>
-      </c>
-      <c r="I10" t="s">
-        <v>192</v>
-      </c>
-      <c r="J10" t="s">
-        <v>191</v>
-      </c>
-      <c r="K10" t="s">
-        <v>169</v>
-      </c>
-      <c r="L10" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>133</v>
-      </c>
-      <c r="B11" t="b">
-        <v>1</v>
-      </c>
-      <c r="C11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>134</v>
-      </c>
-      <c r="E11" t="s">
-        <v>135</v>
-      </c>
-      <c r="F11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G11">
-        <v>90713</v>
-      </c>
-      <c r="H11" t="s">
-        <v>108</v>
-      </c>
-      <c r="I11" t="s">
-        <v>192</v>
-      </c>
-      <c r="J11" t="s">
-        <v>191</v>
-      </c>
-      <c r="K11" t="s">
-        <v>169</v>
-      </c>
-      <c r="L11" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>136</v>
-      </c>
-      <c r="B12" t="b">
-        <v>1</v>
-      </c>
-      <c r="C12" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>137</v>
-      </c>
-      <c r="E12" t="s">
-        <v>138</v>
-      </c>
-      <c r="F12" t="s">
-        <v>107</v>
-      </c>
-      <c r="G12">
-        <v>91344</v>
-      </c>
-      <c r="H12" t="s">
-        <v>108</v>
-      </c>
-      <c r="I12" t="s">
-        <v>192</v>
-      </c>
-      <c r="J12" t="s">
-        <v>191</v>
-      </c>
-      <c r="K12" t="s">
-        <v>169</v>
-      </c>
-      <c r="L12" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>139</v>
-      </c>
-      <c r="B13" t="b">
-        <v>1</v>
-      </c>
-      <c r="C13" t="b">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>140</v>
-      </c>
-      <c r="E13" t="s">
-        <v>141</v>
-      </c>
-      <c r="F13" t="s">
-        <v>107</v>
-      </c>
-      <c r="G13">
-        <v>91606</v>
-      </c>
-      <c r="H13" t="s">
-        <v>108</v>
-      </c>
-      <c r="I13" t="s">
-        <v>192</v>
-      </c>
-      <c r="J13" t="s">
-        <v>191</v>
-      </c>
-      <c r="K13" t="s">
-        <v>169</v>
-      </c>
-      <c r="L13" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>142</v>
-      </c>
-      <c r="B14" t="b">
-        <v>1</v>
-      </c>
-      <c r="C14" t="b">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>143</v>
-      </c>
-      <c r="E14" t="s">
-        <v>144</v>
-      </c>
-      <c r="F14" t="s">
-        <v>107</v>
-      </c>
-      <c r="G14">
-        <v>91803</v>
-      </c>
-      <c r="H14" t="s">
-        <v>108</v>
-      </c>
-      <c r="I14" t="s">
-        <v>192</v>
-      </c>
-      <c r="J14" t="s">
-        <v>191</v>
-      </c>
-      <c r="K14" t="s">
-        <v>169</v>
-      </c>
-      <c r="L14" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>145</v>
-      </c>
-      <c r="B15" t="b">
-        <v>1</v>
-      </c>
-      <c r="C15" t="b">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>146</v>
-      </c>
-      <c r="E15" t="s">
-        <v>147</v>
-      </c>
-      <c r="F15" t="s">
-        <v>107</v>
-      </c>
-      <c r="G15">
-        <v>92009</v>
-      </c>
-      <c r="H15" t="s">
-        <v>108</v>
-      </c>
-      <c r="I15" t="s">
-        <v>192</v>
-      </c>
-      <c r="J15" t="s">
-        <v>191</v>
-      </c>
-      <c r="K15" t="s">
-        <v>169</v>
-      </c>
-      <c r="L15" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>148</v>
-      </c>
-      <c r="B16" t="b">
-        <v>1</v>
-      </c>
-      <c r="C16" t="b">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>149</v>
-      </c>
-      <c r="E16" t="s">
-        <v>150</v>
-      </c>
-      <c r="F16" t="s">
-        <v>107</v>
-      </c>
-      <c r="G16">
-        <v>92105</v>
-      </c>
-      <c r="H16" t="s">
-        <v>108</v>
-      </c>
-      <c r="I16" t="s">
-        <v>192</v>
-      </c>
-      <c r="J16" t="s">
-        <v>191</v>
-      </c>
-      <c r="K16" t="s">
-        <v>169</v>
-      </c>
-      <c r="L16" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>151</v>
-      </c>
-      <c r="B17" t="b">
-        <v>1</v>
-      </c>
-      <c r="C17" t="b">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>152</v>
-      </c>
-      <c r="E17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F17" t="s">
-        <v>107</v>
-      </c>
-      <c r="G17">
-        <v>92284</v>
-      </c>
-      <c r="H17" t="s">
-        <v>108</v>
-      </c>
-      <c r="I17" t="s">
-        <v>192</v>
-      </c>
-      <c r="J17" t="s">
-        <v>191</v>
-      </c>
-      <c r="K17" t="s">
-        <v>169</v>
-      </c>
-      <c r="L17" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>154</v>
-      </c>
-      <c r="B18" t="b">
-        <v>1</v>
-      </c>
-      <c r="C18" t="b">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>155</v>
-      </c>
-      <c r="E18" t="s">
-        <v>156</v>
-      </c>
-      <c r="F18" t="s">
-        <v>107</v>
-      </c>
-      <c r="G18">
-        <v>92595</v>
-      </c>
-      <c r="H18" t="s">
-        <v>108</v>
-      </c>
-      <c r="I18" t="s">
-        <v>192</v>
-      </c>
-      <c r="J18" t="s">
-        <v>191</v>
-      </c>
-      <c r="K18" t="s">
-        <v>169</v>
-      </c>
-      <c r="L18" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>157</v>
-      </c>
-      <c r="B19" t="b">
-        <v>1</v>
-      </c>
-      <c r="C19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>158</v>
-      </c>
-      <c r="E19" t="s">
-        <v>159</v>
-      </c>
-      <c r="F19" t="s">
-        <v>107</v>
-      </c>
-      <c r="G19">
-        <v>92780</v>
-      </c>
-      <c r="H19" t="s">
-        <v>108</v>
-      </c>
-      <c r="I19" t="s">
-        <v>192</v>
-      </c>
-      <c r="J19" t="s">
-        <v>191</v>
-      </c>
-      <c r="K19" t="s">
-        <v>169</v>
-      </c>
-      <c r="L19" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>160</v>
-      </c>
-      <c r="B20" t="b">
-        <v>1</v>
-      </c>
-      <c r="C20" t="b">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>161</v>
-      </c>
-      <c r="E20" t="s">
-        <v>162</v>
-      </c>
-      <c r="F20" t="s">
-        <v>107</v>
-      </c>
-      <c r="G20">
-        <v>93108</v>
-      </c>
-      <c r="H20" t="s">
-        <v>108</v>
-      </c>
-      <c r="I20" t="s">
-        <v>192</v>
-      </c>
-      <c r="J20" t="s">
-        <v>191</v>
-      </c>
-      <c r="K20" t="s">
-        <v>169</v>
-      </c>
-      <c r="L20" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>163</v>
-      </c>
-      <c r="B21" t="b">
-        <v>1</v>
-      </c>
-      <c r="C21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
-        <v>164</v>
-      </c>
-      <c r="E21" t="s">
-        <v>165</v>
-      </c>
-      <c r="F21" t="s">
-        <v>107</v>
-      </c>
-      <c r="G21">
-        <v>93720</v>
-      </c>
-      <c r="H21" t="s">
-        <v>108</v>
-      </c>
-      <c r="I21" t="s">
-        <v>192</v>
-      </c>
-      <c r="J21" t="s">
-        <v>191</v>
-      </c>
-      <c r="K21" t="s">
-        <v>169</v>
-      </c>
-      <c r="L21" t="s">
-        <v>212</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -2048,10 +1177,10 @@
         <v>68</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>84</v>
@@ -2059,7 +1188,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -2068,21 +1197,21 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D3" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -2091,7 +1220,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -2111,7 +1240,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -2119,7 +1248,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -2137,13 +1266,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="B1" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C1" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="D1" t="s">
         <v>84</v>
@@ -2151,86 +1280,86 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B2" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="D2" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B3" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="D3" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B4" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="D4" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B5" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="D5" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B6" t="s">
         <v>190</v>
       </c>
-      <c r="B6" t="s">
-        <v>197</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="D6" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B7" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="D7" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -2239,7 +1368,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
@@ -2258,16 +1387,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B1" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D1" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="E1" t="s">
         <v>84</v>
@@ -2278,16 +1407,16 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="C2" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="D2" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="E2" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2295,16 +1424,16 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="C3" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="D3" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="E3" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2312,16 +1441,16 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="C4" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="D4" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="E4" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2329,16 +1458,16 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C5" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="D5" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="E5" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2346,16 +1475,16 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C6" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="D6" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="E6" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2363,16 +1492,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C7" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="D7" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="E7" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -2380,7 +1509,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
@@ -2477,7 +1606,7 @@
         <v>2400</v>
       </c>
       <c r="L2" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2515,7 +1644,7 @@
         <v>3000</v>
       </c>
       <c r="L3" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2553,7 +1682,7 @@
         <v>3000</v>
       </c>
       <c r="L4" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -2561,45 +1690,59 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="55.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D2" t="s">
         <v>228</v>
       </c>
-      <c r="B1" t="s">
-        <v>229</v>
-      </c>
-      <c r="C1" t="s">
-        <v>230</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E2" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="F2" t="s">
         <v>232</v>
-      </c>
-      <c r="B2" t="s">
-        <v>233</v>
-      </c>
-      <c r="C2" t="s">
-        <v>234</v>
-      </c>
-      <c r="D2" t="s">
-        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -2695,7 +1838,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>80</v>
@@ -2751,78 +1894,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="60.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="60.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2846,10 +1920,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C2" t="s">
         <v>59</v>
@@ -2861,11 +1935,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2921,7 +1995,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L19"/>
   <sheetViews>
@@ -3623,7 +2697,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -3644,33 +2718,33 @@
         <v>68</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>97</v>
-      </c>
       <c r="I1" s="2" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -3691,10 +2765,10 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
+        <v>163</v>
+      </c>
+      <c r="I2" t="s">
         <v>169</v>
-      </c>
-      <c r="I2" t="s">
-        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -3702,7 +2776,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -3717,26 +2791,886 @@
         <v>68</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>176</v>
+        <v>169</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L21"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="60.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="25.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="27.85546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="26.28515625" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J1" t="s">
+        <v>96</v>
+      </c>
+      <c r="K1" t="s">
+        <v>97</v>
+      </c>
+      <c r="L1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2">
+        <v>90001</v>
+      </c>
+      <c r="H2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2" t="s">
+        <v>185</v>
+      </c>
+      <c r="J2" t="s">
+        <v>184</v>
+      </c>
+      <c r="K2" t="s">
+        <v>163</v>
+      </c>
+      <c r="L2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G3">
+        <v>90274</v>
+      </c>
+      <c r="H3" t="s">
+        <v>102</v>
+      </c>
+      <c r="I3" t="s">
+        <v>185</v>
+      </c>
+      <c r="J3" t="s">
+        <v>184</v>
+      </c>
+      <c r="K3" t="s">
+        <v>163</v>
+      </c>
+      <c r="L3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G4">
+        <v>90305</v>
+      </c>
+      <c r="H4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I4" t="s">
+        <v>185</v>
+      </c>
+      <c r="J4" t="s">
+        <v>184</v>
+      </c>
+      <c r="K4" t="s">
+        <v>163</v>
+      </c>
+      <c r="L4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F5" t="s">
+        <v>101</v>
+      </c>
+      <c r="G5">
+        <v>90363</v>
+      </c>
+      <c r="H5" t="s">
+        <v>102</v>
+      </c>
+      <c r="I5" t="s">
+        <v>185</v>
+      </c>
+      <c r="J5" t="s">
+        <v>184</v>
+      </c>
+      <c r="K5" t="s">
+        <v>163</v>
+      </c>
+      <c r="L5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G6">
+        <v>90402</v>
+      </c>
+      <c r="H6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I6" t="s">
+        <v>185</v>
+      </c>
+      <c r="J6" t="s">
+        <v>184</v>
+      </c>
+      <c r="K6" t="s">
+        <v>163</v>
+      </c>
+      <c r="L6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E7" t="s">
+        <v>117</v>
+      </c>
+      <c r="F7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G7">
+        <v>90606</v>
+      </c>
+      <c r="H7" t="s">
+        <v>102</v>
+      </c>
+      <c r="I7" t="s">
+        <v>185</v>
+      </c>
+      <c r="J7" t="s">
+        <v>184</v>
+      </c>
+      <c r="K7" t="s">
+        <v>163</v>
+      </c>
+      <c r="L7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" t="b">
+        <v>1</v>
+      </c>
+      <c r="C8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>119</v>
+      </c>
+      <c r="E8" t="s">
+        <v>120</v>
+      </c>
+      <c r="F8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G8">
+        <v>90620</v>
+      </c>
+      <c r="H8" t="s">
+        <v>102</v>
+      </c>
+      <c r="I8" t="s">
+        <v>185</v>
+      </c>
+      <c r="J8" t="s">
+        <v>184</v>
+      </c>
+      <c r="K8" t="s">
+        <v>163</v>
+      </c>
+      <c r="L8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>122</v>
+      </c>
+      <c r="E9" t="s">
+        <v>123</v>
+      </c>
+      <c r="F9" t="s">
+        <v>101</v>
+      </c>
+      <c r="G9">
+        <v>90630</v>
+      </c>
+      <c r="H9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I9" t="s">
+        <v>185</v>
+      </c>
+      <c r="J9" t="s">
+        <v>184</v>
+      </c>
+      <c r="K9" t="s">
+        <v>163</v>
+      </c>
+      <c r="L9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E10" t="s">
+        <v>126</v>
+      </c>
+      <c r="F10" t="s">
+        <v>101</v>
+      </c>
+      <c r="G10">
+        <v>90631</v>
+      </c>
+      <c r="H10" t="s">
+        <v>102</v>
+      </c>
+      <c r="I10" t="s">
+        <v>185</v>
+      </c>
+      <c r="J10" t="s">
+        <v>184</v>
+      </c>
+      <c r="K10" t="s">
+        <v>163</v>
+      </c>
+      <c r="L10" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E11" t="s">
+        <v>129</v>
+      </c>
+      <c r="F11" t="s">
+        <v>101</v>
+      </c>
+      <c r="G11">
+        <v>90713</v>
+      </c>
+      <c r="H11" t="s">
+        <v>102</v>
+      </c>
+      <c r="I11" t="s">
+        <v>185</v>
+      </c>
+      <c r="J11" t="s">
+        <v>184</v>
+      </c>
+      <c r="K11" t="s">
+        <v>163</v>
+      </c>
+      <c r="L11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>131</v>
+      </c>
+      <c r="E12" t="s">
+        <v>132</v>
+      </c>
+      <c r="F12" t="s">
+        <v>101</v>
+      </c>
+      <c r="G12">
+        <v>91344</v>
+      </c>
+      <c r="H12" t="s">
+        <v>102</v>
+      </c>
+      <c r="I12" t="s">
+        <v>185</v>
+      </c>
+      <c r="J12" t="s">
+        <v>184</v>
+      </c>
+      <c r="K12" t="s">
+        <v>163</v>
+      </c>
+      <c r="L12" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B13" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E13" t="s">
+        <v>135</v>
+      </c>
+      <c r="F13" t="s">
+        <v>101</v>
+      </c>
+      <c r="G13">
+        <v>91606</v>
+      </c>
+      <c r="H13" t="s">
+        <v>102</v>
+      </c>
+      <c r="I13" t="s">
+        <v>185</v>
+      </c>
+      <c r="J13" t="s">
+        <v>184</v>
+      </c>
+      <c r="K13" t="s">
+        <v>163</v>
+      </c>
+      <c r="L13" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>136</v>
+      </c>
+      <c r="B14" t="b">
+        <v>1</v>
+      </c>
+      <c r="C14" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>137</v>
+      </c>
+      <c r="E14" t="s">
+        <v>138</v>
+      </c>
+      <c r="F14" t="s">
+        <v>101</v>
+      </c>
+      <c r="G14">
+        <v>91803</v>
+      </c>
+      <c r="H14" t="s">
+        <v>102</v>
+      </c>
+      <c r="I14" t="s">
+        <v>185</v>
+      </c>
+      <c r="J14" t="s">
+        <v>184</v>
+      </c>
+      <c r="K14" t="s">
+        <v>163</v>
+      </c>
+      <c r="L14" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B15" t="b">
+        <v>1</v>
+      </c>
+      <c r="C15" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>140</v>
+      </c>
+      <c r="E15" t="s">
+        <v>141</v>
+      </c>
+      <c r="F15" t="s">
+        <v>101</v>
+      </c>
+      <c r="G15">
+        <v>92009</v>
+      </c>
+      <c r="H15" t="s">
+        <v>102</v>
+      </c>
+      <c r="I15" t="s">
+        <v>185</v>
+      </c>
+      <c r="J15" t="s">
+        <v>184</v>
+      </c>
+      <c r="K15" t="s">
+        <v>163</v>
+      </c>
+      <c r="L15" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B16" t="b">
+        <v>1</v>
+      </c>
+      <c r="C16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>143</v>
+      </c>
+      <c r="E16" t="s">
+        <v>144</v>
+      </c>
+      <c r="F16" t="s">
+        <v>101</v>
+      </c>
+      <c r="G16">
+        <v>92105</v>
+      </c>
+      <c r="H16" t="s">
+        <v>102</v>
+      </c>
+      <c r="I16" t="s">
+        <v>185</v>
+      </c>
+      <c r="J16" t="s">
+        <v>184</v>
+      </c>
+      <c r="K16" t="s">
+        <v>163</v>
+      </c>
+      <c r="L16" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>145</v>
+      </c>
+      <c r="B17" t="b">
+        <v>1</v>
+      </c>
+      <c r="C17" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>146</v>
+      </c>
+      <c r="E17" t="s">
+        <v>147</v>
+      </c>
+      <c r="F17" t="s">
+        <v>101</v>
+      </c>
+      <c r="G17">
+        <v>92284</v>
+      </c>
+      <c r="H17" t="s">
+        <v>102</v>
+      </c>
+      <c r="I17" t="s">
+        <v>185</v>
+      </c>
+      <c r="J17" t="s">
+        <v>184</v>
+      </c>
+      <c r="K17" t="s">
+        <v>163</v>
+      </c>
+      <c r="L17" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B18" t="b">
+        <v>1</v>
+      </c>
+      <c r="C18" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>149</v>
+      </c>
+      <c r="E18" t="s">
+        <v>150</v>
+      </c>
+      <c r="F18" t="s">
+        <v>101</v>
+      </c>
+      <c r="G18">
+        <v>92595</v>
+      </c>
+      <c r="H18" t="s">
+        <v>102</v>
+      </c>
+      <c r="I18" t="s">
+        <v>185</v>
+      </c>
+      <c r="J18" t="s">
+        <v>184</v>
+      </c>
+      <c r="K18" t="s">
+        <v>163</v>
+      </c>
+      <c r="L18" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>151</v>
+      </c>
+      <c r="B19" t="b">
+        <v>1</v>
+      </c>
+      <c r="C19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>152</v>
+      </c>
+      <c r="E19" t="s">
+        <v>153</v>
+      </c>
+      <c r="F19" t="s">
+        <v>101</v>
+      </c>
+      <c r="G19">
+        <v>92780</v>
+      </c>
+      <c r="H19" t="s">
+        <v>102</v>
+      </c>
+      <c r="I19" t="s">
+        <v>185</v>
+      </c>
+      <c r="J19" t="s">
+        <v>184</v>
+      </c>
+      <c r="K19" t="s">
+        <v>163</v>
+      </c>
+      <c r="L19" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>154</v>
+      </c>
+      <c r="B20" t="b">
+        <v>1</v>
+      </c>
+      <c r="C20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>155</v>
+      </c>
+      <c r="E20" t="s">
+        <v>156</v>
+      </c>
+      <c r="F20" t="s">
+        <v>101</v>
+      </c>
+      <c r="G20">
+        <v>93108</v>
+      </c>
+      <c r="H20" t="s">
+        <v>102</v>
+      </c>
+      <c r="I20" t="s">
+        <v>185</v>
+      </c>
+      <c r="J20" t="s">
+        <v>184</v>
+      </c>
+      <c r="K20" t="s">
+        <v>163</v>
+      </c>
+      <c r="L20" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>157</v>
+      </c>
+      <c r="B21" t="b">
+        <v>1</v>
+      </c>
+      <c r="C21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>158</v>
+      </c>
+      <c r="E21" t="s">
+        <v>159</v>
+      </c>
+      <c r="F21" t="s">
+        <v>101</v>
+      </c>
+      <c r="G21">
+        <v>93720</v>
+      </c>
+      <c r="H21" t="s">
+        <v>102</v>
+      </c>
+      <c r="I21" t="s">
+        <v>185</v>
+      </c>
+      <c r="J21" t="s">
+        <v>184</v>
+      </c>
+      <c r="K21" t="s">
+        <v>163</v>
+      </c>
+      <c r="L21" t="s">
+        <v>205</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
few more changes in data creation & automation
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
+++ b/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
@@ -3,8 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\auto\sahi_pro\userdata\scripts\Sahi_Project\svmx\test_lab\test_cases\optimax\op_excleData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="5640" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="5640" firstSheet="11" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="User_Details" sheetId="1" r:id="rId1"/>
@@ -24,7 +29,6 @@
     <sheet name="Rules" sheetId="21" r:id="rId15"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:H16"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="232">
   <si>
     <t>UserName</t>
   </si>
@@ -582,120 +586,6 @@
     <t>SVMXC__Skill__c</t>
   </si>
   <si>
-    <t>a2N3B000000GzViUAK</t>
-  </si>
-  <si>
-    <t>0013B00000I4z82QAB</t>
-  </si>
-  <si>
-    <t>a2N3B000000GzW7UAK</t>
-  </si>
-  <si>
-    <t>a1y3B000000HhmyQAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4u3QAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4u4QAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4u5QAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4u6QAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4u7QAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4u8QAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4u9QAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4uAQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4uBQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4uCQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4uDQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4uEQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4uFQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4uGQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4uHQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4uIQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4uJQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4uKQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4uLQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4uMQAS</t>
-  </si>
-  <si>
-    <t>a2D3B000002LX9AUAW</t>
-  </si>
-  <si>
-    <t>a2D3B000002LX9BUAW</t>
-  </si>
-  <si>
-    <t>a1x3B0000002sRqQAI</t>
-  </si>
-  <si>
-    <t>a1x3B0000002sRrQAI</t>
-  </si>
-  <si>
-    <t>a1x3B0000002sRsQAI</t>
-  </si>
-  <si>
-    <t>a1x3B0000002sRtQAI</t>
-  </si>
-  <si>
-    <t>a1x3B0000002sRuQAI</t>
-  </si>
-  <si>
-    <t>a1x3B0000002sRvQAI</t>
-  </si>
-  <si>
-    <t>a133B000000OIxzQAG</t>
-  </si>
-  <si>
-    <t>a133B000000OIy0QAG</t>
-  </si>
-  <si>
-    <t>a133B000000OIy1QAG</t>
-  </si>
-  <si>
-    <t>a133B000000OIy2QAG</t>
-  </si>
-  <si>
-    <t>a133B000000OIy3QAG</t>
-  </si>
-  <si>
-    <t>a133B000000OIy4QAG</t>
-  </si>
-  <si>
     <t>Work Order for 6694</t>
   </si>
   <si>
@@ -733,6 +623,117 @@
   </si>
   <si>
     <t>AutomationChildTerritory_Mon Oct 23 2017 15:09:26 GMT+0530 (IST)</t>
+  </si>
+  <si>
+    <t>0013B00000I51lXQAR</t>
+  </si>
+  <si>
+    <t>a2N3B000000GzxNUAS</t>
+  </si>
+  <si>
+    <t>a1y3B000000HhooQAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M530QAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M531QAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M532QAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M533QAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M534QAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M535QAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M536QAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M537QAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M538QAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M539QAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M53AQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M53BQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M53CQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M53DQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M53EQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M53FQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M53GQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M53HQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M53IQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M53JQAS</t>
+  </si>
+  <si>
+    <t>a2D3B000002LXAXUA4</t>
+  </si>
+  <si>
+    <t>a2D3B000002LXAYUA4</t>
+  </si>
+  <si>
+    <t>a1x3B0000002sk1QAA</t>
+  </si>
+  <si>
+    <t>a1x3B0000002sk2QAA</t>
+  </si>
+  <si>
+    <t>a1x3B0000002sk3QAA</t>
+  </si>
+  <si>
+    <t>a1x3B0000002sk4QAA</t>
+  </si>
+  <si>
+    <t>a1x3B0000002sk5QAA</t>
+  </si>
+  <si>
+    <t>a1x3B0000002sk6QAA</t>
+  </si>
+  <si>
+    <t>a133B000000OJ2NQAW</t>
+  </si>
+  <si>
+    <t>a133B000000OJ2OQAW</t>
+  </si>
+  <si>
+    <t>a133B000000OJ2PQAW</t>
+  </si>
+  <si>
+    <t>a133B000000OJ2QQAW</t>
+  </si>
+  <si>
+    <t>a133B000000OJ2RQAW</t>
+  </si>
+  <si>
+    <t>a133B000000OJ2SQAW</t>
   </si>
 </sst>
 </file>
@@ -1163,7 +1164,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1197,7 +1198,7 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1211,7 +1212,7 @@
         <v>162</v>
       </c>
       <c r="D3" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -1253,7 +1254,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1280,86 +1281,86 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="B2" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>175</v>
       </c>
       <c r="D2" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="B3" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>175</v>
       </c>
       <c r="D3" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="B4" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>176</v>
       </c>
       <c r="D4" t="s">
-        <v>216</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="B5" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>176</v>
       </c>
       <c r="D5" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="B6" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>177</v>
       </c>
       <c r="D6" t="s">
-        <v>218</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="B7" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>177</v>
       </c>
       <c r="D7" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -1407,16 +1408,16 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="C2" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="D2" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="E2" t="s">
-        <v>208</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1424,16 +1425,16 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="C3" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="D3" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="E3" t="s">
-        <v>209</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1441,16 +1442,16 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="C4" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="D4" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="E4" t="s">
-        <v>210</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1458,16 +1459,16 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="C5" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="D5" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="E5" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1475,16 +1476,16 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="C6" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="D6" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="E6" t="s">
-        <v>212</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1492,16 +1493,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="C7" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="D7" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="E7" t="s">
-        <v>213</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -1511,10 +1512,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1531,9 +1532,10 @@
     <col min="10" max="10" width="36.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="30.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1561,7 +1563,7 @@
       <c r="I1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K1" t="s">
@@ -1570,8 +1572,11 @@
       <c r="L1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1591,7 +1596,7 @@
         <v>22</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>59</v>
+        <v>196</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>21</v>
@@ -1600,16 +1605,19 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>20</v>
+        <v>169</v>
       </c>
       <c r="K2">
         <v>2400</v>
       </c>
       <c r="L2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+      <c r="M2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1629,7 +1637,7 @@
         <v>22</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>59</v>
+        <v>196</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>21</v>
@@ -1638,16 +1646,19 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>20</v>
+        <v>169</v>
       </c>
       <c r="K3">
         <v>3000</v>
       </c>
       <c r="L3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+      <c r="M3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1667,7 +1678,7 @@
         <v>22</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>59</v>
+        <v>196</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>21</v>
@@ -1676,13 +1687,16 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>20</v>
+        <v>169</v>
       </c>
       <c r="K4">
         <v>3000</v>
       </c>
       <c r="L4" t="s">
-        <v>220</v>
+        <v>182</v>
+      </c>
+      <c r="M4" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -1707,42 +1721,42 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>221</v>
+        <v>183</v>
       </c>
       <c r="B1" t="s">
-        <v>222</v>
+        <v>184</v>
       </c>
       <c r="C1" t="s">
-        <v>223</v>
+        <v>185</v>
       </c>
       <c r="D1" t="s">
-        <v>224</v>
+        <v>186</v>
       </c>
       <c r="E1" t="s">
-        <v>229</v>
+        <v>191</v>
       </c>
       <c r="F1" t="s">
-        <v>230</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>225</v>
+        <v>187</v>
       </c>
       <c r="B2" t="s">
-        <v>226</v>
+        <v>188</v>
       </c>
       <c r="C2" t="s">
-        <v>227</v>
+        <v>189</v>
       </c>
       <c r="D2" t="s">
-        <v>228</v>
+        <v>190</v>
       </c>
       <c r="E2" t="s">
-        <v>231</v>
+        <v>193</v>
       </c>
       <c r="F2" t="s">
-        <v>232</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -1782,7 +1796,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>84</v>
+        <v>163</v>
       </c>
       <c r="B1" t="s">
         <v>68</v>
@@ -1838,7 +1852,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>80</v>
@@ -1896,7 +1910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2702,7 +2716,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2739,7 +2753,7 @@
         <v>91</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>182</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2905,16 +2919,16 @@
         <v>102</v>
       </c>
       <c r="I2" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="J2" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="K2" t="s">
         <v>163</v>
       </c>
       <c r="L2" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2943,16 +2957,16 @@
         <v>102</v>
       </c>
       <c r="I3" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="J3" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="K3" t="s">
         <v>163</v>
       </c>
       <c r="L3" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2981,16 +2995,16 @@
         <v>102</v>
       </c>
       <c r="I4" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="J4" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="K4" t="s">
         <v>163</v>
       </c>
       <c r="L4" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -3019,16 +3033,16 @@
         <v>102</v>
       </c>
       <c r="I5" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="J5" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="K5" t="s">
         <v>163</v>
       </c>
       <c r="L5" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -3057,16 +3071,16 @@
         <v>102</v>
       </c>
       <c r="I6" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="J6" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="K6" t="s">
         <v>163</v>
       </c>
       <c r="L6" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -3095,16 +3109,16 @@
         <v>102</v>
       </c>
       <c r="I7" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="J7" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="K7" t="s">
         <v>163</v>
       </c>
       <c r="L7" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -3133,16 +3147,16 @@
         <v>102</v>
       </c>
       <c r="I8" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="J8" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="K8" t="s">
         <v>163</v>
       </c>
       <c r="L8" t="s">
-        <v>192</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -3171,16 +3185,16 @@
         <v>102</v>
       </c>
       <c r="I9" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="J9" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="K9" t="s">
         <v>163</v>
       </c>
       <c r="L9" t="s">
-        <v>193</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -3209,16 +3223,16 @@
         <v>102</v>
       </c>
       <c r="I10" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="J10" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="K10" t="s">
         <v>163</v>
       </c>
       <c r="L10" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -3247,16 +3261,16 @@
         <v>102</v>
       </c>
       <c r="I11" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="J11" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="K11" t="s">
         <v>163</v>
       </c>
       <c r="L11" t="s">
-        <v>195</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -3285,16 +3299,16 @@
         <v>102</v>
       </c>
       <c r="I12" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="J12" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="K12" t="s">
         <v>163</v>
       </c>
       <c r="L12" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -3323,16 +3337,16 @@
         <v>102</v>
       </c>
       <c r="I13" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="J13" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="K13" t="s">
         <v>163</v>
       </c>
       <c r="L13" t="s">
-        <v>197</v>
+        <v>209</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -3361,16 +3375,16 @@
         <v>102</v>
       </c>
       <c r="I14" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="J14" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="K14" t="s">
         <v>163</v>
       </c>
       <c r="L14" t="s">
-        <v>198</v>
+        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -3399,16 +3413,16 @@
         <v>102</v>
       </c>
       <c r="I15" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="J15" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="K15" t="s">
         <v>163</v>
       </c>
       <c r="L15" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -3437,16 +3451,16 @@
         <v>102</v>
       </c>
       <c r="I16" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="J16" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="K16" t="s">
         <v>163</v>
       </c>
       <c r="L16" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -3475,16 +3489,16 @@
         <v>102</v>
       </c>
       <c r="I17" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="J17" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="K17" t="s">
         <v>163</v>
       </c>
       <c r="L17" t="s">
-        <v>201</v>
+        <v>213</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -3513,16 +3527,16 @@
         <v>102</v>
       </c>
       <c r="I18" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="J18" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="K18" t="s">
         <v>163</v>
       </c>
       <c r="L18" t="s">
-        <v>202</v>
+        <v>214</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -3551,16 +3565,16 @@
         <v>102</v>
       </c>
       <c r="I19" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="J19" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="K19" t="s">
         <v>163</v>
       </c>
       <c r="L19" t="s">
-        <v>203</v>
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -3589,16 +3603,16 @@
         <v>102</v>
       </c>
       <c r="I20" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="J20" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="K20" t="s">
         <v>163</v>
       </c>
       <c r="L20" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -3627,16 +3641,16 @@
         <v>102</v>
       </c>
       <c r="I21" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="J21" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="K21" t="s">
         <v>163</v>
       </c>
       <c r="L21" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -3670,7 +3684,7 @@
         <v>170</v>
       </c>
       <c r="B2" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RTO work order list
RTO work order list
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
+++ b/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="255">
   <si>
     <t>UserName</t>
   </si>
@@ -780,6 +780,30 @@
   </si>
   <si>
     <t>01m3B0000004DGW</t>
+  </si>
+  <si>
+    <t>Order Type</t>
+  </si>
+  <si>
+    <t>Order_Status</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Plano</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>TX</t>
   </si>
 </sst>
 </file>
@@ -1798,10 +1822,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1811,9 +1835,12 @@
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>233</v>
       </c>
@@ -1835,8 +1862,26 @@
       <c r="G1" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>247</v>
+      </c>
+      <c r="I1" t="s">
+        <v>248</v>
+      </c>
+      <c r="J1" t="s">
+        <v>249</v>
+      </c>
+      <c r="K1" t="s">
+        <v>250</v>
+      </c>
+      <c r="L1" t="s">
+        <v>251</v>
+      </c>
+      <c r="M1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>234</v>
       </c>
@@ -1857,6 +1902,24 @@
       </c>
       <c r="G2" t="s">
         <v>246</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2">
+        <v>75024</v>
+      </c>
+      <c r="K2" t="s">
+        <v>102</v>
+      </c>
+      <c r="L2" t="s">
+        <v>252</v>
+      </c>
+      <c r="M2" t="s">
+        <v>254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated  automation excel sheet (adding Account & 80 WO)
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
+++ b/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\auto\sahi_pro\userdata\scripts\Sahi_Project\svmx\test_lab\test_cases\optimax\op_excleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11580" windowHeight="4650" firstSheet="13" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11580" windowHeight="4650" firstSheet="10" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="User_Details" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="321">
   <si>
     <t>UserName</t>
   </si>
@@ -734,9 +734,6 @@
     <t>Child Territory</t>
   </si>
   <si>
-    <t>AutomationTerritory_Mon Oct 23 2017 14:58:18 GMT+0530 (IST)</t>
-  </si>
-  <si>
     <t>AutomationChildTerritory_Mon Oct 23 2017 15:09:26 GMT+0530 (IST)</t>
   </si>
   <si>
@@ -806,20 +803,211 @@
     <t>TX</t>
   </si>
   <si>
-    <t>AutomationTerritory_Tue Oct 24 2017 16:17:38 GMT+0530 (IST)</t>
-  </si>
-  <si>
-    <t>AutomationTerritory_Tue Oct 24 2017 16:55:55 GMT+0530 (IST)</t>
-  </si>
-  <si>
     <t>AutomationTerritory_Tue Oct 24 2017 17:01:45 GMT+0530 (IST)</t>
+  </si>
+  <si>
+    <t>a2N3B000000H0MHUA0</t>
+  </si>
+  <si>
+    <t>0013B00000I5bpsQAB</t>
+  </si>
+  <si>
+    <t>Rue Du Bailli 82</t>
+  </si>
+  <si>
+    <t>Chaussee De Roodebeek 260</t>
+  </si>
+  <si>
+    <t>Broekstraat 1</t>
+  </si>
+  <si>
+    <t>Sint-Kwintensberg 52</t>
+  </si>
+  <si>
+    <t>Georges Van Dammeplein 6</t>
+  </si>
+  <si>
+    <t>Ommeganglaan 60A</t>
+  </si>
+  <si>
+    <t>Harelbekestraat 136</t>
+  </si>
+  <si>
+    <t>Zeedijk 124</t>
+  </si>
+  <si>
+    <t>Heirweg 33</t>
+  </si>
+  <si>
+    <t>Kerkeneind 26</t>
+  </si>
+  <si>
+    <t>Avenue Winston-Churchill 9</t>
+  </si>
+  <si>
+    <t>Hoogstraat 70-72</t>
+  </si>
+  <si>
+    <t>Rue Paulin Ladeuze 4</t>
+  </si>
+  <si>
+    <t>Aartshertoginnestraat 2</t>
+  </si>
+  <si>
+    <t>Place Rabelais 36-38</t>
+  </si>
+  <si>
+    <t>Avenue Charles Deliege 18</t>
+  </si>
+  <si>
+    <t>Av. des Anc. Combattants 350</t>
+  </si>
+  <si>
+    <t>Molenbergstraat 17</t>
+  </si>
+  <si>
+    <t>Grand-Place 15</t>
+  </si>
+  <si>
+    <t>Ferdinand Maesstraat 60</t>
+  </si>
+  <si>
+    <t>Rue Neuvice 5</t>
+  </si>
+  <si>
+    <t>0013B00000I5bptQAB</t>
+  </si>
+  <si>
+    <t>Kruisstraat 162</t>
+  </si>
+  <si>
+    <t>Chaussee De Gand 1096</t>
+  </si>
+  <si>
+    <t>Winketkaai 32</t>
+  </si>
+  <si>
+    <t>Place Des Tilleuls 54</t>
+  </si>
+  <si>
+    <t>Hemelrijk 3</t>
+  </si>
+  <si>
+    <t>Rue De Huy 2</t>
+  </si>
+  <si>
+    <t>Handelsstraat 33</t>
+  </si>
+  <si>
+    <t>Stationsplein 2</t>
+  </si>
+  <si>
+    <t>Saint-Pierre 14</t>
+  </si>
+  <si>
+    <t>Kasteelstraat 22</t>
+  </si>
+  <si>
+    <t>Rue Des Rotisseurs 11, E 3</t>
+  </si>
+  <si>
+    <t>Place De L'Universite 21</t>
+  </si>
+  <si>
+    <t>Avenue Charles Deliege 13</t>
+  </si>
+  <si>
+    <t>Place des Sciences 3, A</t>
+  </si>
+  <si>
+    <t>Grote Markt 17</t>
+  </si>
+  <si>
+    <t>Armeduivelstraat 1</t>
+  </si>
+  <si>
+    <t>Nieuwedokstraat 12</t>
+  </si>
+  <si>
+    <t>Lange Lobroekstraat 113</t>
+  </si>
+  <si>
+    <t>Mechelsesteenweg 4</t>
+  </si>
+  <si>
+    <t>Herkenrode Abdij ZN</t>
+  </si>
+  <si>
+    <t>Zandvoordestraat 93</t>
+  </si>
+  <si>
+    <t>Grote Baan 171</t>
+  </si>
+  <si>
+    <t>Mechelsestraat 55</t>
+  </si>
+  <si>
+    <t>F. Van Cauwenberghstraat 7</t>
+  </si>
+  <si>
+    <t>Markt ZN</t>
+  </si>
+  <si>
+    <t>Marneflaan 3, bus Z</t>
+  </si>
+  <si>
+    <t>Rue Verckruyts 5</t>
+  </si>
+  <si>
+    <t>Rue De Ciney 45</t>
+  </si>
+  <si>
+    <t>Zuivelmarkt 64</t>
+  </si>
+  <si>
+    <t>Grotesteenweg 395-399</t>
+  </si>
+  <si>
+    <t>Kapelstraat 2</t>
+  </si>
+  <si>
+    <t>Rondeweg 2</t>
+  </si>
+  <si>
+    <t>Ruelle Dedale 1A, 201/207</t>
+  </si>
+  <si>
+    <t>Avenue Charles Deliège 7</t>
+  </si>
+  <si>
+    <t>Bld Du Centenaire 1</t>
+  </si>
+  <si>
+    <t>Rue Keramis 9</t>
+  </si>
+  <si>
+    <t>Landbouwstraat ZN</t>
+  </si>
+  <si>
+    <t>Rue De Bouvignes SN</t>
+  </si>
+  <si>
+    <t>Gelukstede 1</t>
+  </si>
+  <si>
+    <t>Wijngaardstraat 8</t>
+  </si>
+  <si>
+    <t>Liezele-Dorp 102</t>
+  </si>
+  <si>
+    <t>John - Automation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1206,9 +1394,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="34.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="26.5703125" collapsed="true"/>
+    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1249,8 +1437,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1311,7 +1499,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -1339,10 +1527,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="27.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1459,11 +1647,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="1" max="1" width="22" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1592,29 +1780,29 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="45.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="36.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="30.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="25.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="45.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="36.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="30.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="19" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1651,8 +1839,11 @@
       <c r="L1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1672,7 +1863,7 @@
         <v>22</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>59</v>
+        <v>255</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>21</v>
@@ -1681,7 +1872,7 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>20</v>
+        <v>163</v>
       </c>
       <c r="K2">
         <v>2400</v>
@@ -1689,8 +1880,11 @@
       <c r="L2" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1710,7 +1904,7 @@
         <v>22</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>59</v>
+        <v>255</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>21</v>
@@ -1719,7 +1913,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>20</v>
+        <v>163</v>
       </c>
       <c r="K3">
         <v>3000</v>
@@ -1727,8 +1921,11 @@
       <c r="L3" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1748,7 +1945,7 @@
         <v>22</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>59</v>
+        <v>255</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>21</v>
@@ -1757,13 +1954,3047 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>20</v>
+        <v>163</v>
       </c>
       <c r="K4">
         <v>3000</v>
       </c>
       <c r="L4" t="s">
         <v>220</v>
+      </c>
+      <c r="M4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5">
+        <v>2900</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>255</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>163</v>
+      </c>
+      <c r="K5">
+        <v>1800</v>
+      </c>
+      <c r="L5" t="s">
+        <v>220</v>
+      </c>
+      <c r="M5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6">
+        <v>1083</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>255</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>163</v>
+      </c>
+      <c r="K6">
+        <v>1800</v>
+      </c>
+      <c r="L6" t="s">
+        <v>220</v>
+      </c>
+      <c r="M6" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7">
+        <v>1340</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" t="s">
+        <v>255</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>163</v>
+      </c>
+      <c r="K7">
+        <v>1800</v>
+      </c>
+      <c r="L7" t="s">
+        <v>220</v>
+      </c>
+      <c r="M7" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8">
+        <v>8870</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" t="s">
+        <v>255</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>163</v>
+      </c>
+      <c r="K8">
+        <v>3000</v>
+      </c>
+      <c r="L8" t="s">
+        <v>220</v>
+      </c>
+      <c r="M8" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9">
+        <v>1370</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" t="s">
+        <v>255</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" t="s">
+        <v>163</v>
+      </c>
+      <c r="K9">
+        <v>2400</v>
+      </c>
+      <c r="L9" t="s">
+        <v>220</v>
+      </c>
+      <c r="M9" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10">
+        <v>1000</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" t="s">
+        <v>255</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" t="b">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>163</v>
+      </c>
+      <c r="K10">
+        <v>2400</v>
+      </c>
+      <c r="L10" t="s">
+        <v>220</v>
+      </c>
+      <c r="M10" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11">
+        <v>2440</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" t="s">
+        <v>255</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>163</v>
+      </c>
+      <c r="K11">
+        <v>2400</v>
+      </c>
+      <c r="L11" t="s">
+        <v>220</v>
+      </c>
+      <c r="M11" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12">
+        <v>2440</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" t="s">
+        <v>255</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>163</v>
+      </c>
+      <c r="K12">
+        <v>1800</v>
+      </c>
+      <c r="L12" t="s">
+        <v>220</v>
+      </c>
+      <c r="M12" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13">
+        <v>1000</v>
+      </c>
+      <c r="F13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" t="s">
+        <v>255</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" t="s">
+        <v>163</v>
+      </c>
+      <c r="K13">
+        <v>2400</v>
+      </c>
+      <c r="L13" t="s">
+        <v>220</v>
+      </c>
+      <c r="M13" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14">
+        <v>4970</v>
+      </c>
+      <c r="F14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" t="s">
+        <v>255</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K14">
+        <v>2400</v>
+      </c>
+      <c r="L14" t="s">
+        <v>220</v>
+      </c>
+      <c r="M14" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15">
+        <v>4983</v>
+      </c>
+      <c r="F15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" t="s">
+        <v>255</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" t="b">
+        <v>1</v>
+      </c>
+      <c r="J15" t="s">
+        <v>163</v>
+      </c>
+      <c r="K15">
+        <v>2400</v>
+      </c>
+      <c r="L15" t="s">
+        <v>220</v>
+      </c>
+      <c r="M15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16">
+        <v>4834</v>
+      </c>
+      <c r="F16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" t="s">
+        <v>255</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J16" t="s">
+        <v>163</v>
+      </c>
+      <c r="K16">
+        <v>2400</v>
+      </c>
+      <c r="L16" t="s">
+        <v>220</v>
+      </c>
+      <c r="M16" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17">
+        <v>4900</v>
+      </c>
+      <c r="F17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" t="s">
+        <v>255</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" t="b">
+        <v>1</v>
+      </c>
+      <c r="J17" t="s">
+        <v>163</v>
+      </c>
+      <c r="K17">
+        <v>1800</v>
+      </c>
+      <c r="L17" t="s">
+        <v>220</v>
+      </c>
+      <c r="M17" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18">
+        <v>3300</v>
+      </c>
+      <c r="F18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" t="s">
+        <v>255</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" t="b">
+        <v>1</v>
+      </c>
+      <c r="J18" t="s">
+        <v>163</v>
+      </c>
+      <c r="K18">
+        <v>3000</v>
+      </c>
+      <c r="L18" t="s">
+        <v>220</v>
+      </c>
+      <c r="M18" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19">
+        <v>2018</v>
+      </c>
+      <c r="F19" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" t="s">
+        <v>255</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J19" t="s">
+        <v>163</v>
+      </c>
+      <c r="K19">
+        <v>2400</v>
+      </c>
+      <c r="L19" t="s">
+        <v>220</v>
+      </c>
+      <c r="M19" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>257</v>
+      </c>
+      <c r="E20">
+        <v>4400</v>
+      </c>
+      <c r="F20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" t="s">
+        <v>255</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" t="s">
+        <v>163</v>
+      </c>
+      <c r="K20">
+        <v>2400</v>
+      </c>
+      <c r="L20" t="s">
+        <v>220</v>
+      </c>
+      <c r="M20" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>258</v>
+      </c>
+      <c r="E21">
+        <v>9250</v>
+      </c>
+      <c r="F21" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" t="s">
+        <v>255</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J21" t="s">
+        <v>163</v>
+      </c>
+      <c r="K21">
+        <v>2400</v>
+      </c>
+      <c r="L21" t="s">
+        <v>220</v>
+      </c>
+      <c r="M21" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" t="s">
+        <v>259</v>
+      </c>
+      <c r="E22">
+        <v>2610</v>
+      </c>
+      <c r="F22" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" t="s">
+        <v>255</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" t="b">
+        <v>1</v>
+      </c>
+      <c r="J22" t="s">
+        <v>163</v>
+      </c>
+      <c r="K22">
+        <v>2400</v>
+      </c>
+      <c r="L22" t="s">
+        <v>220</v>
+      </c>
+      <c r="M22" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s">
+        <v>260</v>
+      </c>
+      <c r="E23">
+        <v>1050</v>
+      </c>
+      <c r="F23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" t="s">
+        <v>255</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J23" t="s">
+        <v>163</v>
+      </c>
+      <c r="K23">
+        <v>1800</v>
+      </c>
+      <c r="L23" t="s">
+        <v>220</v>
+      </c>
+      <c r="M23" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>261</v>
+      </c>
+      <c r="E24">
+        <v>1200</v>
+      </c>
+      <c r="F24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" t="s">
+        <v>255</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" t="b">
+        <v>1</v>
+      </c>
+      <c r="J24" t="s">
+        <v>163</v>
+      </c>
+      <c r="K24">
+        <v>3000</v>
+      </c>
+      <c r="L24" t="s">
+        <v>220</v>
+      </c>
+      <c r="M24" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" t="s">
+        <v>262</v>
+      </c>
+      <c r="E25">
+        <v>3300</v>
+      </c>
+      <c r="F25" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" t="s">
+        <v>255</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25" t="b">
+        <v>1</v>
+      </c>
+      <c r="J25" t="s">
+        <v>163</v>
+      </c>
+      <c r="K25">
+        <v>3000</v>
+      </c>
+      <c r="L25" t="s">
+        <v>220</v>
+      </c>
+      <c r="M25" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" t="s">
+        <v>263</v>
+      </c>
+      <c r="E26">
+        <v>9000</v>
+      </c>
+      <c r="F26" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" t="s">
+        <v>255</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I26" t="b">
+        <v>1</v>
+      </c>
+      <c r="J26" t="s">
+        <v>163</v>
+      </c>
+      <c r="K26">
+        <v>3000</v>
+      </c>
+      <c r="L26" t="s">
+        <v>220</v>
+      </c>
+      <c r="M26" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" t="s">
+        <v>264</v>
+      </c>
+      <c r="E27">
+        <v>9140</v>
+      </c>
+      <c r="F27" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" t="s">
+        <v>255</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I27" t="b">
+        <v>1</v>
+      </c>
+      <c r="J27" t="s">
+        <v>163</v>
+      </c>
+      <c r="K27">
+        <v>2400</v>
+      </c>
+      <c r="L27" t="s">
+        <v>220</v>
+      </c>
+      <c r="M27" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" t="s">
+        <v>265</v>
+      </c>
+      <c r="E28">
+        <v>9340</v>
+      </c>
+      <c r="F28" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" t="s">
+        <v>255</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I28" t="b">
+        <v>1</v>
+      </c>
+      <c r="J28" t="s">
+        <v>163</v>
+      </c>
+      <c r="K28">
+        <v>2400</v>
+      </c>
+      <c r="L28" t="s">
+        <v>220</v>
+      </c>
+      <c r="M28" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" t="s">
+        <v>266</v>
+      </c>
+      <c r="E29">
+        <v>8540</v>
+      </c>
+      <c r="F29" t="s">
+        <v>22</v>
+      </c>
+      <c r="G29" t="s">
+        <v>255</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I29" t="b">
+        <v>1</v>
+      </c>
+      <c r="J29" t="s">
+        <v>163</v>
+      </c>
+      <c r="K29">
+        <v>1800</v>
+      </c>
+      <c r="L29" t="s">
+        <v>220</v>
+      </c>
+      <c r="M29" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" t="s">
+        <v>267</v>
+      </c>
+      <c r="E30">
+        <v>8620</v>
+      </c>
+      <c r="F30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G30" t="s">
+        <v>255</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I30" t="b">
+        <v>1</v>
+      </c>
+      <c r="J30" t="s">
+        <v>163</v>
+      </c>
+      <c r="K30">
+        <v>3000</v>
+      </c>
+      <c r="L30" t="s">
+        <v>220</v>
+      </c>
+      <c r="M30" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" t="s">
+        <v>268</v>
+      </c>
+      <c r="E31">
+        <v>8430</v>
+      </c>
+      <c r="F31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G31" t="s">
+        <v>255</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I31" t="b">
+        <v>1</v>
+      </c>
+      <c r="J31" t="s">
+        <v>163</v>
+      </c>
+      <c r="K31">
+        <v>1800</v>
+      </c>
+      <c r="L31" t="s">
+        <v>220</v>
+      </c>
+      <c r="M31" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" t="s">
+        <v>269</v>
+      </c>
+      <c r="E32">
+        <v>2920</v>
+      </c>
+      <c r="F32" t="s">
+        <v>22</v>
+      </c>
+      <c r="G32" t="s">
+        <v>255</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I32" t="b">
+        <v>1</v>
+      </c>
+      <c r="J32" t="s">
+        <v>163</v>
+      </c>
+      <c r="K32">
+        <v>1800</v>
+      </c>
+      <c r="L32" t="s">
+        <v>220</v>
+      </c>
+      <c r="M32" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" t="s">
+        <v>270</v>
+      </c>
+      <c r="E33">
+        <v>5500</v>
+      </c>
+      <c r="F33" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33" t="s">
+        <v>255</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I33" t="b">
+        <v>1</v>
+      </c>
+      <c r="J33" t="s">
+        <v>163</v>
+      </c>
+      <c r="K33">
+        <v>3000</v>
+      </c>
+      <c r="L33" t="s">
+        <v>220</v>
+      </c>
+      <c r="M33" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" t="s">
+        <v>271</v>
+      </c>
+      <c r="E34">
+        <v>2000</v>
+      </c>
+      <c r="F34" t="s">
+        <v>22</v>
+      </c>
+      <c r="G34" t="s">
+        <v>255</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I34" t="b">
+        <v>1</v>
+      </c>
+      <c r="J34" t="s">
+        <v>163</v>
+      </c>
+      <c r="K34">
+        <v>2400</v>
+      </c>
+      <c r="L34" t="s">
+        <v>220</v>
+      </c>
+      <c r="M34" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" t="s">
+        <v>272</v>
+      </c>
+      <c r="E35">
+        <v>1348</v>
+      </c>
+      <c r="F35" t="s">
+        <v>22</v>
+      </c>
+      <c r="G35" t="s">
+        <v>255</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I35" t="b">
+        <v>1</v>
+      </c>
+      <c r="J35" t="s">
+        <v>163</v>
+      </c>
+      <c r="K35">
+        <v>3000</v>
+      </c>
+      <c r="L35" t="s">
+        <v>220</v>
+      </c>
+      <c r="M35" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" t="s">
+        <v>273</v>
+      </c>
+      <c r="E36">
+        <v>8400</v>
+      </c>
+      <c r="F36" t="s">
+        <v>22</v>
+      </c>
+      <c r="G36" t="s">
+        <v>255</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I36" t="b">
+        <v>1</v>
+      </c>
+      <c r="J36" t="s">
+        <v>163</v>
+      </c>
+      <c r="K36">
+        <v>2400</v>
+      </c>
+      <c r="L36" t="s">
+        <v>220</v>
+      </c>
+      <c r="M36" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" t="s">
+        <v>274</v>
+      </c>
+      <c r="E37">
+        <v>1348</v>
+      </c>
+      <c r="F37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G37" t="s">
+        <v>255</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I37" t="b">
+        <v>1</v>
+      </c>
+      <c r="J37" t="s">
+        <v>163</v>
+      </c>
+      <c r="K37">
+        <v>2400</v>
+      </c>
+      <c r="L37" t="s">
+        <v>220</v>
+      </c>
+      <c r="M37" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" t="s">
+        <v>275</v>
+      </c>
+      <c r="E38">
+        <v>7130</v>
+      </c>
+      <c r="F38" t="s">
+        <v>22</v>
+      </c>
+      <c r="G38" t="s">
+        <v>255</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I38" t="b">
+        <v>1</v>
+      </c>
+      <c r="J38" t="s">
+        <v>163</v>
+      </c>
+      <c r="K38">
+        <v>2400</v>
+      </c>
+      <c r="L38" t="s">
+        <v>220</v>
+      </c>
+      <c r="M38" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" t="s">
+        <v>276</v>
+      </c>
+      <c r="E39">
+        <v>1140</v>
+      </c>
+      <c r="F39" t="s">
+        <v>22</v>
+      </c>
+      <c r="G39" t="s">
+        <v>255</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I39" t="b">
+        <v>1</v>
+      </c>
+      <c r="J39" t="s">
+        <v>163</v>
+      </c>
+      <c r="K39">
+        <v>3000</v>
+      </c>
+      <c r="L39" t="s">
+        <v>220</v>
+      </c>
+      <c r="M39" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" t="s">
+        <v>277</v>
+      </c>
+      <c r="E40">
+        <v>2840</v>
+      </c>
+      <c r="F40" t="s">
+        <v>22</v>
+      </c>
+      <c r="G40" t="s">
+        <v>255</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I40" t="b">
+        <v>1</v>
+      </c>
+      <c r="J40" t="s">
+        <v>163</v>
+      </c>
+      <c r="K40">
+        <v>3000</v>
+      </c>
+      <c r="L40" t="s">
+        <v>220</v>
+      </c>
+      <c r="M40" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" t="s">
+        <v>279</v>
+      </c>
+      <c r="E41">
+        <v>1348</v>
+      </c>
+      <c r="F41" t="s">
+        <v>22</v>
+      </c>
+      <c r="G41" t="s">
+        <v>255</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I41" t="b">
+        <v>1</v>
+      </c>
+      <c r="J41" t="s">
+        <v>163</v>
+      </c>
+      <c r="K41">
+        <v>3000</v>
+      </c>
+      <c r="L41" t="s">
+        <v>220</v>
+      </c>
+      <c r="M41" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" t="s">
+        <v>280</v>
+      </c>
+      <c r="E42">
+        <v>2550</v>
+      </c>
+      <c r="F42" t="s">
+        <v>22</v>
+      </c>
+      <c r="G42" t="s">
+        <v>255</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I42" t="b">
+        <v>1</v>
+      </c>
+      <c r="J42" t="s">
+        <v>163</v>
+      </c>
+      <c r="K42">
+        <v>1800</v>
+      </c>
+      <c r="L42" t="s">
+        <v>220</v>
+      </c>
+      <c r="M42" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" t="s">
+        <v>281</v>
+      </c>
+      <c r="E43">
+        <v>4000</v>
+      </c>
+      <c r="F43" t="s">
+        <v>22</v>
+      </c>
+      <c r="G43" t="s">
+        <v>255</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I43" t="b">
+        <v>1</v>
+      </c>
+      <c r="J43" t="s">
+        <v>163</v>
+      </c>
+      <c r="K43">
+        <v>1800</v>
+      </c>
+      <c r="L43" t="s">
+        <v>220</v>
+      </c>
+      <c r="M43" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" t="s">
+        <v>282</v>
+      </c>
+      <c r="E44">
+        <v>2570</v>
+      </c>
+      <c r="F44" t="s">
+        <v>22</v>
+      </c>
+      <c r="G44" t="s">
+        <v>255</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I44" t="b">
+        <v>1</v>
+      </c>
+      <c r="J44" t="s">
+        <v>163</v>
+      </c>
+      <c r="K44">
+        <v>2400</v>
+      </c>
+      <c r="L44" t="s">
+        <v>220</v>
+      </c>
+      <c r="M44" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" t="s">
+        <v>283</v>
+      </c>
+      <c r="E45">
+        <v>1082</v>
+      </c>
+      <c r="F45" t="s">
+        <v>22</v>
+      </c>
+      <c r="G45" t="s">
+        <v>255</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I45" t="b">
+        <v>1</v>
+      </c>
+      <c r="J45" t="s">
+        <v>163</v>
+      </c>
+      <c r="K45">
+        <v>2280</v>
+      </c>
+      <c r="L45" t="s">
+        <v>220</v>
+      </c>
+      <c r="M45" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" t="s">
+        <v>284</v>
+      </c>
+      <c r="E46">
+        <v>2800</v>
+      </c>
+      <c r="F46" t="s">
+        <v>22</v>
+      </c>
+      <c r="G46" t="s">
+        <v>255</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I46" t="b">
+        <v>1</v>
+      </c>
+      <c r="J46" t="s">
+        <v>163</v>
+      </c>
+      <c r="K46">
+        <v>2400</v>
+      </c>
+      <c r="L46" t="s">
+        <v>220</v>
+      </c>
+      <c r="M46" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" t="s">
+        <v>285</v>
+      </c>
+      <c r="E47">
+        <v>5300</v>
+      </c>
+      <c r="F47" t="s">
+        <v>22</v>
+      </c>
+      <c r="G47" t="s">
+        <v>255</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I47" t="b">
+        <v>1</v>
+      </c>
+      <c r="J47" t="s">
+        <v>163</v>
+      </c>
+      <c r="K47">
+        <v>2400</v>
+      </c>
+      <c r="L47" t="s">
+        <v>220</v>
+      </c>
+      <c r="M47" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" t="s">
+        <v>286</v>
+      </c>
+      <c r="E48">
+        <v>3500</v>
+      </c>
+      <c r="F48" t="s">
+        <v>22</v>
+      </c>
+      <c r="G48" t="s">
+        <v>255</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I48" t="b">
+        <v>1</v>
+      </c>
+      <c r="J48" t="s">
+        <v>163</v>
+      </c>
+      <c r="K48">
+        <v>2400</v>
+      </c>
+      <c r="L48" t="s">
+        <v>220</v>
+      </c>
+      <c r="M48" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" t="s">
+        <v>287</v>
+      </c>
+      <c r="E49">
+        <v>5380</v>
+      </c>
+      <c r="F49" t="s">
+        <v>22</v>
+      </c>
+      <c r="G49" t="s">
+        <v>255</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I49" t="b">
+        <v>1</v>
+      </c>
+      <c r="J49" t="s">
+        <v>163</v>
+      </c>
+      <c r="K49">
+        <v>1800</v>
+      </c>
+      <c r="L49" t="s">
+        <v>220</v>
+      </c>
+      <c r="M49" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>6</v>
+      </c>
+      <c r="B50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" t="s">
+        <v>288</v>
+      </c>
+      <c r="E50">
+        <v>2570</v>
+      </c>
+      <c r="F50" t="s">
+        <v>22</v>
+      </c>
+      <c r="G50" t="s">
+        <v>255</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I50" t="b">
+        <v>1</v>
+      </c>
+      <c r="J50" t="s">
+        <v>163</v>
+      </c>
+      <c r="K50">
+        <v>1800</v>
+      </c>
+      <c r="L50" t="s">
+        <v>220</v>
+      </c>
+      <c r="M50" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" t="s">
+        <v>289</v>
+      </c>
+      <c r="E51">
+        <v>1982</v>
+      </c>
+      <c r="F51" t="s">
+        <v>22</v>
+      </c>
+      <c r="G51" t="s">
+        <v>255</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I51" t="b">
+        <v>1</v>
+      </c>
+      <c r="J51" t="s">
+        <v>163</v>
+      </c>
+      <c r="K51">
+        <v>1800</v>
+      </c>
+      <c r="L51" t="s">
+        <v>220</v>
+      </c>
+      <c r="M51" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" t="s">
+        <v>290</v>
+      </c>
+      <c r="E52">
+        <v>6800</v>
+      </c>
+      <c r="F52" t="s">
+        <v>22</v>
+      </c>
+      <c r="G52" t="s">
+        <v>255</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I52" t="b">
+        <v>1</v>
+      </c>
+      <c r="J52" t="s">
+        <v>163</v>
+      </c>
+      <c r="K52">
+        <v>2400</v>
+      </c>
+      <c r="L52" t="s">
+        <v>220</v>
+      </c>
+      <c r="M52" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>6</v>
+      </c>
+      <c r="B53" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" t="s">
+        <v>291</v>
+      </c>
+      <c r="E53">
+        <v>8400</v>
+      </c>
+      <c r="F53" t="s">
+        <v>22</v>
+      </c>
+      <c r="G53" t="s">
+        <v>255</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I53" t="b">
+        <v>1</v>
+      </c>
+      <c r="J53" t="s">
+        <v>163</v>
+      </c>
+      <c r="K53">
+        <v>2400</v>
+      </c>
+      <c r="L53" t="s">
+        <v>220</v>
+      </c>
+      <c r="M53" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" t="s">
+        <v>292</v>
+      </c>
+      <c r="E54">
+        <v>4500</v>
+      </c>
+      <c r="F54" t="s">
+        <v>22</v>
+      </c>
+      <c r="G54" t="s">
+        <v>255</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I54" t="b">
+        <v>1</v>
+      </c>
+      <c r="J54" t="s">
+        <v>163</v>
+      </c>
+      <c r="K54">
+        <v>3000</v>
+      </c>
+      <c r="L54" t="s">
+        <v>220</v>
+      </c>
+      <c r="M54" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>6</v>
+      </c>
+      <c r="B55" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" t="s">
+        <v>293</v>
+      </c>
+      <c r="E55">
+        <v>1348</v>
+      </c>
+      <c r="F55" t="s">
+        <v>22</v>
+      </c>
+      <c r="G55" t="s">
+        <v>255</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I55" t="b">
+        <v>1</v>
+      </c>
+      <c r="J55" t="s">
+        <v>163</v>
+      </c>
+      <c r="K55">
+        <v>4920</v>
+      </c>
+      <c r="L55" t="s">
+        <v>220</v>
+      </c>
+      <c r="M55" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" t="s">
+        <v>294</v>
+      </c>
+      <c r="E56">
+        <v>7130</v>
+      </c>
+      <c r="F56" t="s">
+        <v>22</v>
+      </c>
+      <c r="G56" t="s">
+        <v>255</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I56" t="b">
+        <v>1</v>
+      </c>
+      <c r="J56" t="s">
+        <v>163</v>
+      </c>
+      <c r="K56">
+        <v>2400</v>
+      </c>
+      <c r="L56" t="s">
+        <v>220</v>
+      </c>
+      <c r="M56" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" t="s">
+        <v>295</v>
+      </c>
+      <c r="E57">
+        <v>1348</v>
+      </c>
+      <c r="F57" t="s">
+        <v>22</v>
+      </c>
+      <c r="G57" t="s">
+        <v>255</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I57" t="b">
+        <v>1</v>
+      </c>
+      <c r="J57" t="s">
+        <v>163</v>
+      </c>
+      <c r="K57">
+        <v>2400</v>
+      </c>
+      <c r="L57" t="s">
+        <v>220</v>
+      </c>
+      <c r="M57" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" t="s">
+        <v>296</v>
+      </c>
+      <c r="E58">
+        <v>3500</v>
+      </c>
+      <c r="F58" t="s">
+        <v>22</v>
+      </c>
+      <c r="G58" t="s">
+        <v>255</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I58" t="b">
+        <v>1</v>
+      </c>
+      <c r="J58" t="s">
+        <v>163</v>
+      </c>
+      <c r="K58">
+        <v>2400</v>
+      </c>
+      <c r="L58" t="s">
+        <v>220</v>
+      </c>
+      <c r="M58" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>6</v>
+      </c>
+      <c r="B59" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" t="s">
+        <v>297</v>
+      </c>
+      <c r="E59">
+        <v>2000</v>
+      </c>
+      <c r="F59" t="s">
+        <v>22</v>
+      </c>
+      <c r="G59" t="s">
+        <v>255</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I59" t="b">
+        <v>1</v>
+      </c>
+      <c r="J59" t="s">
+        <v>163</v>
+      </c>
+      <c r="K59">
+        <v>2400</v>
+      </c>
+      <c r="L59" t="s">
+        <v>220</v>
+      </c>
+      <c r="M59" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>6</v>
+      </c>
+      <c r="B60" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" t="s">
+        <v>298</v>
+      </c>
+      <c r="E60">
+        <v>8400</v>
+      </c>
+      <c r="F60" t="s">
+        <v>22</v>
+      </c>
+      <c r="G60" t="s">
+        <v>255</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I60" t="b">
+        <v>1</v>
+      </c>
+      <c r="J60" t="s">
+        <v>163</v>
+      </c>
+      <c r="K60">
+        <v>2280</v>
+      </c>
+      <c r="L60" t="s">
+        <v>220</v>
+      </c>
+      <c r="M60" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>6</v>
+      </c>
+      <c r="B61" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61" t="s">
+        <v>299</v>
+      </c>
+      <c r="E61">
+        <v>2060</v>
+      </c>
+      <c r="F61" t="s">
+        <v>22</v>
+      </c>
+      <c r="G61" t="s">
+        <v>255</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I61" t="b">
+        <v>1</v>
+      </c>
+      <c r="J61" t="s">
+        <v>163</v>
+      </c>
+      <c r="K61">
+        <v>1800</v>
+      </c>
+      <c r="L61" t="s">
+        <v>220</v>
+      </c>
+      <c r="M61" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62" t="s">
+        <v>8</v>
+      </c>
+      <c r="C62" t="s">
+        <v>300</v>
+      </c>
+      <c r="E62">
+        <v>2640</v>
+      </c>
+      <c r="F62" t="s">
+        <v>22</v>
+      </c>
+      <c r="G62" t="s">
+        <v>255</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I62" t="b">
+        <v>1</v>
+      </c>
+      <c r="J62" t="s">
+        <v>163</v>
+      </c>
+      <c r="K62">
+        <v>3360</v>
+      </c>
+      <c r="L62" t="s">
+        <v>220</v>
+      </c>
+      <c r="M62" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>6</v>
+      </c>
+      <c r="B63" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" t="s">
+        <v>301</v>
+      </c>
+      <c r="E63">
+        <v>3511</v>
+      </c>
+      <c r="F63" t="s">
+        <v>22</v>
+      </c>
+      <c r="G63" t="s">
+        <v>255</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I63" t="b">
+        <v>1</v>
+      </c>
+      <c r="J63" t="s">
+        <v>163</v>
+      </c>
+      <c r="K63">
+        <v>2400</v>
+      </c>
+      <c r="L63" t="s">
+        <v>220</v>
+      </c>
+      <c r="M63" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>6</v>
+      </c>
+      <c r="B64" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" t="s">
+        <v>302</v>
+      </c>
+      <c r="E64">
+        <v>8400</v>
+      </c>
+      <c r="F64" t="s">
+        <v>22</v>
+      </c>
+      <c r="G64" t="s">
+        <v>255</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I64" t="b">
+        <v>1</v>
+      </c>
+      <c r="J64" t="s">
+        <v>163</v>
+      </c>
+      <c r="K64">
+        <v>2400</v>
+      </c>
+      <c r="L64" t="s">
+        <v>220</v>
+      </c>
+      <c r="M64" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>6</v>
+      </c>
+      <c r="B65" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65" t="s">
+        <v>303</v>
+      </c>
+      <c r="E65">
+        <v>3511</v>
+      </c>
+      <c r="F65" t="s">
+        <v>22</v>
+      </c>
+      <c r="G65" t="s">
+        <v>255</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I65" t="b">
+        <v>1</v>
+      </c>
+      <c r="J65" t="s">
+        <v>163</v>
+      </c>
+      <c r="K65">
+        <v>2400</v>
+      </c>
+      <c r="L65" t="s">
+        <v>220</v>
+      </c>
+      <c r="M65" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>6</v>
+      </c>
+      <c r="B66" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66" t="s">
+        <v>304</v>
+      </c>
+      <c r="E66">
+        <v>1800</v>
+      </c>
+      <c r="F66" t="s">
+        <v>22</v>
+      </c>
+      <c r="G66" t="s">
+        <v>255</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I66" t="b">
+        <v>1</v>
+      </c>
+      <c r="J66" t="s">
+        <v>163</v>
+      </c>
+      <c r="K66">
+        <v>2400</v>
+      </c>
+      <c r="L66" t="s">
+        <v>220</v>
+      </c>
+      <c r="M66" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>6</v>
+      </c>
+      <c r="B67" t="s">
+        <v>8</v>
+      </c>
+      <c r="C67" t="s">
+        <v>305</v>
+      </c>
+      <c r="E67">
+        <v>2500</v>
+      </c>
+      <c r="F67" t="s">
+        <v>22</v>
+      </c>
+      <c r="G67" t="s">
+        <v>255</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I67" t="b">
+        <v>1</v>
+      </c>
+      <c r="J67" t="s">
+        <v>163</v>
+      </c>
+      <c r="K67">
+        <v>1800</v>
+      </c>
+      <c r="L67" t="s">
+        <v>220</v>
+      </c>
+      <c r="M67" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>6</v>
+      </c>
+      <c r="B68" t="s">
+        <v>8</v>
+      </c>
+      <c r="C68" t="s">
+        <v>306</v>
+      </c>
+      <c r="E68">
+        <v>2840</v>
+      </c>
+      <c r="F68" t="s">
+        <v>22</v>
+      </c>
+      <c r="G68" t="s">
+        <v>255</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I68" t="b">
+        <v>1</v>
+      </c>
+      <c r="J68" t="s">
+        <v>163</v>
+      </c>
+      <c r="K68">
+        <v>2400</v>
+      </c>
+      <c r="L68" t="s">
+        <v>220</v>
+      </c>
+      <c r="M68" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>6</v>
+      </c>
+      <c r="B69" t="s">
+        <v>8</v>
+      </c>
+      <c r="C69" t="s">
+        <v>307</v>
+      </c>
+      <c r="E69">
+        <v>2660</v>
+      </c>
+      <c r="F69" t="s">
+        <v>22</v>
+      </c>
+      <c r="G69" t="s">
+        <v>255</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I69" t="b">
+        <v>1</v>
+      </c>
+      <c r="J69" t="s">
+        <v>163</v>
+      </c>
+      <c r="K69">
+        <v>2280</v>
+      </c>
+      <c r="L69" t="s">
+        <v>220</v>
+      </c>
+      <c r="M69" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>6</v>
+      </c>
+      <c r="B70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C70" t="s">
+        <v>308</v>
+      </c>
+      <c r="E70">
+        <v>4681</v>
+      </c>
+      <c r="F70" t="s">
+        <v>22</v>
+      </c>
+      <c r="G70" t="s">
+        <v>255</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I70" t="b">
+        <v>1</v>
+      </c>
+      <c r="J70" t="s">
+        <v>163</v>
+      </c>
+      <c r="K70">
+        <v>1800</v>
+      </c>
+      <c r="L70" t="s">
+        <v>220</v>
+      </c>
+      <c r="M70" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>6</v>
+      </c>
+      <c r="B71" t="s">
+        <v>8</v>
+      </c>
+      <c r="C71" t="s">
+        <v>309</v>
+      </c>
+      <c r="E71">
+        <v>5350</v>
+      </c>
+      <c r="F71" t="s">
+        <v>22</v>
+      </c>
+      <c r="G71" t="s">
+        <v>255</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I71" t="b">
+        <v>1</v>
+      </c>
+      <c r="J71" t="s">
+        <v>163</v>
+      </c>
+      <c r="K71">
+        <v>1800</v>
+      </c>
+      <c r="L71" t="s">
+        <v>220</v>
+      </c>
+      <c r="M71" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>6</v>
+      </c>
+      <c r="B72" t="s">
+        <v>8</v>
+      </c>
+      <c r="C72" t="s">
+        <v>310</v>
+      </c>
+      <c r="E72">
+        <v>3500</v>
+      </c>
+      <c r="F72" t="s">
+        <v>22</v>
+      </c>
+      <c r="G72" t="s">
+        <v>255</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I72" t="b">
+        <v>1</v>
+      </c>
+      <c r="J72" t="s">
+        <v>163</v>
+      </c>
+      <c r="K72">
+        <v>1800</v>
+      </c>
+      <c r="L72" t="s">
+        <v>220</v>
+      </c>
+      <c r="M72" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>6</v>
+      </c>
+      <c r="B73" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73" t="s">
+        <v>311</v>
+      </c>
+      <c r="E73">
+        <v>2600</v>
+      </c>
+      <c r="F73" t="s">
+        <v>22</v>
+      </c>
+      <c r="G73" t="s">
+        <v>255</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I73" t="b">
+        <v>1</v>
+      </c>
+      <c r="J73" t="s">
+        <v>163</v>
+      </c>
+      <c r="K73">
+        <v>2400</v>
+      </c>
+      <c r="L73" t="s">
+        <v>220</v>
+      </c>
+      <c r="M73" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>6</v>
+      </c>
+      <c r="B74" t="s">
+        <v>8</v>
+      </c>
+      <c r="C74" t="s">
+        <v>312</v>
+      </c>
+      <c r="E74">
+        <v>9150</v>
+      </c>
+      <c r="F74" t="s">
+        <v>22</v>
+      </c>
+      <c r="G74" t="s">
+        <v>255</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I74" t="b">
+        <v>1</v>
+      </c>
+      <c r="J74" t="s">
+        <v>163</v>
+      </c>
+      <c r="K74">
+        <v>1800</v>
+      </c>
+      <c r="L74" t="s">
+        <v>220</v>
+      </c>
+      <c r="M74" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>6</v>
+      </c>
+      <c r="B75" t="s">
+        <v>8</v>
+      </c>
+      <c r="C75" t="s">
+        <v>313</v>
+      </c>
+      <c r="E75">
+        <v>1800</v>
+      </c>
+      <c r="F75" t="s">
+        <v>22</v>
+      </c>
+      <c r="G75" t="s">
+        <v>255</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I75" t="b">
+        <v>1</v>
+      </c>
+      <c r="J75" t="s">
+        <v>163</v>
+      </c>
+      <c r="K75">
+        <v>2400</v>
+      </c>
+      <c r="L75" t="s">
+        <v>220</v>
+      </c>
+      <c r="M75" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>6</v>
+      </c>
+      <c r="B76" t="s">
+        <v>8</v>
+      </c>
+      <c r="C76" t="s">
+        <v>314</v>
+      </c>
+      <c r="E76">
+        <v>1348</v>
+      </c>
+      <c r="F76" t="s">
+        <v>22</v>
+      </c>
+      <c r="G76" t="s">
+        <v>255</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I76" t="b">
+        <v>1</v>
+      </c>
+      <c r="J76" t="s">
+        <v>163</v>
+      </c>
+      <c r="K76">
+        <v>1800</v>
+      </c>
+      <c r="L76" t="s">
+        <v>220</v>
+      </c>
+      <c r="M76" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>6</v>
+      </c>
+      <c r="B77" t="s">
+        <v>8</v>
+      </c>
+      <c r="C77" t="s">
+        <v>315</v>
+      </c>
+      <c r="E77">
+        <v>7130</v>
+      </c>
+      <c r="F77" t="s">
+        <v>22</v>
+      </c>
+      <c r="G77" t="s">
+        <v>255</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I77" t="b">
+        <v>1</v>
+      </c>
+      <c r="J77" t="s">
+        <v>163</v>
+      </c>
+      <c r="K77">
+        <v>1800</v>
+      </c>
+      <c r="L77" t="s">
+        <v>220</v>
+      </c>
+      <c r="M77" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>6</v>
+      </c>
+      <c r="B78" t="s">
+        <v>8</v>
+      </c>
+      <c r="C78" t="s">
+        <v>316</v>
+      </c>
+      <c r="E78">
+        <v>1020</v>
+      </c>
+      <c r="F78" t="s">
+        <v>22</v>
+      </c>
+      <c r="G78" t="s">
+        <v>255</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I78" t="b">
+        <v>1</v>
+      </c>
+      <c r="J78" t="s">
+        <v>163</v>
+      </c>
+      <c r="K78">
+        <v>1800</v>
+      </c>
+      <c r="L78" t="s">
+        <v>220</v>
+      </c>
+      <c r="M78" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>6</v>
+      </c>
+      <c r="B79" t="s">
+        <v>8</v>
+      </c>
+      <c r="C79" t="s">
+        <v>317</v>
+      </c>
+      <c r="E79">
+        <v>7100</v>
+      </c>
+      <c r="F79" t="s">
+        <v>22</v>
+      </c>
+      <c r="G79" t="s">
+        <v>255</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I79" t="b">
+        <v>1</v>
+      </c>
+      <c r="J79" t="s">
+        <v>163</v>
+      </c>
+      <c r="K79">
+        <v>1800</v>
+      </c>
+      <c r="L79" t="s">
+        <v>220</v>
+      </c>
+      <c r="M79" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>6</v>
+      </c>
+      <c r="B80" t="s">
+        <v>8</v>
+      </c>
+      <c r="C80" t="s">
+        <v>318</v>
+      </c>
+      <c r="E80">
+        <v>2845</v>
+      </c>
+      <c r="F80" t="s">
+        <v>22</v>
+      </c>
+      <c r="G80" t="s">
+        <v>255</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I80" t="b">
+        <v>1</v>
+      </c>
+      <c r="J80" t="s">
+        <v>163</v>
+      </c>
+      <c r="K80">
+        <v>1800</v>
+      </c>
+      <c r="L80" t="s">
+        <v>220</v>
+      </c>
+      <c r="M80" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>6</v>
+      </c>
+      <c r="B81" t="s">
+        <v>8</v>
+      </c>
+      <c r="C81" t="s">
+        <v>319</v>
+      </c>
+      <c r="E81">
+        <v>5523</v>
+      </c>
+      <c r="F81" t="s">
+        <v>22</v>
+      </c>
+      <c r="G81" t="s">
+        <v>255</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I81" t="b">
+        <v>1</v>
+      </c>
+      <c r="J81" t="s">
+        <v>163</v>
+      </c>
+      <c r="K81">
+        <v>3000</v>
+      </c>
+      <c r="L81" t="s">
+        <v>220</v>
+      </c>
+      <c r="M81" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>6</v>
+      </c>
+      <c r="B82" t="s">
+        <v>8</v>
+      </c>
+      <c r="E82">
+        <v>9700</v>
+      </c>
+      <c r="F82" t="s">
+        <v>22</v>
+      </c>
+      <c r="G82" t="s">
+        <v>255</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I82" t="b">
+        <v>1</v>
+      </c>
+      <c r="J82" t="s">
+        <v>163</v>
+      </c>
+      <c r="K82">
+        <v>1800</v>
+      </c>
+      <c r="L82" t="s">
+        <v>220</v>
+      </c>
+      <c r="M82" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>6</v>
+      </c>
+      <c r="B83" t="s">
+        <v>8</v>
+      </c>
+      <c r="E83">
+        <v>2000</v>
+      </c>
+      <c r="F83" t="s">
+        <v>22</v>
+      </c>
+      <c r="G83" t="s">
+        <v>255</v>
+      </c>
+      <c r="H83" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I83" t="b">
+        <v>1</v>
+      </c>
+      <c r="J83" t="s">
+        <v>163</v>
+      </c>
+      <c r="K83">
+        <v>1800</v>
+      </c>
+      <c r="L83" t="s">
+        <v>220</v>
+      </c>
+      <c r="M83" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>6</v>
+      </c>
+      <c r="B84" t="s">
+        <v>8</v>
+      </c>
+      <c r="E84">
+        <v>2870</v>
+      </c>
+      <c r="F84" t="s">
+        <v>22</v>
+      </c>
+      <c r="G84" t="s">
+        <v>255</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I84" t="b">
+        <v>1</v>
+      </c>
+      <c r="J84" t="s">
+        <v>163</v>
+      </c>
+      <c r="K84">
+        <v>3000</v>
+      </c>
+      <c r="L84" t="s">
+        <v>220</v>
+      </c>
+      <c r="M84" t="s">
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -1779,10 +5010,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="55.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="62.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="4" max="4" width="55.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="62.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1819,10 +5050,10 @@
         <v>228</v>
       </c>
       <c r="E2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -1834,66 +5065,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C1" t="s">
         <v>235</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>236</v>
       </c>
-      <c r="D1" t="s">
-        <v>237</v>
-      </c>
       <c r="E1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F1" t="s">
+        <v>242</v>
+      </c>
+      <c r="G1" t="s">
         <v>243</v>
       </c>
-      <c r="G1" t="s">
-        <v>244</v>
-      </c>
       <c r="H1" t="s">
+        <v>246</v>
+      </c>
+      <c r="I1" t="s">
         <v>247</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>248</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>249</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>250</v>
       </c>
-      <c r="L1" t="s">
-        <v>251</v>
-      </c>
       <c r="M1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B2">
         <v>7</v>
@@ -1905,13 +5136,13 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F2" t="s">
+        <v>244</v>
+      </c>
+      <c r="G2" t="s">
         <v>245</v>
-      </c>
-      <c r="G2" t="s">
-        <v>246</v>
       </c>
       <c r="H2" t="s">
         <v>6</v>
@@ -1926,10 +5157,10 @@
         <v>102</v>
       </c>
       <c r="L2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="M2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -1947,24 +5178,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -2089,9 +5320,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="96.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="1" max="1" width="96" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2118,13 +5349,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>237</v>
+      </c>
+      <c r="B3" t="s">
         <v>238</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>239</v>
-      </c>
-      <c r="C3" t="s">
-        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -2141,8 +5372,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2203,13 +5434,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="2" max="4" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="1" max="1" width="23" customWidth="1" collapsed="1"/>
+    <col min="2" max="4" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="34.42578125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="30.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -2905,10 +6136,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="35.140625" collapsed="true"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="35.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -3026,17 +6257,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="29.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="60.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="25.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="27.85546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="60.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="25.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="27.85546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="26.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -3844,15 +7075,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -3871,6 +7102,11 @@
         <v>183</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>320</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated few more datas
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
+++ b/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11580" windowHeight="4650" firstSheet="10" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11580" windowHeight="4650" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="User_Details" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="316">
   <si>
     <t>UserName</t>
   </si>
@@ -530,9 +530,6 @@
     <t>Installation</t>
   </si>
   <si>
-    <t>01m3B0000004DHPQA2</t>
-  </si>
-  <si>
     <t>govendhan@svmx-cct5.org.cct5part1</t>
   </si>
   <si>
@@ -554,9 +551,6 @@
     <t>Mandt Account</t>
   </si>
   <si>
-    <t>a1y3B000000HhjjQAC</t>
-  </si>
-  <si>
     <t>SVMXC__Company__c</t>
   </si>
   <si>
@@ -587,84 +581,6 @@
     <t>SVMXC__Skill__c</t>
   </si>
   <si>
-    <t>a2N3B000000GzViUAK</t>
-  </si>
-  <si>
-    <t>0013B00000I4z82QAB</t>
-  </si>
-  <si>
-    <t>a2N3B000000GzW7UAK</t>
-  </si>
-  <si>
-    <t>a1y3B000000HhmyQAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4u3QAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4u4QAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4u5QAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4u6QAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4u7QAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4u8QAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4u9QAC</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4uAQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4uBQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4uCQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4uDQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4uEQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4uFQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4uGQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4uHQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4uIQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4uJQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4uKQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4uLQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M4uMQAS</t>
-  </si>
-  <si>
-    <t>a2D3B000002LX9AUAW</t>
-  </si>
-  <si>
-    <t>a2D3B000002LX9BUAW</t>
-  </si>
-  <si>
     <t>a1x3B0000002sRqQAI</t>
   </si>
   <si>
@@ -806,12 +722,6 @@
     <t>AutomationTerritory_Tue Oct 24 2017 17:01:45 GMT+0530 (IST)</t>
   </si>
   <si>
-    <t>a2N3B000000H0MHUA0</t>
-  </si>
-  <si>
-    <t>0013B00000I5bpsQAB</t>
-  </si>
-  <si>
     <t>Rue Du Bailli 82</t>
   </si>
   <si>
@@ -875,9 +785,6 @@
     <t>Rue Neuvice 5</t>
   </si>
   <si>
-    <t>0013B00000I5bptQAB</t>
-  </si>
-  <si>
     <t>Kruisstraat 162</t>
   </si>
   <si>
@@ -1002,6 +909,84 @@
   </si>
   <si>
     <t>John - Automation</t>
+  </si>
+  <si>
+    <t>a2D3B000002LXJhUAO</t>
+  </si>
+  <si>
+    <t>a2D3B000002LXJiUAO</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5bHQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5bIQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5bJQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5bKQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5bLQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5bMQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5bNQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5bOQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5bPQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5bQQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5bRQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5bSQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5bTQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5bUQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5bVQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5bWQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5bXQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5bYQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5bZQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5baQAC</t>
+  </si>
+  <si>
+    <t>a2N3B000000H0oYUAS</t>
+  </si>
+  <si>
+    <t>a1y3B000000HhtBQAS</t>
+  </si>
+  <si>
+    <t>0013B00000I5jyhQAB</t>
+  </si>
+  <si>
+    <t>0013B00000I5jyiQAB</t>
   </si>
 </sst>
 </file>
@@ -1412,10 +1397,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>164</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>165</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -1457,7 +1442,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -1466,12 +1451,12 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>206</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -1480,7 +1465,7 @@
         <v>162</v>
       </c>
       <c r="D3" t="s">
-        <v>207</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -1509,7 +1494,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1535,13 +1520,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1" t="s">
         <v>172</v>
-      </c>
-      <c r="B1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C1" t="s">
-        <v>174</v>
       </c>
       <c r="D1" t="s">
         <v>84</v>
@@ -1549,86 +1534,86 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>183</v>
+        <v>314</v>
       </c>
       <c r="B2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" t="s">
         <v>186</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D2" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>183</v>
+        <v>315</v>
       </c>
       <c r="B3" t="s">
+        <v>293</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D3" t="s">
         <v>187</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D3" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>315</v>
       </c>
       <c r="B4" t="s">
+        <v>294</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D4" t="s">
         <v>188</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D4" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>183</v>
+        <v>315</v>
       </c>
       <c r="B5" t="s">
+        <v>295</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D5" t="s">
         <v>189</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D5" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>183</v>
+        <v>315</v>
       </c>
       <c r="B6" t="s">
+        <v>296</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D6" t="s">
         <v>190</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D6" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>183</v>
+        <v>314</v>
       </c>
       <c r="B7" t="s">
+        <v>297</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D7" t="s">
         <v>191</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D7" t="s">
-        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -1642,135 +1627,135 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="B1" t="s">
-        <v>173</v>
+        <v>95</v>
       </c>
       <c r="C1" t="s">
-        <v>95</v>
+        <v>179</v>
       </c>
       <c r="D1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E1" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D2">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>186</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>293</v>
+      </c>
+      <c r="B3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C3" t="s">
+        <v>290</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C4" t="s">
+        <v>290</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>295</v>
+      </c>
+      <c r="B5" t="s">
+        <v>313</v>
+      </c>
+      <c r="C5" t="s">
+        <v>291</v>
+      </c>
+      <c r="D5">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>296</v>
+      </c>
+      <c r="B6" t="s">
+        <v>313</v>
+      </c>
+      <c r="C6" t="s">
+        <v>291</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>297</v>
+      </c>
+      <c r="B7" t="s">
+        <v>313</v>
+      </c>
+      <c r="C7" t="s">
+        <v>291</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
         <v>185</v>
-      </c>
-      <c r="D2" t="s">
-        <v>206</v>
-      </c>
-      <c r="E2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>187</v>
-      </c>
-      <c r="C3" t="s">
-        <v>185</v>
-      </c>
-      <c r="D3" t="s">
-        <v>206</v>
-      </c>
-      <c r="E3" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>188</v>
-      </c>
-      <c r="C4" t="s">
-        <v>185</v>
-      </c>
-      <c r="D4" t="s">
-        <v>206</v>
-      </c>
-      <c r="E4" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>189</v>
-      </c>
-      <c r="C5" t="s">
-        <v>185</v>
-      </c>
-      <c r="D5" t="s">
-        <v>207</v>
-      </c>
-      <c r="E5" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>190</v>
-      </c>
-      <c r="C6" t="s">
-        <v>185</v>
-      </c>
-      <c r="D6" t="s">
-        <v>207</v>
-      </c>
-      <c r="E6" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>191</v>
-      </c>
-      <c r="C7" t="s">
-        <v>185</v>
-      </c>
-      <c r="D7" t="s">
-        <v>207</v>
-      </c>
-      <c r="E7" t="s">
-        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -1782,7 +1767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -1840,7 +1825,7 @@
         <v>10</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -1863,7 +1848,7 @@
         <v>22</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>21</v>
@@ -1872,16 +1857,16 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K2">
         <v>2400</v>
       </c>
       <c r="L2" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M2" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1904,7 +1889,7 @@
         <v>22</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>21</v>
@@ -1913,16 +1898,16 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K3">
         <v>3000</v>
       </c>
       <c r="L3" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M3" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1945,7 +1930,7 @@
         <v>22</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>21</v>
@@ -1954,16 +1939,16 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K4">
         <v>3000</v>
       </c>
       <c r="L4" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M4" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1983,7 +1968,7 @@
         <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>21</v>
@@ -1992,16 +1977,16 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K5">
         <v>1800</v>
       </c>
       <c r="L5" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M5" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2021,7 +2006,7 @@
         <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>21</v>
@@ -2030,16 +2015,16 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K6">
         <v>1800</v>
       </c>
       <c r="L6" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M6" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -2059,7 +2044,7 @@
         <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>21</v>
@@ -2068,16 +2053,16 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K7">
         <v>1800</v>
       </c>
       <c r="L7" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M7" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -2097,7 +2082,7 @@
         <v>22</v>
       </c>
       <c r="G8" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>21</v>
@@ -2106,16 +2091,16 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K8">
         <v>3000</v>
       </c>
       <c r="L8" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M8" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -2135,7 +2120,7 @@
         <v>22</v>
       </c>
       <c r="G9" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>21</v>
@@ -2144,16 +2129,16 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K9">
         <v>2400</v>
       </c>
       <c r="L9" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M9" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -2173,7 +2158,7 @@
         <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>21</v>
@@ -2182,16 +2167,16 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K10">
         <v>2400</v>
       </c>
       <c r="L10" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M10" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -2211,7 +2196,7 @@
         <v>22</v>
       </c>
       <c r="G11" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>21</v>
@@ -2220,16 +2205,16 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K11">
         <v>2400</v>
       </c>
       <c r="L11" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M11" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -2249,7 +2234,7 @@
         <v>22</v>
       </c>
       <c r="G12" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>21</v>
@@ -2258,16 +2243,16 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K12">
         <v>1800</v>
       </c>
       <c r="L12" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M12" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -2287,7 +2272,7 @@
         <v>22</v>
       </c>
       <c r="G13" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>21</v>
@@ -2296,16 +2281,16 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K13">
         <v>2400</v>
       </c>
       <c r="L13" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M13" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -2325,7 +2310,7 @@
         <v>22</v>
       </c>
       <c r="G14" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>21</v>
@@ -2334,16 +2319,16 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K14">
         <v>2400</v>
       </c>
       <c r="L14" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M14" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -2363,7 +2348,7 @@
         <v>22</v>
       </c>
       <c r="G15" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>21</v>
@@ -2372,16 +2357,16 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K15">
         <v>2400</v>
       </c>
       <c r="L15" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M15" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -2401,7 +2386,7 @@
         <v>22</v>
       </c>
       <c r="G16" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>21</v>
@@ -2410,16 +2395,16 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K16">
         <v>2400</v>
       </c>
       <c r="L16" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M16" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -2439,7 +2424,7 @@
         <v>22</v>
       </c>
       <c r="G17" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>21</v>
@@ -2448,16 +2433,16 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K17">
         <v>1800</v>
       </c>
       <c r="L17" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M17" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -2477,7 +2462,7 @@
         <v>22</v>
       </c>
       <c r="G18" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>21</v>
@@ -2486,16 +2471,16 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K18">
         <v>3000</v>
       </c>
       <c r="L18" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M18" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -2515,7 +2500,7 @@
         <v>22</v>
       </c>
       <c r="G19" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>21</v>
@@ -2524,16 +2509,16 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K19">
         <v>2400</v>
       </c>
       <c r="L19" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M19" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -2544,7 +2529,7 @@
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>257</v>
+        <v>227</v>
       </c>
       <c r="E20">
         <v>4400</v>
@@ -2553,7 +2538,7 @@
         <v>22</v>
       </c>
       <c r="G20" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>21</v>
@@ -2562,16 +2547,16 @@
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K20">
         <v>2400</v>
       </c>
       <c r="L20" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M20" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -2582,7 +2567,7 @@
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>258</v>
+        <v>228</v>
       </c>
       <c r="E21">
         <v>9250</v>
@@ -2591,7 +2576,7 @@
         <v>22</v>
       </c>
       <c r="G21" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>21</v>
@@ -2600,16 +2585,16 @@
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K21">
         <v>2400</v>
       </c>
       <c r="L21" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M21" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -2620,7 +2605,7 @@
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>259</v>
+        <v>229</v>
       </c>
       <c r="E22">
         <v>2610</v>
@@ -2629,7 +2614,7 @@
         <v>22</v>
       </c>
       <c r="G22" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>21</v>
@@ -2638,16 +2623,16 @@
         <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K22">
         <v>2400</v>
       </c>
       <c r="L22" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M22" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -2658,7 +2643,7 @@
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>260</v>
+        <v>230</v>
       </c>
       <c r="E23">
         <v>1050</v>
@@ -2667,7 +2652,7 @@
         <v>22</v>
       </c>
       <c r="G23" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>21</v>
@@ -2676,16 +2661,16 @@
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K23">
         <v>1800</v>
       </c>
       <c r="L23" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M23" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -2696,7 +2681,7 @@
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>261</v>
+        <v>231</v>
       </c>
       <c r="E24">
         <v>1200</v>
@@ -2705,7 +2690,7 @@
         <v>22</v>
       </c>
       <c r="G24" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>21</v>
@@ -2714,16 +2699,16 @@
         <v>1</v>
       </c>
       <c r="J24" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K24">
         <v>3000</v>
       </c>
       <c r="L24" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M24" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -2734,7 +2719,7 @@
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>262</v>
+        <v>232</v>
       </c>
       <c r="E25">
         <v>3300</v>
@@ -2743,7 +2728,7 @@
         <v>22</v>
       </c>
       <c r="G25" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>21</v>
@@ -2752,16 +2737,16 @@
         <v>1</v>
       </c>
       <c r="J25" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K25">
         <v>3000</v>
       </c>
       <c r="L25" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M25" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -2772,7 +2757,7 @@
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>263</v>
+        <v>233</v>
       </c>
       <c r="E26">
         <v>9000</v>
@@ -2781,7 +2766,7 @@
         <v>22</v>
       </c>
       <c r="G26" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>21</v>
@@ -2790,16 +2775,16 @@
         <v>1</v>
       </c>
       <c r="J26" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K26">
         <v>3000</v>
       </c>
       <c r="L26" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M26" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -2810,7 +2795,7 @@
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>264</v>
+        <v>234</v>
       </c>
       <c r="E27">
         <v>9140</v>
@@ -2819,7 +2804,7 @@
         <v>22</v>
       </c>
       <c r="G27" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>21</v>
@@ -2828,16 +2813,16 @@
         <v>1</v>
       </c>
       <c r="J27" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K27">
         <v>2400</v>
       </c>
       <c r="L27" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M27" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -2848,7 +2833,7 @@
         <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>265</v>
+        <v>235</v>
       </c>
       <c r="E28">
         <v>9340</v>
@@ -2857,7 +2842,7 @@
         <v>22</v>
       </c>
       <c r="G28" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>21</v>
@@ -2866,16 +2851,16 @@
         <v>1</v>
       </c>
       <c r="J28" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K28">
         <v>2400</v>
       </c>
       <c r="L28" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M28" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -2886,7 +2871,7 @@
         <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>266</v>
+        <v>236</v>
       </c>
       <c r="E29">
         <v>8540</v>
@@ -2895,7 +2880,7 @@
         <v>22</v>
       </c>
       <c r="G29" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>21</v>
@@ -2904,16 +2889,16 @@
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K29">
         <v>1800</v>
       </c>
       <c r="L29" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M29" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -2924,7 +2909,7 @@
         <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>267</v>
+        <v>237</v>
       </c>
       <c r="E30">
         <v>8620</v>
@@ -2933,7 +2918,7 @@
         <v>22</v>
       </c>
       <c r="G30" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>21</v>
@@ -2942,16 +2927,16 @@
         <v>1</v>
       </c>
       <c r="J30" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K30">
         <v>3000</v>
       </c>
       <c r="L30" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M30" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -2962,7 +2947,7 @@
         <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>268</v>
+        <v>238</v>
       </c>
       <c r="E31">
         <v>8430</v>
@@ -2971,7 +2956,7 @@
         <v>22</v>
       </c>
       <c r="G31" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>21</v>
@@ -2980,16 +2965,16 @@
         <v>1</v>
       </c>
       <c r="J31" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K31">
         <v>1800</v>
       </c>
       <c r="L31" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M31" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -3000,7 +2985,7 @@
         <v>8</v>
       </c>
       <c r="C32" t="s">
-        <v>269</v>
+        <v>239</v>
       </c>
       <c r="E32">
         <v>2920</v>
@@ -3009,7 +2994,7 @@
         <v>22</v>
       </c>
       <c r="G32" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>21</v>
@@ -3018,16 +3003,16 @@
         <v>1</v>
       </c>
       <c r="J32" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K32">
         <v>1800</v>
       </c>
       <c r="L32" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M32" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -3038,7 +3023,7 @@
         <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>270</v>
+        <v>240</v>
       </c>
       <c r="E33">
         <v>5500</v>
@@ -3047,7 +3032,7 @@
         <v>22</v>
       </c>
       <c r="G33" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>21</v>
@@ -3056,16 +3041,16 @@
         <v>1</v>
       </c>
       <c r="J33" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K33">
         <v>3000</v>
       </c>
       <c r="L33" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M33" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -3076,7 +3061,7 @@
         <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>271</v>
+        <v>241</v>
       </c>
       <c r="E34">
         <v>2000</v>
@@ -3085,7 +3070,7 @@
         <v>22</v>
       </c>
       <c r="G34" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>21</v>
@@ -3094,16 +3079,16 @@
         <v>1</v>
       </c>
       <c r="J34" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K34">
         <v>2400</v>
       </c>
       <c r="L34" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M34" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -3114,7 +3099,7 @@
         <v>8</v>
       </c>
       <c r="C35" t="s">
-        <v>272</v>
+        <v>242</v>
       </c>
       <c r="E35">
         <v>1348</v>
@@ -3123,7 +3108,7 @@
         <v>22</v>
       </c>
       <c r="G35" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>21</v>
@@ -3132,16 +3117,16 @@
         <v>1</v>
       </c>
       <c r="J35" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K35">
         <v>3000</v>
       </c>
       <c r="L35" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M35" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -3152,7 +3137,7 @@
         <v>8</v>
       </c>
       <c r="C36" t="s">
-        <v>273</v>
+        <v>243</v>
       </c>
       <c r="E36">
         <v>8400</v>
@@ -3161,7 +3146,7 @@
         <v>22</v>
       </c>
       <c r="G36" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>21</v>
@@ -3170,16 +3155,16 @@
         <v>1</v>
       </c>
       <c r="J36" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K36">
         <v>2400</v>
       </c>
       <c r="L36" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M36" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -3190,7 +3175,7 @@
         <v>8</v>
       </c>
       <c r="C37" t="s">
-        <v>274</v>
+        <v>244</v>
       </c>
       <c r="E37">
         <v>1348</v>
@@ -3199,7 +3184,7 @@
         <v>22</v>
       </c>
       <c r="G37" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>21</v>
@@ -3208,16 +3193,16 @@
         <v>1</v>
       </c>
       <c r="J37" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K37">
         <v>2400</v>
       </c>
       <c r="L37" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M37" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -3228,7 +3213,7 @@
         <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>275</v>
+        <v>245</v>
       </c>
       <c r="E38">
         <v>7130</v>
@@ -3237,7 +3222,7 @@
         <v>22</v>
       </c>
       <c r="G38" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>21</v>
@@ -3246,16 +3231,16 @@
         <v>1</v>
       </c>
       <c r="J38" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K38">
         <v>2400</v>
       </c>
       <c r="L38" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M38" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -3266,7 +3251,7 @@
         <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>276</v>
+        <v>246</v>
       </c>
       <c r="E39">
         <v>1140</v>
@@ -3275,7 +3260,7 @@
         <v>22</v>
       </c>
       <c r="G39" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>21</v>
@@ -3284,16 +3269,16 @@
         <v>1</v>
       </c>
       <c r="J39" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K39">
         <v>3000</v>
       </c>
       <c r="L39" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M39" t="s">
-        <v>256</v>
+        <v>314</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -3304,7 +3289,7 @@
         <v>8</v>
       </c>
       <c r="C40" t="s">
-        <v>277</v>
+        <v>247</v>
       </c>
       <c r="E40">
         <v>2840</v>
@@ -3313,7 +3298,7 @@
         <v>22</v>
       </c>
       <c r="G40" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>21</v>
@@ -3322,16 +3307,16 @@
         <v>1</v>
       </c>
       <c r="J40" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K40">
         <v>3000</v>
       </c>
       <c r="L40" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M40" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -3342,7 +3327,7 @@
         <v>8</v>
       </c>
       <c r="C41" t="s">
-        <v>279</v>
+        <v>248</v>
       </c>
       <c r="E41">
         <v>1348</v>
@@ -3351,7 +3336,7 @@
         <v>22</v>
       </c>
       <c r="G41" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>21</v>
@@ -3360,16 +3345,16 @@
         <v>1</v>
       </c>
       <c r="J41" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K41">
         <v>3000</v>
       </c>
       <c r="L41" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M41" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
@@ -3380,7 +3365,7 @@
         <v>8</v>
       </c>
       <c r="C42" t="s">
-        <v>280</v>
+        <v>249</v>
       </c>
       <c r="E42">
         <v>2550</v>
@@ -3389,7 +3374,7 @@
         <v>22</v>
       </c>
       <c r="G42" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>21</v>
@@ -3398,16 +3383,16 @@
         <v>1</v>
       </c>
       <c r="J42" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K42">
         <v>1800</v>
       </c>
       <c r="L42" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M42" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -3418,7 +3403,7 @@
         <v>8</v>
       </c>
       <c r="C43" t="s">
-        <v>281</v>
+        <v>250</v>
       </c>
       <c r="E43">
         <v>4000</v>
@@ -3427,7 +3412,7 @@
         <v>22</v>
       </c>
       <c r="G43" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>21</v>
@@ -3436,16 +3421,16 @@
         <v>1</v>
       </c>
       <c r="J43" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K43">
         <v>1800</v>
       </c>
       <c r="L43" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M43" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -3456,7 +3441,7 @@
         <v>8</v>
       </c>
       <c r="C44" t="s">
-        <v>282</v>
+        <v>251</v>
       </c>
       <c r="E44">
         <v>2570</v>
@@ -3465,7 +3450,7 @@
         <v>22</v>
       </c>
       <c r="G44" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>21</v>
@@ -3474,16 +3459,16 @@
         <v>1</v>
       </c>
       <c r="J44" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K44">
         <v>2400</v>
       </c>
       <c r="L44" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M44" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
@@ -3494,7 +3479,7 @@
         <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>283</v>
+        <v>252</v>
       </c>
       <c r="E45">
         <v>1082</v>
@@ -3503,7 +3488,7 @@
         <v>22</v>
       </c>
       <c r="G45" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>21</v>
@@ -3512,16 +3497,16 @@
         <v>1</v>
       </c>
       <c r="J45" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K45">
         <v>2280</v>
       </c>
       <c r="L45" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M45" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
@@ -3532,7 +3517,7 @@
         <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>284</v>
+        <v>253</v>
       </c>
       <c r="E46">
         <v>2800</v>
@@ -3541,7 +3526,7 @@
         <v>22</v>
       </c>
       <c r="G46" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>21</v>
@@ -3550,16 +3535,16 @@
         <v>1</v>
       </c>
       <c r="J46" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K46">
         <v>2400</v>
       </c>
       <c r="L46" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M46" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -3570,7 +3555,7 @@
         <v>8</v>
       </c>
       <c r="C47" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="E47">
         <v>5300</v>
@@ -3579,7 +3564,7 @@
         <v>22</v>
       </c>
       <c r="G47" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H47" s="2" t="s">
         <v>21</v>
@@ -3588,16 +3573,16 @@
         <v>1</v>
       </c>
       <c r="J47" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K47">
         <v>2400</v>
       </c>
       <c r="L47" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M47" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
@@ -3608,7 +3593,7 @@
         <v>8</v>
       </c>
       <c r="C48" t="s">
-        <v>286</v>
+        <v>255</v>
       </c>
       <c r="E48">
         <v>3500</v>
@@ -3617,7 +3602,7 @@
         <v>22</v>
       </c>
       <c r="G48" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H48" s="2" t="s">
         <v>21</v>
@@ -3626,16 +3611,16 @@
         <v>1</v>
       </c>
       <c r="J48" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K48">
         <v>2400</v>
       </c>
       <c r="L48" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M48" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
@@ -3646,7 +3631,7 @@
         <v>8</v>
       </c>
       <c r="C49" t="s">
-        <v>287</v>
+        <v>256</v>
       </c>
       <c r="E49">
         <v>5380</v>
@@ -3655,7 +3640,7 @@
         <v>22</v>
       </c>
       <c r="G49" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H49" s="2" t="s">
         <v>21</v>
@@ -3664,16 +3649,16 @@
         <v>1</v>
       </c>
       <c r="J49" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K49">
         <v>1800</v>
       </c>
       <c r="L49" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M49" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
@@ -3684,7 +3669,7 @@
         <v>8</v>
       </c>
       <c r="C50" t="s">
-        <v>288</v>
+        <v>257</v>
       </c>
       <c r="E50">
         <v>2570</v>
@@ -3693,7 +3678,7 @@
         <v>22</v>
       </c>
       <c r="G50" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H50" s="2" t="s">
         <v>21</v>
@@ -3702,16 +3687,16 @@
         <v>1</v>
       </c>
       <c r="J50" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K50">
         <v>1800</v>
       </c>
       <c r="L50" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M50" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
@@ -3722,7 +3707,7 @@
         <v>8</v>
       </c>
       <c r="C51" t="s">
-        <v>289</v>
+        <v>258</v>
       </c>
       <c r="E51">
         <v>1982</v>
@@ -3731,7 +3716,7 @@
         <v>22</v>
       </c>
       <c r="G51" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H51" s="2" t="s">
         <v>21</v>
@@ -3740,16 +3725,16 @@
         <v>1</v>
       </c>
       <c r="J51" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K51">
         <v>1800</v>
       </c>
       <c r="L51" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M51" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
@@ -3760,7 +3745,7 @@
         <v>8</v>
       </c>
       <c r="C52" t="s">
-        <v>290</v>
+        <v>259</v>
       </c>
       <c r="E52">
         <v>6800</v>
@@ -3769,7 +3754,7 @@
         <v>22</v>
       </c>
       <c r="G52" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H52" s="2" t="s">
         <v>21</v>
@@ -3778,16 +3763,16 @@
         <v>1</v>
       </c>
       <c r="J52" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K52">
         <v>2400</v>
       </c>
       <c r="L52" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M52" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
@@ -3798,7 +3783,7 @@
         <v>8</v>
       </c>
       <c r="C53" t="s">
-        <v>291</v>
+        <v>260</v>
       </c>
       <c r="E53">
         <v>8400</v>
@@ -3807,7 +3792,7 @@
         <v>22</v>
       </c>
       <c r="G53" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H53" s="2" t="s">
         <v>21</v>
@@ -3816,16 +3801,16 @@
         <v>1</v>
       </c>
       <c r="J53" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K53">
         <v>2400</v>
       </c>
       <c r="L53" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M53" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
@@ -3836,7 +3821,7 @@
         <v>8</v>
       </c>
       <c r="C54" t="s">
-        <v>292</v>
+        <v>261</v>
       </c>
       <c r="E54">
         <v>4500</v>
@@ -3845,7 +3830,7 @@
         <v>22</v>
       </c>
       <c r="G54" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H54" s="2" t="s">
         <v>21</v>
@@ -3854,16 +3839,16 @@
         <v>1</v>
       </c>
       <c r="J54" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K54">
         <v>3000</v>
       </c>
       <c r="L54" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M54" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
@@ -3874,7 +3859,7 @@
         <v>8</v>
       </c>
       <c r="C55" t="s">
-        <v>293</v>
+        <v>262</v>
       </c>
       <c r="E55">
         <v>1348</v>
@@ -3883,7 +3868,7 @@
         <v>22</v>
       </c>
       <c r="G55" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>21</v>
@@ -3892,16 +3877,16 @@
         <v>1</v>
       </c>
       <c r="J55" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K55">
         <v>4920</v>
       </c>
       <c r="L55" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M55" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
@@ -3912,7 +3897,7 @@
         <v>8</v>
       </c>
       <c r="C56" t="s">
-        <v>294</v>
+        <v>263</v>
       </c>
       <c r="E56">
         <v>7130</v>
@@ -3921,7 +3906,7 @@
         <v>22</v>
       </c>
       <c r="G56" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H56" s="2" t="s">
         <v>21</v>
@@ -3930,16 +3915,16 @@
         <v>1</v>
       </c>
       <c r="J56" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K56">
         <v>2400</v>
       </c>
       <c r="L56" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M56" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
@@ -3950,7 +3935,7 @@
         <v>8</v>
       </c>
       <c r="C57" t="s">
-        <v>295</v>
+        <v>264</v>
       </c>
       <c r="E57">
         <v>1348</v>
@@ -3959,7 +3944,7 @@
         <v>22</v>
       </c>
       <c r="G57" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H57" s="2" t="s">
         <v>21</v>
@@ -3968,16 +3953,16 @@
         <v>1</v>
       </c>
       <c r="J57" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K57">
         <v>2400</v>
       </c>
       <c r="L57" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M57" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -3988,7 +3973,7 @@
         <v>8</v>
       </c>
       <c r="C58" t="s">
-        <v>296</v>
+        <v>265</v>
       </c>
       <c r="E58">
         <v>3500</v>
@@ -3997,7 +3982,7 @@
         <v>22</v>
       </c>
       <c r="G58" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>21</v>
@@ -4006,16 +3991,16 @@
         <v>1</v>
       </c>
       <c r="J58" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K58">
         <v>2400</v>
       </c>
       <c r="L58" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M58" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
@@ -4026,7 +4011,7 @@
         <v>8</v>
       </c>
       <c r="C59" t="s">
-        <v>297</v>
+        <v>266</v>
       </c>
       <c r="E59">
         <v>2000</v>
@@ -4035,7 +4020,7 @@
         <v>22</v>
       </c>
       <c r="G59" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>21</v>
@@ -4044,16 +4029,16 @@
         <v>1</v>
       </c>
       <c r="J59" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K59">
         <v>2400</v>
       </c>
       <c r="L59" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M59" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
@@ -4064,7 +4049,7 @@
         <v>8</v>
       </c>
       <c r="C60" t="s">
-        <v>298</v>
+        <v>267</v>
       </c>
       <c r="E60">
         <v>8400</v>
@@ -4073,7 +4058,7 @@
         <v>22</v>
       </c>
       <c r="G60" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H60" s="2" t="s">
         <v>21</v>
@@ -4082,16 +4067,16 @@
         <v>1</v>
       </c>
       <c r="J60" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K60">
         <v>2280</v>
       </c>
       <c r="L60" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M60" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
@@ -4102,7 +4087,7 @@
         <v>8</v>
       </c>
       <c r="C61" t="s">
-        <v>299</v>
+        <v>268</v>
       </c>
       <c r="E61">
         <v>2060</v>
@@ -4111,7 +4096,7 @@
         <v>22</v>
       </c>
       <c r="G61" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H61" s="2" t="s">
         <v>21</v>
@@ -4120,16 +4105,16 @@
         <v>1</v>
       </c>
       <c r="J61" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K61">
         <v>1800</v>
       </c>
       <c r="L61" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M61" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
@@ -4140,7 +4125,7 @@
         <v>8</v>
       </c>
       <c r="C62" t="s">
-        <v>300</v>
+        <v>269</v>
       </c>
       <c r="E62">
         <v>2640</v>
@@ -4149,7 +4134,7 @@
         <v>22</v>
       </c>
       <c r="G62" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H62" s="2" t="s">
         <v>21</v>
@@ -4158,16 +4143,16 @@
         <v>1</v>
       </c>
       <c r="J62" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K62">
         <v>3360</v>
       </c>
       <c r="L62" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M62" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
@@ -4178,7 +4163,7 @@
         <v>8</v>
       </c>
       <c r="C63" t="s">
-        <v>301</v>
+        <v>270</v>
       </c>
       <c r="E63">
         <v>3511</v>
@@ -4187,7 +4172,7 @@
         <v>22</v>
       </c>
       <c r="G63" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H63" s="2" t="s">
         <v>21</v>
@@ -4196,16 +4181,16 @@
         <v>1</v>
       </c>
       <c r="J63" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K63">
         <v>2400</v>
       </c>
       <c r="L63" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M63" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
@@ -4216,7 +4201,7 @@
         <v>8</v>
       </c>
       <c r="C64" t="s">
-        <v>302</v>
+        <v>271</v>
       </c>
       <c r="E64">
         <v>8400</v>
@@ -4225,7 +4210,7 @@
         <v>22</v>
       </c>
       <c r="G64" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H64" s="2" t="s">
         <v>21</v>
@@ -4234,16 +4219,16 @@
         <v>1</v>
       </c>
       <c r="J64" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K64">
         <v>2400</v>
       </c>
       <c r="L64" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M64" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
@@ -4254,7 +4239,7 @@
         <v>8</v>
       </c>
       <c r="C65" t="s">
-        <v>303</v>
+        <v>272</v>
       </c>
       <c r="E65">
         <v>3511</v>
@@ -4263,7 +4248,7 @@
         <v>22</v>
       </c>
       <c r="G65" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H65" s="2" t="s">
         <v>21</v>
@@ -4272,16 +4257,16 @@
         <v>1</v>
       </c>
       <c r="J65" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K65">
         <v>2400</v>
       </c>
       <c r="L65" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M65" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
@@ -4292,7 +4277,7 @@
         <v>8</v>
       </c>
       <c r="C66" t="s">
-        <v>304</v>
+        <v>273</v>
       </c>
       <c r="E66">
         <v>1800</v>
@@ -4301,7 +4286,7 @@
         <v>22</v>
       </c>
       <c r="G66" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H66" s="2" t="s">
         <v>21</v>
@@ -4310,16 +4295,16 @@
         <v>1</v>
       </c>
       <c r="J66" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K66">
         <v>2400</v>
       </c>
       <c r="L66" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M66" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
@@ -4330,7 +4315,7 @@
         <v>8</v>
       </c>
       <c r="C67" t="s">
-        <v>305</v>
+        <v>274</v>
       </c>
       <c r="E67">
         <v>2500</v>
@@ -4339,7 +4324,7 @@
         <v>22</v>
       </c>
       <c r="G67" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H67" s="2" t="s">
         <v>21</v>
@@ -4348,16 +4333,16 @@
         <v>1</v>
       </c>
       <c r="J67" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K67">
         <v>1800</v>
       </c>
       <c r="L67" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M67" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
@@ -4368,7 +4353,7 @@
         <v>8</v>
       </c>
       <c r="C68" t="s">
-        <v>306</v>
+        <v>275</v>
       </c>
       <c r="E68">
         <v>2840</v>
@@ -4377,7 +4362,7 @@
         <v>22</v>
       </c>
       <c r="G68" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H68" s="2" t="s">
         <v>21</v>
@@ -4386,16 +4371,16 @@
         <v>1</v>
       </c>
       <c r="J68" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K68">
         <v>2400</v>
       </c>
       <c r="L68" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M68" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
@@ -4406,7 +4391,7 @@
         <v>8</v>
       </c>
       <c r="C69" t="s">
-        <v>307</v>
+        <v>276</v>
       </c>
       <c r="E69">
         <v>2660</v>
@@ -4415,7 +4400,7 @@
         <v>22</v>
       </c>
       <c r="G69" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H69" s="2" t="s">
         <v>21</v>
@@ -4424,16 +4409,16 @@
         <v>1</v>
       </c>
       <c r="J69" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K69">
         <v>2280</v>
       </c>
       <c r="L69" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M69" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
@@ -4444,7 +4429,7 @@
         <v>8</v>
       </c>
       <c r="C70" t="s">
-        <v>308</v>
+        <v>277</v>
       </c>
       <c r="E70">
         <v>4681</v>
@@ -4453,7 +4438,7 @@
         <v>22</v>
       </c>
       <c r="G70" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H70" s="2" t="s">
         <v>21</v>
@@ -4462,16 +4447,16 @@
         <v>1</v>
       </c>
       <c r="J70" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K70">
         <v>1800</v>
       </c>
       <c r="L70" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M70" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
@@ -4482,7 +4467,7 @@
         <v>8</v>
       </c>
       <c r="C71" t="s">
-        <v>309</v>
+        <v>278</v>
       </c>
       <c r="E71">
         <v>5350</v>
@@ -4491,7 +4476,7 @@
         <v>22</v>
       </c>
       <c r="G71" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H71" s="2" t="s">
         <v>21</v>
@@ -4500,16 +4485,16 @@
         <v>1</v>
       </c>
       <c r="J71" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K71">
         <v>1800</v>
       </c>
       <c r="L71" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M71" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
@@ -4520,7 +4505,7 @@
         <v>8</v>
       </c>
       <c r="C72" t="s">
-        <v>310</v>
+        <v>279</v>
       </c>
       <c r="E72">
         <v>3500</v>
@@ -4529,7 +4514,7 @@
         <v>22</v>
       </c>
       <c r="G72" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H72" s="2" t="s">
         <v>21</v>
@@ -4538,16 +4523,16 @@
         <v>1</v>
       </c>
       <c r="J72" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K72">
         <v>1800</v>
       </c>
       <c r="L72" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M72" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
@@ -4558,7 +4543,7 @@
         <v>8</v>
       </c>
       <c r="C73" t="s">
-        <v>311</v>
+        <v>280</v>
       </c>
       <c r="E73">
         <v>2600</v>
@@ -4567,7 +4552,7 @@
         <v>22</v>
       </c>
       <c r="G73" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H73" s="2" t="s">
         <v>21</v>
@@ -4576,16 +4561,16 @@
         <v>1</v>
       </c>
       <c r="J73" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K73">
         <v>2400</v>
       </c>
       <c r="L73" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M73" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
@@ -4596,7 +4581,7 @@
         <v>8</v>
       </c>
       <c r="C74" t="s">
-        <v>312</v>
+        <v>281</v>
       </c>
       <c r="E74">
         <v>9150</v>
@@ -4605,7 +4590,7 @@
         <v>22</v>
       </c>
       <c r="G74" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H74" s="2" t="s">
         <v>21</v>
@@ -4614,16 +4599,16 @@
         <v>1</v>
       </c>
       <c r="J74" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K74">
         <v>1800</v>
       </c>
       <c r="L74" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M74" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
@@ -4634,7 +4619,7 @@
         <v>8</v>
       </c>
       <c r="C75" t="s">
-        <v>313</v>
+        <v>282</v>
       </c>
       <c r="E75">
         <v>1800</v>
@@ -4643,7 +4628,7 @@
         <v>22</v>
       </c>
       <c r="G75" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H75" s="2" t="s">
         <v>21</v>
@@ -4652,16 +4637,16 @@
         <v>1</v>
       </c>
       <c r="J75" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K75">
         <v>2400</v>
       </c>
       <c r="L75" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M75" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
@@ -4672,7 +4657,7 @@
         <v>8</v>
       </c>
       <c r="C76" t="s">
-        <v>314</v>
+        <v>283</v>
       </c>
       <c r="E76">
         <v>1348</v>
@@ -4681,7 +4666,7 @@
         <v>22</v>
       </c>
       <c r="G76" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H76" s="2" t="s">
         <v>21</v>
@@ -4690,16 +4675,16 @@
         <v>1</v>
       </c>
       <c r="J76" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K76">
         <v>1800</v>
       </c>
       <c r="L76" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M76" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
@@ -4710,7 +4695,7 @@
         <v>8</v>
       </c>
       <c r="C77" t="s">
-        <v>315</v>
+        <v>284</v>
       </c>
       <c r="E77">
         <v>7130</v>
@@ -4719,7 +4704,7 @@
         <v>22</v>
       </c>
       <c r="G77" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H77" s="2" t="s">
         <v>21</v>
@@ -4728,16 +4713,16 @@
         <v>1</v>
       </c>
       <c r="J77" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K77">
         <v>1800</v>
       </c>
       <c r="L77" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M77" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
@@ -4748,7 +4733,7 @@
         <v>8</v>
       </c>
       <c r="C78" t="s">
-        <v>316</v>
+        <v>285</v>
       </c>
       <c r="E78">
         <v>1020</v>
@@ -4757,7 +4742,7 @@
         <v>22</v>
       </c>
       <c r="G78" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H78" s="2" t="s">
         <v>21</v>
@@ -4766,16 +4751,16 @@
         <v>1</v>
       </c>
       <c r="J78" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K78">
         <v>1800</v>
       </c>
       <c r="L78" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M78" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
@@ -4786,7 +4771,7 @@
         <v>8</v>
       </c>
       <c r="C79" t="s">
-        <v>317</v>
+        <v>286</v>
       </c>
       <c r="E79">
         <v>7100</v>
@@ -4795,7 +4780,7 @@
         <v>22</v>
       </c>
       <c r="G79" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>21</v>
@@ -4804,16 +4789,16 @@
         <v>1</v>
       </c>
       <c r="J79" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K79">
         <v>1800</v>
       </c>
       <c r="L79" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M79" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
@@ -4824,7 +4809,7 @@
         <v>8</v>
       </c>
       <c r="C80" t="s">
-        <v>318</v>
+        <v>287</v>
       </c>
       <c r="E80">
         <v>2845</v>
@@ -4833,7 +4818,7 @@
         <v>22</v>
       </c>
       <c r="G80" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H80" s="2" t="s">
         <v>21</v>
@@ -4842,16 +4827,16 @@
         <v>1</v>
       </c>
       <c r="J80" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K80">
         <v>1800</v>
       </c>
       <c r="L80" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M80" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
@@ -4862,7 +4847,7 @@
         <v>8</v>
       </c>
       <c r="C81" t="s">
-        <v>319</v>
+        <v>288</v>
       </c>
       <c r="E81">
         <v>5523</v>
@@ -4871,7 +4856,7 @@
         <v>22</v>
       </c>
       <c r="G81" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H81" s="2" t="s">
         <v>21</v>
@@ -4880,16 +4865,16 @@
         <v>1</v>
       </c>
       <c r="J81" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K81">
         <v>3000</v>
       </c>
       <c r="L81" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M81" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
@@ -4906,7 +4891,7 @@
         <v>22</v>
       </c>
       <c r="G82" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H82" s="2" t="s">
         <v>21</v>
@@ -4915,16 +4900,16 @@
         <v>1</v>
       </c>
       <c r="J82" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K82">
         <v>1800</v>
       </c>
       <c r="L82" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M82" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
@@ -4941,7 +4926,7 @@
         <v>22</v>
       </c>
       <c r="G83" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H83" s="2" t="s">
         <v>21</v>
@@ -4950,16 +4935,16 @@
         <v>1</v>
       </c>
       <c r="J83" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K83">
         <v>1800</v>
       </c>
       <c r="L83" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M83" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
@@ -4976,7 +4961,7 @@
         <v>22</v>
       </c>
       <c r="G84" t="s">
-        <v>255</v>
+        <v>312</v>
       </c>
       <c r="H84" s="2" t="s">
         <v>21</v>
@@ -4985,16 +4970,16 @@
         <v>1</v>
       </c>
       <c r="J84" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="K84">
         <v>3000</v>
       </c>
       <c r="L84" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="M84" t="s">
-        <v>278</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -5018,42 +5003,42 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>221</v>
+        <v>193</v>
       </c>
       <c r="B1" t="s">
-        <v>222</v>
+        <v>194</v>
       </c>
       <c r="C1" t="s">
-        <v>223</v>
+        <v>195</v>
       </c>
       <c r="D1" t="s">
-        <v>224</v>
+        <v>196</v>
       </c>
       <c r="E1" t="s">
-        <v>229</v>
+        <v>201</v>
       </c>
       <c r="F1" t="s">
-        <v>230</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>225</v>
+        <v>197</v>
       </c>
       <c r="B2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E2" t="s">
         <v>226</v>
       </c>
-      <c r="C2" t="s">
-        <v>227</v>
-      </c>
-      <c r="D2" t="s">
-        <v>228</v>
-      </c>
-      <c r="E2" t="s">
-        <v>254</v>
-      </c>
       <c r="F2" t="s">
-        <v>231</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -5083,48 +5068,48 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>232</v>
+        <v>204</v>
       </c>
       <c r="B1" t="s">
-        <v>234</v>
+        <v>206</v>
       </c>
       <c r="C1" t="s">
-        <v>235</v>
+        <v>207</v>
       </c>
       <c r="D1" t="s">
-        <v>236</v>
+        <v>208</v>
       </c>
       <c r="E1" t="s">
-        <v>240</v>
+        <v>212</v>
       </c>
       <c r="F1" t="s">
-        <v>242</v>
+        <v>214</v>
       </c>
       <c r="G1" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
       <c r="H1" t="s">
-        <v>246</v>
+        <v>218</v>
       </c>
       <c r="I1" t="s">
-        <v>247</v>
+        <v>219</v>
       </c>
       <c r="J1" t="s">
-        <v>248</v>
+        <v>220</v>
       </c>
       <c r="K1" t="s">
-        <v>249</v>
+        <v>221</v>
       </c>
       <c r="L1" t="s">
-        <v>250</v>
+        <v>222</v>
       </c>
       <c r="M1" t="s">
-        <v>252</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>233</v>
+        <v>205</v>
       </c>
       <c r="B2">
         <v>7</v>
@@ -5136,13 +5121,13 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>241</v>
+        <v>213</v>
       </c>
       <c r="F2" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
       <c r="G2" t="s">
-        <v>245</v>
+        <v>217</v>
       </c>
       <c r="H2" t="s">
         <v>6</v>
@@ -5157,10 +5142,10 @@
         <v>102</v>
       </c>
       <c r="L2" t="s">
-        <v>251</v>
+        <v>223</v>
       </c>
       <c r="M2" t="s">
-        <v>253</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -5256,7 +5241,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>80</v>
@@ -5338,10 +5323,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" t="s">
         <v>166</v>
-      </c>
-      <c r="B2" t="s">
-        <v>167</v>
       </c>
       <c r="C2" t="s">
         <v>59</v>
@@ -5349,13 +5334,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>237</v>
+        <v>209</v>
       </c>
       <c r="B3" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="C3" t="s">
-        <v>239</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -5368,7 +5353,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5429,7 +5416,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection sqref="A1:L19"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6131,7 +6118,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6168,7 +6155,7 @@
         <v>91</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>182</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -6194,10 +6181,10 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="I2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -6207,10 +6194,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6223,7 +6210,7 @@
         <v>85</v>
       </c>
       <c r="C1" t="s">
-        <v>171</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -6234,12 +6221,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -6334,16 +6316,16 @@
         <v>102</v>
       </c>
       <c r="I2" t="s">
-        <v>185</v>
+        <v>313</v>
       </c>
       <c r="J2" t="s">
-        <v>184</v>
+        <v>312</v>
       </c>
       <c r="K2" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="L2" t="s">
-        <v>186</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -6372,16 +6354,16 @@
         <v>102</v>
       </c>
       <c r="I3" t="s">
-        <v>185</v>
+        <v>313</v>
       </c>
       <c r="J3" t="s">
-        <v>184</v>
+        <v>312</v>
       </c>
       <c r="K3" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="L3" t="s">
-        <v>187</v>
+        <v>293</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -6410,16 +6392,16 @@
         <v>102</v>
       </c>
       <c r="I4" t="s">
-        <v>185</v>
+        <v>313</v>
       </c>
       <c r="J4" t="s">
-        <v>184</v>
+        <v>312</v>
       </c>
       <c r="K4" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="L4" t="s">
-        <v>188</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -6448,16 +6430,16 @@
         <v>102</v>
       </c>
       <c r="I5" t="s">
-        <v>185</v>
+        <v>313</v>
       </c>
       <c r="J5" t="s">
-        <v>184</v>
+        <v>312</v>
       </c>
       <c r="K5" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="L5" t="s">
-        <v>189</v>
+        <v>295</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -6486,16 +6468,16 @@
         <v>102</v>
       </c>
       <c r="I6" t="s">
-        <v>185</v>
+        <v>313</v>
       </c>
       <c r="J6" t="s">
-        <v>184</v>
+        <v>312</v>
       </c>
       <c r="K6" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="L6" t="s">
-        <v>190</v>
+        <v>296</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -6524,16 +6506,16 @@
         <v>102</v>
       </c>
       <c r="I7" t="s">
-        <v>185</v>
+        <v>313</v>
       </c>
       <c r="J7" t="s">
-        <v>184</v>
+        <v>312</v>
       </c>
       <c r="K7" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="L7" t="s">
-        <v>191</v>
+        <v>297</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -6562,16 +6544,16 @@
         <v>102</v>
       </c>
       <c r="I8" t="s">
-        <v>185</v>
+        <v>313</v>
       </c>
       <c r="J8" t="s">
-        <v>184</v>
+        <v>312</v>
       </c>
       <c r="K8" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="L8" t="s">
-        <v>192</v>
+        <v>298</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -6600,16 +6582,16 @@
         <v>102</v>
       </c>
       <c r="I9" t="s">
-        <v>185</v>
+        <v>313</v>
       </c>
       <c r="J9" t="s">
-        <v>184</v>
+        <v>312</v>
       </c>
       <c r="K9" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="L9" t="s">
-        <v>193</v>
+        <v>299</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -6638,16 +6620,16 @@
         <v>102</v>
       </c>
       <c r="I10" t="s">
-        <v>185</v>
+        <v>313</v>
       </c>
       <c r="J10" t="s">
-        <v>184</v>
+        <v>312</v>
       </c>
       <c r="K10" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="L10" t="s">
-        <v>194</v>
+        <v>300</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -6676,16 +6658,16 @@
         <v>102</v>
       </c>
       <c r="I11" t="s">
-        <v>185</v>
+        <v>313</v>
       </c>
       <c r="J11" t="s">
-        <v>184</v>
+        <v>312</v>
       </c>
       <c r="K11" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="L11" t="s">
-        <v>195</v>
+        <v>301</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -6714,16 +6696,16 @@
         <v>102</v>
       </c>
       <c r="I12" t="s">
-        <v>185</v>
+        <v>313</v>
       </c>
       <c r="J12" t="s">
-        <v>184</v>
+        <v>312</v>
       </c>
       <c r="K12" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="L12" t="s">
-        <v>196</v>
+        <v>302</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -6752,16 +6734,16 @@
         <v>102</v>
       </c>
       <c r="I13" t="s">
-        <v>185</v>
+        <v>313</v>
       </c>
       <c r="J13" t="s">
-        <v>184</v>
+        <v>312</v>
       </c>
       <c r="K13" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="L13" t="s">
-        <v>197</v>
+        <v>303</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -6790,16 +6772,16 @@
         <v>102</v>
       </c>
       <c r="I14" t="s">
-        <v>185</v>
+        <v>313</v>
       </c>
       <c r="J14" t="s">
-        <v>184</v>
+        <v>312</v>
       </c>
       <c r="K14" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="L14" t="s">
-        <v>198</v>
+        <v>304</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -6828,16 +6810,16 @@
         <v>102</v>
       </c>
       <c r="I15" t="s">
-        <v>185</v>
+        <v>313</v>
       </c>
       <c r="J15" t="s">
-        <v>184</v>
+        <v>312</v>
       </c>
       <c r="K15" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="L15" t="s">
-        <v>199</v>
+        <v>305</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -6866,16 +6848,16 @@
         <v>102</v>
       </c>
       <c r="I16" t="s">
-        <v>185</v>
+        <v>313</v>
       </c>
       <c r="J16" t="s">
-        <v>184</v>
+        <v>312</v>
       </c>
       <c r="K16" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="L16" t="s">
-        <v>200</v>
+        <v>306</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -6904,16 +6886,16 @@
         <v>102</v>
       </c>
       <c r="I17" t="s">
-        <v>185</v>
+        <v>313</v>
       </c>
       <c r="J17" t="s">
-        <v>184</v>
+        <v>312</v>
       </c>
       <c r="K17" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="L17" t="s">
-        <v>201</v>
+        <v>307</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -6942,16 +6924,16 @@
         <v>102</v>
       </c>
       <c r="I18" t="s">
-        <v>185</v>
+        <v>313</v>
       </c>
       <c r="J18" t="s">
-        <v>184</v>
+        <v>312</v>
       </c>
       <c r="K18" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="L18" t="s">
-        <v>202</v>
+        <v>308</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -6980,16 +6962,16 @@
         <v>102</v>
       </c>
       <c r="I19" t="s">
-        <v>185</v>
+        <v>313</v>
       </c>
       <c r="J19" t="s">
-        <v>184</v>
+        <v>312</v>
       </c>
       <c r="K19" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="L19" t="s">
-        <v>203</v>
+        <v>309</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -7018,16 +7000,16 @@
         <v>102</v>
       </c>
       <c r="I20" t="s">
-        <v>185</v>
+        <v>313</v>
       </c>
       <c r="J20" t="s">
-        <v>184</v>
+        <v>312</v>
       </c>
       <c r="K20" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="L20" t="s">
-        <v>204</v>
+        <v>310</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -7056,16 +7038,16 @@
         <v>102</v>
       </c>
       <c r="I21" t="s">
-        <v>185</v>
+        <v>313</v>
       </c>
       <c r="J21" t="s">
-        <v>184</v>
+        <v>312</v>
       </c>
       <c r="K21" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="L21" t="s">
-        <v>205</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -7096,15 +7078,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B2" t="s">
-        <v>183</v>
+        <v>314</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>320</v>
+        <v>289</v>
+      </c>
+      <c r="B3" t="s">
+        <v>315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
95% completed 6694, need to validate the job is success or not..
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
+++ b/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11580" windowHeight="4650" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11580" windowHeight="4650" firstSheet="7" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="User_Details" sheetId="1" r:id="rId1"/>
@@ -545,9 +545,6 @@
     <t>a0N3B0000014s9d</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Mandt Account</t>
   </si>
   <si>
@@ -581,42 +578,6 @@
     <t>SVMXC__Skill__c</t>
   </si>
   <si>
-    <t>a1x3B0000002sRqQAI</t>
-  </si>
-  <si>
-    <t>a1x3B0000002sRrQAI</t>
-  </si>
-  <si>
-    <t>a1x3B0000002sRsQAI</t>
-  </si>
-  <si>
-    <t>a1x3B0000002sRtQAI</t>
-  </si>
-  <si>
-    <t>a1x3B0000002sRuQAI</t>
-  </si>
-  <si>
-    <t>a1x3B0000002sRvQAI</t>
-  </si>
-  <si>
-    <t>a133B000000OIxzQAG</t>
-  </si>
-  <si>
-    <t>a133B000000OIy0QAG</t>
-  </si>
-  <si>
-    <t>a133B000000OIy1QAG</t>
-  </si>
-  <si>
-    <t>a133B000000OIy2QAG</t>
-  </si>
-  <si>
-    <t>a133B000000OIy3QAG</t>
-  </si>
-  <si>
-    <t>a133B000000OIy4QAG</t>
-  </si>
-  <si>
     <t>Work Order for 6694</t>
   </si>
   <si>
@@ -911,82 +872,121 @@
     <t>John - Automation</t>
   </si>
   <si>
-    <t>a2D3B000002LXJhUAO</t>
-  </si>
-  <si>
-    <t>a2D3B000002LXJiUAO</t>
-  </si>
-  <si>
-    <t>a1u3B000000M5bHQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M5bIQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M5bJQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M5bKQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M5bLQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M5bMQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M5bNQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M5bOQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M5bPQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M5bQQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M5bRQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M5bSQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M5bTQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M5bUQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M5bVQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M5bWQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M5bXQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M5bYQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M5bZQAS</t>
-  </si>
-  <si>
-    <t>a1u3B000000M5baQAC</t>
-  </si>
-  <si>
-    <t>a2N3B000000H0oYUAS</t>
-  </si>
-  <si>
-    <t>a1y3B000000HhtBQAS</t>
-  </si>
-  <si>
-    <t>0013B00000I5jyhQAB</t>
-  </si>
-  <si>
-    <t>0013B00000I5jyiQAB</t>
+    <t>0013B00000I5jzGQAR</t>
+  </si>
+  <si>
+    <t>0013B00000I5jzHQAR</t>
+  </si>
+  <si>
+    <t>01m3B0000004DHPQA2</t>
+  </si>
+  <si>
+    <t>a2N3B000000H0qAUAS</t>
+  </si>
+  <si>
+    <t>a1y3B000000HhtGQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5bvQAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5bwQAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5bxQAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5byQAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5bzQAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5c0QAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5c1QAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5c2QAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5c3QAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5c4QAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5c5QAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5c6QAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5c7QAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5c8QAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5c9QAC</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5cAQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5cBQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5cCQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5cDQAS</t>
+  </si>
+  <si>
+    <t>a1u3B000000M5cEQAS</t>
+  </si>
+  <si>
+    <t>a2D3B000002LXJrUAO</t>
+  </si>
+  <si>
+    <t>a2D3B000002LXJsUAO</t>
+  </si>
+  <si>
+    <t>a1x3B0000002suCQAQ</t>
+  </si>
+  <si>
+    <t>a1x3B0000002suDQAQ</t>
+  </si>
+  <si>
+    <t>a1x3B0000002suEQAQ</t>
+  </si>
+  <si>
+    <t>a1x3B0000002suFQAQ</t>
+  </si>
+  <si>
+    <t>a1x3B0000002suGQAQ</t>
+  </si>
+  <si>
+    <t>a1x3B0000002suHQAQ</t>
+  </si>
+  <si>
+    <t>a133B000000OJk7QAG</t>
+  </si>
+  <si>
+    <t>a133B000000OJk8QAG</t>
+  </si>
+  <si>
+    <t>a133B000000OJk9QAG</t>
+  </si>
+  <si>
+    <t>a133B000000OJkAQAW</t>
+  </si>
+  <si>
+    <t>a133B000000OJkBQAW</t>
+  </si>
+  <si>
+    <t>a133B000000OJkCQAW</t>
   </si>
 </sst>
 </file>
@@ -1442,7 +1442,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -1451,12 +1451,12 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>290</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -1465,7 +1465,7 @@
         <v>162</v>
       </c>
       <c r="D3" t="s">
-        <v>291</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -1507,7 +1507,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1520,13 +1520,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" t="s">
         <v>170</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>171</v>
-      </c>
-      <c r="C1" t="s">
-        <v>172</v>
       </c>
       <c r="D1" t="s">
         <v>84</v>
@@ -1534,86 +1534,86 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
       <c r="B2" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D2" t="s">
-        <v>186</v>
+        <v>310</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
       <c r="B3" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D3" t="s">
-        <v>187</v>
+        <v>311</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
       <c r="B4" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D4" t="s">
-        <v>188</v>
+        <v>312</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
       <c r="B5" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D5" t="s">
-        <v>189</v>
+        <v>313</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
       <c r="B6" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D6" t="s">
-        <v>190</v>
+        <v>314</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
       <c r="B7" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D7" t="s">
-        <v>191</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -1641,16 +1641,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B1" t="s">
         <v>95</v>
       </c>
       <c r="C1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E1" t="s">
         <v>84</v>
@@ -1658,104 +1658,104 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="B2" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="C2" t="s">
-        <v>290</v>
+        <v>302</v>
       </c>
       <c r="D2">
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>180</v>
+        <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="B3" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="C3" t="s">
-        <v>290</v>
+        <v>302</v>
       </c>
       <c r="D3">
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>181</v>
+        <v>305</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="B4" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="C4" t="s">
-        <v>290</v>
+        <v>302</v>
       </c>
       <c r="D4">
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>182</v>
+        <v>306</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="B5" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="C5" t="s">
-        <v>291</v>
+        <v>303</v>
       </c>
       <c r="D5">
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>183</v>
+        <v>307</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="B6" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="C6" t="s">
-        <v>291</v>
+        <v>303</v>
       </c>
       <c r="D6">
         <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>184</v>
+        <v>308</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="B7" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="C7" t="s">
-        <v>291</v>
+        <v>303</v>
       </c>
       <c r="D7">
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>185</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -1825,7 +1825,7 @@
         <v>10</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -1848,7 +1848,7 @@
         <v>22</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>21</v>
@@ -1857,16 +1857,16 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K2">
         <v>2400</v>
       </c>
       <c r="L2" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M2" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1889,7 +1889,7 @@
         <v>22</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>21</v>
@@ -1898,16 +1898,16 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K3">
         <v>3000</v>
       </c>
       <c r="L3" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M3" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1930,7 +1930,7 @@
         <v>22</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>21</v>
@@ -1939,16 +1939,16 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K4">
         <v>3000</v>
       </c>
       <c r="L4" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M4" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1968,7 +1968,7 @@
         <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>21</v>
@@ -1977,16 +1977,16 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K5">
         <v>1800</v>
       </c>
       <c r="L5" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M5" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2006,7 +2006,7 @@
         <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>21</v>
@@ -2015,16 +2015,16 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K6">
         <v>1800</v>
       </c>
       <c r="L6" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M6" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -2044,7 +2044,7 @@
         <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>21</v>
@@ -2053,16 +2053,16 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K7">
         <v>1800</v>
       </c>
       <c r="L7" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M7" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -2082,7 +2082,7 @@
         <v>22</v>
       </c>
       <c r="G8" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>21</v>
@@ -2091,16 +2091,16 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K8">
         <v>3000</v>
       </c>
       <c r="L8" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M8" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -2120,7 +2120,7 @@
         <v>22</v>
       </c>
       <c r="G9" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>21</v>
@@ -2129,16 +2129,16 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K9">
         <v>2400</v>
       </c>
       <c r="L9" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M9" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -2158,7 +2158,7 @@
         <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>21</v>
@@ -2167,16 +2167,16 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K10">
         <v>2400</v>
       </c>
       <c r="L10" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M10" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -2196,7 +2196,7 @@
         <v>22</v>
       </c>
       <c r="G11" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>21</v>
@@ -2205,16 +2205,16 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K11">
         <v>2400</v>
       </c>
       <c r="L11" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M11" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -2234,7 +2234,7 @@
         <v>22</v>
       </c>
       <c r="G12" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>21</v>
@@ -2243,16 +2243,16 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K12">
         <v>1800</v>
       </c>
       <c r="L12" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M12" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -2272,7 +2272,7 @@
         <v>22</v>
       </c>
       <c r="G13" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>21</v>
@@ -2281,16 +2281,16 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K13">
         <v>2400</v>
       </c>
       <c r="L13" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M13" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -2310,7 +2310,7 @@
         <v>22</v>
       </c>
       <c r="G14" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>21</v>
@@ -2319,16 +2319,16 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K14">
         <v>2400</v>
       </c>
       <c r="L14" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M14" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -2348,7 +2348,7 @@
         <v>22</v>
       </c>
       <c r="G15" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>21</v>
@@ -2357,16 +2357,16 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K15">
         <v>2400</v>
       </c>
       <c r="L15" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M15" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -2386,7 +2386,7 @@
         <v>22</v>
       </c>
       <c r="G16" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>21</v>
@@ -2395,16 +2395,16 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K16">
         <v>2400</v>
       </c>
       <c r="L16" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M16" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -2424,7 +2424,7 @@
         <v>22</v>
       </c>
       <c r="G17" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>21</v>
@@ -2433,16 +2433,16 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K17">
         <v>1800</v>
       </c>
       <c r="L17" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M17" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -2462,7 +2462,7 @@
         <v>22</v>
       </c>
       <c r="G18" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>21</v>
@@ -2471,16 +2471,16 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K18">
         <v>3000</v>
       </c>
       <c r="L18" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M18" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -2500,7 +2500,7 @@
         <v>22</v>
       </c>
       <c r="G19" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>21</v>
@@ -2509,16 +2509,16 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K19">
         <v>2400</v>
       </c>
       <c r="L19" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M19" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -2529,7 +2529,7 @@
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="E20">
         <v>4400</v>
@@ -2538,7 +2538,7 @@
         <v>22</v>
       </c>
       <c r="G20" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>21</v>
@@ -2547,16 +2547,16 @@
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K20">
         <v>2400</v>
       </c>
       <c r="L20" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M20" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -2567,7 +2567,7 @@
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="E21">
         <v>9250</v>
@@ -2576,7 +2576,7 @@
         <v>22</v>
       </c>
       <c r="G21" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>21</v>
@@ -2585,16 +2585,16 @@
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K21">
         <v>2400</v>
       </c>
       <c r="L21" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M21" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -2605,7 +2605,7 @@
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="E22">
         <v>2610</v>
@@ -2614,7 +2614,7 @@
         <v>22</v>
       </c>
       <c r="G22" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>21</v>
@@ -2623,16 +2623,16 @@
         <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K22">
         <v>2400</v>
       </c>
       <c r="L22" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M22" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -2643,7 +2643,7 @@
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="E23">
         <v>1050</v>
@@ -2652,7 +2652,7 @@
         <v>22</v>
       </c>
       <c r="G23" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>21</v>
@@ -2661,16 +2661,16 @@
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K23">
         <v>1800</v>
       </c>
       <c r="L23" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M23" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -2681,7 +2681,7 @@
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="E24">
         <v>1200</v>
@@ -2690,7 +2690,7 @@
         <v>22</v>
       </c>
       <c r="G24" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>21</v>
@@ -2699,16 +2699,16 @@
         <v>1</v>
       </c>
       <c r="J24" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K24">
         <v>3000</v>
       </c>
       <c r="L24" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M24" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -2719,7 +2719,7 @@
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="E25">
         <v>3300</v>
@@ -2728,7 +2728,7 @@
         <v>22</v>
       </c>
       <c r="G25" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>21</v>
@@ -2737,16 +2737,16 @@
         <v>1</v>
       </c>
       <c r="J25" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K25">
         <v>3000</v>
       </c>
       <c r="L25" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M25" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -2757,7 +2757,7 @@
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="E26">
         <v>9000</v>
@@ -2766,7 +2766,7 @@
         <v>22</v>
       </c>
       <c r="G26" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>21</v>
@@ -2775,16 +2775,16 @@
         <v>1</v>
       </c>
       <c r="J26" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K26">
         <v>3000</v>
       </c>
       <c r="L26" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M26" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -2795,7 +2795,7 @@
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="E27">
         <v>9140</v>
@@ -2804,7 +2804,7 @@
         <v>22</v>
       </c>
       <c r="G27" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>21</v>
@@ -2813,16 +2813,16 @@
         <v>1</v>
       </c>
       <c r="J27" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K27">
         <v>2400</v>
       </c>
       <c r="L27" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M27" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -2833,7 +2833,7 @@
         <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="E28">
         <v>9340</v>
@@ -2842,7 +2842,7 @@
         <v>22</v>
       </c>
       <c r="G28" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>21</v>
@@ -2851,16 +2851,16 @@
         <v>1</v>
       </c>
       <c r="J28" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K28">
         <v>2400</v>
       </c>
       <c r="L28" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M28" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -2871,7 +2871,7 @@
         <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="E29">
         <v>8540</v>
@@ -2880,7 +2880,7 @@
         <v>22</v>
       </c>
       <c r="G29" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>21</v>
@@ -2889,16 +2889,16 @@
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K29">
         <v>1800</v>
       </c>
       <c r="L29" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M29" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -2909,7 +2909,7 @@
         <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="E30">
         <v>8620</v>
@@ -2918,7 +2918,7 @@
         <v>22</v>
       </c>
       <c r="G30" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>21</v>
@@ -2927,16 +2927,16 @@
         <v>1</v>
       </c>
       <c r="J30" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K30">
         <v>3000</v>
       </c>
       <c r="L30" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M30" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -2947,7 +2947,7 @@
         <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="E31">
         <v>8430</v>
@@ -2956,7 +2956,7 @@
         <v>22</v>
       </c>
       <c r="G31" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>21</v>
@@ -2965,16 +2965,16 @@
         <v>1</v>
       </c>
       <c r="J31" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K31">
         <v>1800</v>
       </c>
       <c r="L31" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M31" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -2985,7 +2985,7 @@
         <v>8</v>
       </c>
       <c r="C32" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="E32">
         <v>2920</v>
@@ -2994,7 +2994,7 @@
         <v>22</v>
       </c>
       <c r="G32" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>21</v>
@@ -3003,16 +3003,16 @@
         <v>1</v>
       </c>
       <c r="J32" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K32">
         <v>1800</v>
       </c>
       <c r="L32" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M32" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -3023,7 +3023,7 @@
         <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="E33">
         <v>5500</v>
@@ -3032,7 +3032,7 @@
         <v>22</v>
       </c>
       <c r="G33" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>21</v>
@@ -3041,16 +3041,16 @@
         <v>1</v>
       </c>
       <c r="J33" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K33">
         <v>3000</v>
       </c>
       <c r="L33" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M33" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -3061,7 +3061,7 @@
         <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="E34">
         <v>2000</v>
@@ -3070,7 +3070,7 @@
         <v>22</v>
       </c>
       <c r="G34" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>21</v>
@@ -3079,16 +3079,16 @@
         <v>1</v>
       </c>
       <c r="J34" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K34">
         <v>2400</v>
       </c>
       <c r="L34" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M34" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -3099,7 +3099,7 @@
         <v>8</v>
       </c>
       <c r="C35" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="E35">
         <v>1348</v>
@@ -3108,7 +3108,7 @@
         <v>22</v>
       </c>
       <c r="G35" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>21</v>
@@ -3117,16 +3117,16 @@
         <v>1</v>
       </c>
       <c r="J35" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K35">
         <v>3000</v>
       </c>
       <c r="L35" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M35" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -3137,7 +3137,7 @@
         <v>8</v>
       </c>
       <c r="C36" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="E36">
         <v>8400</v>
@@ -3146,7 +3146,7 @@
         <v>22</v>
       </c>
       <c r="G36" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>21</v>
@@ -3155,16 +3155,16 @@
         <v>1</v>
       </c>
       <c r="J36" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K36">
         <v>2400</v>
       </c>
       <c r="L36" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M36" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -3175,7 +3175,7 @@
         <v>8</v>
       </c>
       <c r="C37" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="E37">
         <v>1348</v>
@@ -3184,7 +3184,7 @@
         <v>22</v>
       </c>
       <c r="G37" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>21</v>
@@ -3193,16 +3193,16 @@
         <v>1</v>
       </c>
       <c r="J37" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K37">
         <v>2400</v>
       </c>
       <c r="L37" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M37" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -3213,7 +3213,7 @@
         <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="E38">
         <v>7130</v>
@@ -3222,7 +3222,7 @@
         <v>22</v>
       </c>
       <c r="G38" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>21</v>
@@ -3231,16 +3231,16 @@
         <v>1</v>
       </c>
       <c r="J38" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K38">
         <v>2400</v>
       </c>
       <c r="L38" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M38" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -3251,7 +3251,7 @@
         <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="E39">
         <v>1140</v>
@@ -3260,7 +3260,7 @@
         <v>22</v>
       </c>
       <c r="G39" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>21</v>
@@ -3269,16 +3269,16 @@
         <v>1</v>
       </c>
       <c r="J39" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K39">
         <v>3000</v>
       </c>
       <c r="L39" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M39" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -3289,7 +3289,7 @@
         <v>8</v>
       </c>
       <c r="C40" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="E40">
         <v>2840</v>
@@ -3298,7 +3298,7 @@
         <v>22</v>
       </c>
       <c r="G40" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>21</v>
@@ -3307,16 +3307,16 @@
         <v>1</v>
       </c>
       <c r="J40" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K40">
         <v>3000</v>
       </c>
       <c r="L40" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M40" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -3327,7 +3327,7 @@
         <v>8</v>
       </c>
       <c r="C41" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="E41">
         <v>1348</v>
@@ -3336,7 +3336,7 @@
         <v>22</v>
       </c>
       <c r="G41" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>21</v>
@@ -3345,16 +3345,16 @@
         <v>1</v>
       </c>
       <c r="J41" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K41">
         <v>3000</v>
       </c>
       <c r="L41" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M41" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
@@ -3365,7 +3365,7 @@
         <v>8</v>
       </c>
       <c r="C42" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="E42">
         <v>2550</v>
@@ -3374,7 +3374,7 @@
         <v>22</v>
       </c>
       <c r="G42" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>21</v>
@@ -3383,16 +3383,16 @@
         <v>1</v>
       </c>
       <c r="J42" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K42">
         <v>1800</v>
       </c>
       <c r="L42" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M42" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -3403,7 +3403,7 @@
         <v>8</v>
       </c>
       <c r="C43" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="E43">
         <v>4000</v>
@@ -3412,7 +3412,7 @@
         <v>22</v>
       </c>
       <c r="G43" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>21</v>
@@ -3421,16 +3421,16 @@
         <v>1</v>
       </c>
       <c r="J43" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K43">
         <v>1800</v>
       </c>
       <c r="L43" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M43" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -3441,7 +3441,7 @@
         <v>8</v>
       </c>
       <c r="C44" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="E44">
         <v>2570</v>
@@ -3450,7 +3450,7 @@
         <v>22</v>
       </c>
       <c r="G44" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>21</v>
@@ -3459,16 +3459,16 @@
         <v>1</v>
       </c>
       <c r="J44" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K44">
         <v>2400</v>
       </c>
       <c r="L44" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M44" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
@@ -3479,7 +3479,7 @@
         <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="E45">
         <v>1082</v>
@@ -3488,7 +3488,7 @@
         <v>22</v>
       </c>
       <c r="G45" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>21</v>
@@ -3497,16 +3497,16 @@
         <v>1</v>
       </c>
       <c r="J45" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K45">
         <v>2280</v>
       </c>
       <c r="L45" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M45" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
@@ -3517,7 +3517,7 @@
         <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="E46">
         <v>2800</v>
@@ -3526,7 +3526,7 @@
         <v>22</v>
       </c>
       <c r="G46" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>21</v>
@@ -3535,16 +3535,16 @@
         <v>1</v>
       </c>
       <c r="J46" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K46">
         <v>2400</v>
       </c>
       <c r="L46" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M46" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -3555,7 +3555,7 @@
         <v>8</v>
       </c>
       <c r="C47" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="E47">
         <v>5300</v>
@@ -3564,7 +3564,7 @@
         <v>22</v>
       </c>
       <c r="G47" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H47" s="2" t="s">
         <v>21</v>
@@ -3573,16 +3573,16 @@
         <v>1</v>
       </c>
       <c r="J47" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K47">
         <v>2400</v>
       </c>
       <c r="L47" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M47" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
@@ -3593,7 +3593,7 @@
         <v>8</v>
       </c>
       <c r="C48" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="E48">
         <v>3500</v>
@@ -3602,7 +3602,7 @@
         <v>22</v>
       </c>
       <c r="G48" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H48" s="2" t="s">
         <v>21</v>
@@ -3611,16 +3611,16 @@
         <v>1</v>
       </c>
       <c r="J48" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K48">
         <v>2400</v>
       </c>
       <c r="L48" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M48" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
@@ -3631,7 +3631,7 @@
         <v>8</v>
       </c>
       <c r="C49" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="E49">
         <v>5380</v>
@@ -3640,7 +3640,7 @@
         <v>22</v>
       </c>
       <c r="G49" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H49" s="2" t="s">
         <v>21</v>
@@ -3649,16 +3649,16 @@
         <v>1</v>
       </c>
       <c r="J49" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K49">
         <v>1800</v>
       </c>
       <c r="L49" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M49" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
@@ -3669,7 +3669,7 @@
         <v>8</v>
       </c>
       <c r="C50" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="E50">
         <v>2570</v>
@@ -3678,7 +3678,7 @@
         <v>22</v>
       </c>
       <c r="G50" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H50" s="2" t="s">
         <v>21</v>
@@ -3687,16 +3687,16 @@
         <v>1</v>
       </c>
       <c r="J50" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K50">
         <v>1800</v>
       </c>
       <c r="L50" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M50" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
@@ -3707,7 +3707,7 @@
         <v>8</v>
       </c>
       <c r="C51" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="E51">
         <v>1982</v>
@@ -3716,7 +3716,7 @@
         <v>22</v>
       </c>
       <c r="G51" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H51" s="2" t="s">
         <v>21</v>
@@ -3725,16 +3725,16 @@
         <v>1</v>
       </c>
       <c r="J51" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K51">
         <v>1800</v>
       </c>
       <c r="L51" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M51" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
@@ -3745,7 +3745,7 @@
         <v>8</v>
       </c>
       <c r="C52" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="E52">
         <v>6800</v>
@@ -3754,7 +3754,7 @@
         <v>22</v>
       </c>
       <c r="G52" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H52" s="2" t="s">
         <v>21</v>
@@ -3763,16 +3763,16 @@
         <v>1</v>
       </c>
       <c r="J52" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K52">
         <v>2400</v>
       </c>
       <c r="L52" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M52" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
@@ -3783,7 +3783,7 @@
         <v>8</v>
       </c>
       <c r="C53" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="E53">
         <v>8400</v>
@@ -3792,7 +3792,7 @@
         <v>22</v>
       </c>
       <c r="G53" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H53" s="2" t="s">
         <v>21</v>
@@ -3801,16 +3801,16 @@
         <v>1</v>
       </c>
       <c r="J53" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K53">
         <v>2400</v>
       </c>
       <c r="L53" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M53" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
@@ -3821,7 +3821,7 @@
         <v>8</v>
       </c>
       <c r="C54" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="E54">
         <v>4500</v>
@@ -3830,7 +3830,7 @@
         <v>22</v>
       </c>
       <c r="G54" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H54" s="2" t="s">
         <v>21</v>
@@ -3839,16 +3839,16 @@
         <v>1</v>
       </c>
       <c r="J54" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K54">
         <v>3000</v>
       </c>
       <c r="L54" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M54" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
@@ -3859,7 +3859,7 @@
         <v>8</v>
       </c>
       <c r="C55" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="E55">
         <v>1348</v>
@@ -3868,7 +3868,7 @@
         <v>22</v>
       </c>
       <c r="G55" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>21</v>
@@ -3877,16 +3877,16 @@
         <v>1</v>
       </c>
       <c r="J55" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K55">
         <v>4920</v>
       </c>
       <c r="L55" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M55" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
@@ -3897,7 +3897,7 @@
         <v>8</v>
       </c>
       <c r="C56" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="E56">
         <v>7130</v>
@@ -3906,7 +3906,7 @@
         <v>22</v>
       </c>
       <c r="G56" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H56" s="2" t="s">
         <v>21</v>
@@ -3915,16 +3915,16 @@
         <v>1</v>
       </c>
       <c r="J56" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K56">
         <v>2400</v>
       </c>
       <c r="L56" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M56" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
@@ -3935,7 +3935,7 @@
         <v>8</v>
       </c>
       <c r="C57" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="E57">
         <v>1348</v>
@@ -3944,7 +3944,7 @@
         <v>22</v>
       </c>
       <c r="G57" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H57" s="2" t="s">
         <v>21</v>
@@ -3953,16 +3953,16 @@
         <v>1</v>
       </c>
       <c r="J57" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K57">
         <v>2400</v>
       </c>
       <c r="L57" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M57" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -3973,7 +3973,7 @@
         <v>8</v>
       </c>
       <c r="C58" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="E58">
         <v>3500</v>
@@ -3982,7 +3982,7 @@
         <v>22</v>
       </c>
       <c r="G58" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>21</v>
@@ -3991,16 +3991,16 @@
         <v>1</v>
       </c>
       <c r="J58" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K58">
         <v>2400</v>
       </c>
       <c r="L58" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M58" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
@@ -4011,7 +4011,7 @@
         <v>8</v>
       </c>
       <c r="C59" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="E59">
         <v>2000</v>
@@ -4020,7 +4020,7 @@
         <v>22</v>
       </c>
       <c r="G59" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>21</v>
@@ -4029,16 +4029,16 @@
         <v>1</v>
       </c>
       <c r="J59" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K59">
         <v>2400</v>
       </c>
       <c r="L59" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M59" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
@@ -4049,7 +4049,7 @@
         <v>8</v>
       </c>
       <c r="C60" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="E60">
         <v>8400</v>
@@ -4058,7 +4058,7 @@
         <v>22</v>
       </c>
       <c r="G60" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H60" s="2" t="s">
         <v>21</v>
@@ -4067,16 +4067,16 @@
         <v>1</v>
       </c>
       <c r="J60" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K60">
         <v>2280</v>
       </c>
       <c r="L60" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M60" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
@@ -4087,7 +4087,7 @@
         <v>8</v>
       </c>
       <c r="C61" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="E61">
         <v>2060</v>
@@ -4096,7 +4096,7 @@
         <v>22</v>
       </c>
       <c r="G61" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H61" s="2" t="s">
         <v>21</v>
@@ -4105,16 +4105,16 @@
         <v>1</v>
       </c>
       <c r="J61" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K61">
         <v>1800</v>
       </c>
       <c r="L61" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M61" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
@@ -4125,7 +4125,7 @@
         <v>8</v>
       </c>
       <c r="C62" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="E62">
         <v>2640</v>
@@ -4134,7 +4134,7 @@
         <v>22</v>
       </c>
       <c r="G62" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H62" s="2" t="s">
         <v>21</v>
@@ -4143,16 +4143,16 @@
         <v>1</v>
       </c>
       <c r="J62" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K62">
         <v>3360</v>
       </c>
       <c r="L62" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M62" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
@@ -4163,7 +4163,7 @@
         <v>8</v>
       </c>
       <c r="C63" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="E63">
         <v>3511</v>
@@ -4172,7 +4172,7 @@
         <v>22</v>
       </c>
       <c r="G63" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H63" s="2" t="s">
         <v>21</v>
@@ -4181,16 +4181,16 @@
         <v>1</v>
       </c>
       <c r="J63" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K63">
         <v>2400</v>
       </c>
       <c r="L63" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M63" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
@@ -4201,7 +4201,7 @@
         <v>8</v>
       </c>
       <c r="C64" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="E64">
         <v>8400</v>
@@ -4210,7 +4210,7 @@
         <v>22</v>
       </c>
       <c r="G64" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H64" s="2" t="s">
         <v>21</v>
@@ -4219,16 +4219,16 @@
         <v>1</v>
       </c>
       <c r="J64" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K64">
         <v>2400</v>
       </c>
       <c r="L64" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M64" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
@@ -4239,7 +4239,7 @@
         <v>8</v>
       </c>
       <c r="C65" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="E65">
         <v>3511</v>
@@ -4248,7 +4248,7 @@
         <v>22</v>
       </c>
       <c r="G65" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H65" s="2" t="s">
         <v>21</v>
@@ -4257,16 +4257,16 @@
         <v>1</v>
       </c>
       <c r="J65" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K65">
         <v>2400</v>
       </c>
       <c r="L65" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M65" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
@@ -4277,7 +4277,7 @@
         <v>8</v>
       </c>
       <c r="C66" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="E66">
         <v>1800</v>
@@ -4286,7 +4286,7 @@
         <v>22</v>
       </c>
       <c r="G66" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H66" s="2" t="s">
         <v>21</v>
@@ -4295,16 +4295,16 @@
         <v>1</v>
       </c>
       <c r="J66" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K66">
         <v>2400</v>
       </c>
       <c r="L66" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M66" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
@@ -4315,7 +4315,7 @@
         <v>8</v>
       </c>
       <c r="C67" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
       <c r="E67">
         <v>2500</v>
@@ -4324,7 +4324,7 @@
         <v>22</v>
       </c>
       <c r="G67" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H67" s="2" t="s">
         <v>21</v>
@@ -4333,16 +4333,16 @@
         <v>1</v>
       </c>
       <c r="J67" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K67">
         <v>1800</v>
       </c>
       <c r="L67" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M67" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
@@ -4353,7 +4353,7 @@
         <v>8</v>
       </c>
       <c r="C68" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
       <c r="E68">
         <v>2840</v>
@@ -4362,7 +4362,7 @@
         <v>22</v>
       </c>
       <c r="G68" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H68" s="2" t="s">
         <v>21</v>
@@ -4371,16 +4371,16 @@
         <v>1</v>
       </c>
       <c r="J68" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K68">
         <v>2400</v>
       </c>
       <c r="L68" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M68" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
@@ -4391,7 +4391,7 @@
         <v>8</v>
       </c>
       <c r="C69" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="E69">
         <v>2660</v>
@@ -4400,7 +4400,7 @@
         <v>22</v>
       </c>
       <c r="G69" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H69" s="2" t="s">
         <v>21</v>
@@ -4409,16 +4409,16 @@
         <v>1</v>
       </c>
       <c r="J69" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K69">
         <v>2280</v>
       </c>
       <c r="L69" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M69" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
@@ -4429,7 +4429,7 @@
         <v>8</v>
       </c>
       <c r="C70" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
       <c r="E70">
         <v>4681</v>
@@ -4438,7 +4438,7 @@
         <v>22</v>
       </c>
       <c r="G70" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H70" s="2" t="s">
         <v>21</v>
@@ -4447,16 +4447,16 @@
         <v>1</v>
       </c>
       <c r="J70" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K70">
         <v>1800</v>
       </c>
       <c r="L70" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M70" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
@@ -4467,7 +4467,7 @@
         <v>8</v>
       </c>
       <c r="C71" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="E71">
         <v>5350</v>
@@ -4476,7 +4476,7 @@
         <v>22</v>
       </c>
       <c r="G71" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H71" s="2" t="s">
         <v>21</v>
@@ -4485,16 +4485,16 @@
         <v>1</v>
       </c>
       <c r="J71" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K71">
         <v>1800</v>
       </c>
       <c r="L71" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M71" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
@@ -4505,7 +4505,7 @@
         <v>8</v>
       </c>
       <c r="C72" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="E72">
         <v>3500</v>
@@ -4514,7 +4514,7 @@
         <v>22</v>
       </c>
       <c r="G72" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H72" s="2" t="s">
         <v>21</v>
@@ -4523,16 +4523,16 @@
         <v>1</v>
       </c>
       <c r="J72" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K72">
         <v>1800</v>
       </c>
       <c r="L72" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M72" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
@@ -4543,7 +4543,7 @@
         <v>8</v>
       </c>
       <c r="C73" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="E73">
         <v>2600</v>
@@ -4552,7 +4552,7 @@
         <v>22</v>
       </c>
       <c r="G73" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H73" s="2" t="s">
         <v>21</v>
@@ -4561,16 +4561,16 @@
         <v>1</v>
       </c>
       <c r="J73" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K73">
         <v>2400</v>
       </c>
       <c r="L73" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M73" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
@@ -4581,7 +4581,7 @@
         <v>8</v>
       </c>
       <c r="C74" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="E74">
         <v>9150</v>
@@ -4590,7 +4590,7 @@
         <v>22</v>
       </c>
       <c r="G74" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H74" s="2" t="s">
         <v>21</v>
@@ -4599,16 +4599,16 @@
         <v>1</v>
       </c>
       <c r="J74" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K74">
         <v>1800</v>
       </c>
       <c r="L74" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M74" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
@@ -4619,7 +4619,7 @@
         <v>8</v>
       </c>
       <c r="C75" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="E75">
         <v>1800</v>
@@ -4628,7 +4628,7 @@
         <v>22</v>
       </c>
       <c r="G75" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H75" s="2" t="s">
         <v>21</v>
@@ -4637,16 +4637,16 @@
         <v>1</v>
       </c>
       <c r="J75" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K75">
         <v>2400</v>
       </c>
       <c r="L75" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M75" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
@@ -4657,7 +4657,7 @@
         <v>8</v>
       </c>
       <c r="C76" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="E76">
         <v>1348</v>
@@ -4666,7 +4666,7 @@
         <v>22</v>
       </c>
       <c r="G76" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H76" s="2" t="s">
         <v>21</v>
@@ -4675,16 +4675,16 @@
         <v>1</v>
       </c>
       <c r="J76" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K76">
         <v>1800</v>
       </c>
       <c r="L76" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M76" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
@@ -4695,7 +4695,7 @@
         <v>8</v>
       </c>
       <c r="C77" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
       <c r="E77">
         <v>7130</v>
@@ -4704,7 +4704,7 @@
         <v>22</v>
       </c>
       <c r="G77" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H77" s="2" t="s">
         <v>21</v>
@@ -4713,16 +4713,16 @@
         <v>1</v>
       </c>
       <c r="J77" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K77">
         <v>1800</v>
       </c>
       <c r="L77" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M77" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
@@ -4733,7 +4733,7 @@
         <v>8</v>
       </c>
       <c r="C78" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="E78">
         <v>1020</v>
@@ -4742,7 +4742,7 @@
         <v>22</v>
       </c>
       <c r="G78" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H78" s="2" t="s">
         <v>21</v>
@@ -4751,16 +4751,16 @@
         <v>1</v>
       </c>
       <c r="J78" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K78">
         <v>1800</v>
       </c>
       <c r="L78" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M78" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
@@ -4771,7 +4771,7 @@
         <v>8</v>
       </c>
       <c r="C79" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="E79">
         <v>7100</v>
@@ -4780,7 +4780,7 @@
         <v>22</v>
       </c>
       <c r="G79" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>21</v>
@@ -4789,16 +4789,16 @@
         <v>1</v>
       </c>
       <c r="J79" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K79">
         <v>1800</v>
       </c>
       <c r="L79" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M79" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
@@ -4809,7 +4809,7 @@
         <v>8</v>
       </c>
       <c r="C80" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
       <c r="E80">
         <v>2845</v>
@@ -4818,7 +4818,7 @@
         <v>22</v>
       </c>
       <c r="G80" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H80" s="2" t="s">
         <v>21</v>
@@ -4827,16 +4827,16 @@
         <v>1</v>
       </c>
       <c r="J80" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K80">
         <v>1800</v>
       </c>
       <c r="L80" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M80" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
@@ -4847,7 +4847,7 @@
         <v>8</v>
       </c>
       <c r="C81" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
       <c r="E81">
         <v>5523</v>
@@ -4856,7 +4856,7 @@
         <v>22</v>
       </c>
       <c r="G81" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H81" s="2" t="s">
         <v>21</v>
@@ -4865,16 +4865,16 @@
         <v>1</v>
       </c>
       <c r="J81" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K81">
         <v>3000</v>
       </c>
       <c r="L81" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M81" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
@@ -4891,7 +4891,7 @@
         <v>22</v>
       </c>
       <c r="G82" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H82" s="2" t="s">
         <v>21</v>
@@ -4900,16 +4900,16 @@
         <v>1</v>
       </c>
       <c r="J82" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K82">
         <v>1800</v>
       </c>
       <c r="L82" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M82" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
@@ -4926,7 +4926,7 @@
         <v>22</v>
       </c>
       <c r="G83" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H83" s="2" t="s">
         <v>21</v>
@@ -4935,16 +4935,16 @@
         <v>1</v>
       </c>
       <c r="J83" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K83">
         <v>1800</v>
       </c>
       <c r="L83" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M83" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
@@ -4961,7 +4961,7 @@
         <v>22</v>
       </c>
       <c r="G84" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="H84" s="2" t="s">
         <v>21</v>
@@ -4970,16 +4970,16 @@
         <v>1</v>
       </c>
       <c r="J84" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="K84">
         <v>3000</v>
       </c>
       <c r="L84" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M84" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -5003,42 +5003,42 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="B1" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="C1" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="D1" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="E1" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="F1" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="B2" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="C2" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="D2" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="E2" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="F2" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -5068,48 +5068,48 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="B1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H1" t="s">
+        <v>205</v>
+      </c>
+      <c r="I1" t="s">
         <v>206</v>
       </c>
-      <c r="C1" t="s">
+      <c r="J1" t="s">
         <v>207</v>
       </c>
-      <c r="D1" t="s">
+      <c r="K1" t="s">
         <v>208</v>
       </c>
-      <c r="E1" t="s">
-        <v>212</v>
-      </c>
-      <c r="F1" t="s">
-        <v>214</v>
-      </c>
-      <c r="G1" t="s">
-        <v>215</v>
-      </c>
-      <c r="H1" t="s">
-        <v>218</v>
-      </c>
-      <c r="I1" t="s">
-        <v>219</v>
-      </c>
-      <c r="J1" t="s">
-        <v>220</v>
-      </c>
-      <c r="K1" t="s">
-        <v>221</v>
-      </c>
       <c r="L1" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="M1" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="B2">
         <v>7</v>
@@ -5121,13 +5121,13 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="F2" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="G2" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="H2" t="s">
         <v>6</v>
@@ -5142,10 +5142,10 @@
         <v>102</v>
       </c>
       <c r="L2" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="M2" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -5241,7 +5241,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>80</v>
@@ -5334,13 +5334,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="B3" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="C3" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -6181,10 +6181,10 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="I2" t="s">
-        <v>168</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -6196,7 +6196,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
@@ -6221,7 +6221,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>168</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -6233,8 +6233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6250,6 +6250,7 @@
     <col min="9" max="9" width="25.5703125" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="27.85546875" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="26.28515625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -6316,16 +6317,16 @@
         <v>102</v>
       </c>
       <c r="I2" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="J2" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="K2" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="L2" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -6354,16 +6355,16 @@
         <v>102</v>
       </c>
       <c r="I3" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="J3" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="K3" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="L3" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -6392,16 +6393,16 @@
         <v>102</v>
       </c>
       <c r="I4" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="J4" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="K4" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="L4" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -6430,16 +6431,16 @@
         <v>102</v>
       </c>
       <c r="I5" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="J5" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="K5" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="L5" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -6468,16 +6469,16 @@
         <v>102</v>
       </c>
       <c r="I6" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="J6" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="K6" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="L6" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -6506,16 +6507,16 @@
         <v>102</v>
       </c>
       <c r="I7" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="J7" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="K7" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="L7" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -6544,16 +6545,16 @@
         <v>102</v>
       </c>
       <c r="I8" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="J8" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="K8" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="L8" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -6561,10 +6562,10 @@
         <v>121</v>
       </c>
       <c r="B9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
         <v>122</v>
@@ -6582,16 +6583,16 @@
         <v>102</v>
       </c>
       <c r="I9" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="J9" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="K9" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="L9" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -6599,10 +6600,10 @@
         <v>124</v>
       </c>
       <c r="B10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
         <v>125</v>
@@ -6620,16 +6621,16 @@
         <v>102</v>
       </c>
       <c r="I10" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="J10" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="K10" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="L10" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -6637,10 +6638,10 @@
         <v>127</v>
       </c>
       <c r="B11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
         <v>128</v>
@@ -6658,16 +6659,16 @@
         <v>102</v>
       </c>
       <c r="I11" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="J11" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="K11" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="L11" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -6675,10 +6676,10 @@
         <v>130</v>
       </c>
       <c r="B12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
         <v>131</v>
@@ -6696,16 +6697,16 @@
         <v>102</v>
       </c>
       <c r="I12" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="J12" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="K12" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="L12" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -6713,10 +6714,10 @@
         <v>133</v>
       </c>
       <c r="B13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" t="s">
         <v>134</v>
@@ -6734,16 +6735,16 @@
         <v>102</v>
       </c>
       <c r="I13" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="J13" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="K13" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="L13" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -6751,10 +6752,10 @@
         <v>136</v>
       </c>
       <c r="B14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" t="s">
         <v>137</v>
@@ -6772,16 +6773,16 @@
         <v>102</v>
       </c>
       <c r="I14" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="J14" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="K14" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="L14" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -6789,10 +6790,10 @@
         <v>139</v>
       </c>
       <c r="B15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" t="s">
         <v>140</v>
@@ -6810,16 +6811,16 @@
         <v>102</v>
       </c>
       <c r="I15" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="J15" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="K15" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="L15" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -6827,10 +6828,10 @@
         <v>142</v>
       </c>
       <c r="B16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" t="s">
         <v>143</v>
@@ -6848,16 +6849,16 @@
         <v>102</v>
       </c>
       <c r="I16" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="J16" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="K16" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="L16" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -6865,10 +6866,10 @@
         <v>145</v>
       </c>
       <c r="B17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" t="s">
         <v>146</v>
@@ -6886,16 +6887,16 @@
         <v>102</v>
       </c>
       <c r="I17" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="J17" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="K17" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="L17" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -6903,10 +6904,10 @@
         <v>148</v>
       </c>
       <c r="B18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" t="s">
         <v>149</v>
@@ -6924,16 +6925,16 @@
         <v>102</v>
       </c>
       <c r="I18" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="J18" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="K18" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="L18" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -6941,10 +6942,10 @@
         <v>151</v>
       </c>
       <c r="B19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" t="s">
         <v>152</v>
@@ -6962,16 +6963,16 @@
         <v>102</v>
       </c>
       <c r="I19" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="J19" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="K19" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="L19" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -6979,10 +6980,10 @@
         <v>154</v>
       </c>
       <c r="B20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
         <v>155</v>
@@ -7000,16 +7001,16 @@
         <v>102</v>
       </c>
       <c r="I20" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="J20" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="K20" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="L20" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -7017,10 +7018,10 @@
         <v>157</v>
       </c>
       <c r="B21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" t="s">
         <v>158</v>
@@ -7038,16 +7039,16 @@
         <v>102</v>
       </c>
       <c r="I21" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="J21" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="K21" t="s">
-        <v>168</v>
+        <v>279</v>
       </c>
       <c r="L21" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -7078,18 +7079,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B2" t="s">
-        <v>314</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
       <c r="B3" t="s">
-        <v>315</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Password updated in the user details sheet
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
+++ b/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\auto\sahi_pro\userdata\scripts\Sahi_Project\svmx\test_lab\test_cases\optimax\op_excleData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11760" windowHeight="4650" firstSheet="15" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11760" windowHeight="4650"/>
   </bookViews>
   <sheets>
     <sheet name="User_Details" sheetId="1" r:id="rId1"/>
@@ -32,8 +27,9 @@
     <sheet name="RS_9547" sheetId="24" r:id="rId18"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:G13"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -535,9 +531,6 @@
     <t>govendhan@svmx-cct5.org.cct5part1</t>
   </si>
   <si>
-    <t>maxpl0re2</t>
-  </si>
-  <si>
     <t>AM load testing</t>
   </si>
   <si>
@@ -1049,13 +1042,15 @@
   </si>
   <si>
     <t>ONS_Policy_Wed Nov 08 2017 14:53:54 GMT+0530 (IST)</t>
+  </si>
+  <si>
+    <t>maxpl0re3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1436,15 +1431,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="34.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="26.5703125" collapsed="true"/>
+    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1463,7 +1456,7 @@
         <v>163</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>164</v>
+        <v>335</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -1485,7 +1478,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1498,18 +1491,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -1527,8 +1520,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1547,7 +1540,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -1556,12 +1549,12 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -1570,7 +1563,7 @@
         <v>162</v>
       </c>
       <c r="D3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -1589,7 +1582,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -1599,7 +1592,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -1617,21 +1610,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="27.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1" t="s">
         <v>169</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>170</v>
-      </c>
-      <c r="C1" t="s">
-        <v>171</v>
       </c>
       <c r="D1" t="s">
         <v>84</v>
@@ -1639,86 +1632,86 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D7" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -1737,25 +1730,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B1" t="s">
         <v>95</v>
       </c>
       <c r="C1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E1" t="s">
         <v>84</v>
@@ -1763,104 +1756,104 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D2">
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D3">
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D4">
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D5">
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D6">
         <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D7">
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -1878,18 +1871,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="45.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="36.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="30.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="25.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="45.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="36.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="30.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="19" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1930,7 +1923,7 @@
         <v>10</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -1953,7 +1946,7 @@
         <v>22</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>21</v>
@@ -1962,16 +1955,16 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K2">
         <v>2400</v>
       </c>
       <c r="L2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1994,7 +1987,7 @@
         <v>22</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>21</v>
@@ -2003,16 +1996,16 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K3">
         <v>3000</v>
       </c>
       <c r="L3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -2035,7 +2028,7 @@
         <v>22</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>21</v>
@@ -2044,16 +2037,16 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K4">
         <v>3000</v>
       </c>
       <c r="L4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -2073,7 +2066,7 @@
         <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>21</v>
@@ -2082,16 +2075,16 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K5">
         <v>1800</v>
       </c>
       <c r="L5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2111,7 +2104,7 @@
         <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>21</v>
@@ -2120,16 +2113,16 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K6">
         <v>1800</v>
       </c>
       <c r="L6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -2149,7 +2142,7 @@
         <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>21</v>
@@ -2158,16 +2151,16 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K7">
         <v>1800</v>
       </c>
       <c r="L7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -2187,7 +2180,7 @@
         <v>22</v>
       </c>
       <c r="G8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>21</v>
@@ -2196,16 +2189,16 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K8">
         <v>3000</v>
       </c>
       <c r="L8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -2225,7 +2218,7 @@
         <v>22</v>
       </c>
       <c r="G9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>21</v>
@@ -2234,16 +2227,16 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K9">
         <v>2400</v>
       </c>
       <c r="L9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -2263,7 +2256,7 @@
         <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>21</v>
@@ -2272,16 +2265,16 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K10">
         <v>2400</v>
       </c>
       <c r="L10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -2301,7 +2294,7 @@
         <v>22</v>
       </c>
       <c r="G11" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>21</v>
@@ -2310,16 +2303,16 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K11">
         <v>2400</v>
       </c>
       <c r="L11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M11" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -2339,7 +2332,7 @@
         <v>22</v>
       </c>
       <c r="G12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>21</v>
@@ -2348,16 +2341,16 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K12">
         <v>1800</v>
       </c>
       <c r="L12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -2377,7 +2370,7 @@
         <v>22</v>
       </c>
       <c r="G13" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>21</v>
@@ -2386,16 +2379,16 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K13">
         <v>2400</v>
       </c>
       <c r="L13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -2415,7 +2408,7 @@
         <v>22</v>
       </c>
       <c r="G14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>21</v>
@@ -2424,16 +2417,16 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K14">
         <v>2400</v>
       </c>
       <c r="L14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -2453,7 +2446,7 @@
         <v>22</v>
       </c>
       <c r="G15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>21</v>
@@ -2462,16 +2455,16 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K15">
         <v>2400</v>
       </c>
       <c r="L15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M15" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -2491,7 +2484,7 @@
         <v>22</v>
       </c>
       <c r="G16" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>21</v>
@@ -2500,16 +2493,16 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K16">
         <v>2400</v>
       </c>
       <c r="L16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M16" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -2529,7 +2522,7 @@
         <v>22</v>
       </c>
       <c r="G17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>21</v>
@@ -2538,16 +2531,16 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K17">
         <v>1800</v>
       </c>
       <c r="L17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -2567,7 +2560,7 @@
         <v>22</v>
       </c>
       <c r="G18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>21</v>
@@ -2576,16 +2569,16 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K18">
         <v>3000</v>
       </c>
       <c r="L18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M18" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -2605,7 +2598,7 @@
         <v>22</v>
       </c>
       <c r="G19" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>21</v>
@@ -2614,16 +2607,16 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K19">
         <v>2400</v>
       </c>
       <c r="L19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M19" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -2634,7 +2627,7 @@
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E20">
         <v>4400</v>
@@ -2643,7 +2636,7 @@
         <v>22</v>
       </c>
       <c r="G20" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>21</v>
@@ -2652,16 +2645,16 @@
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K20">
         <v>2400</v>
       </c>
       <c r="L20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M20" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -2672,7 +2665,7 @@
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E21">
         <v>9250</v>
@@ -2681,7 +2674,7 @@
         <v>22</v>
       </c>
       <c r="G21" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>21</v>
@@ -2690,16 +2683,16 @@
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K21">
         <v>2400</v>
       </c>
       <c r="L21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M21" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -2710,7 +2703,7 @@
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E22">
         <v>2610</v>
@@ -2719,7 +2712,7 @@
         <v>22</v>
       </c>
       <c r="G22" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>21</v>
@@ -2728,16 +2721,16 @@
         <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K22">
         <v>2400</v>
       </c>
       <c r="L22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M22" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -2748,7 +2741,7 @@
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E23">
         <v>1050</v>
@@ -2757,7 +2750,7 @@
         <v>22</v>
       </c>
       <c r="G23" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>21</v>
@@ -2766,16 +2759,16 @@
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K23">
         <v>1800</v>
       </c>
       <c r="L23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M23" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -2786,7 +2779,7 @@
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E24">
         <v>1200</v>
@@ -2795,7 +2788,7 @@
         <v>22</v>
       </c>
       <c r="G24" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>21</v>
@@ -2804,16 +2797,16 @@
         <v>1</v>
       </c>
       <c r="J24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K24">
         <v>3000</v>
       </c>
       <c r="L24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M24" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -2824,7 +2817,7 @@
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E25">
         <v>3300</v>
@@ -2833,7 +2826,7 @@
         <v>22</v>
       </c>
       <c r="G25" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>21</v>
@@ -2842,16 +2835,16 @@
         <v>1</v>
       </c>
       <c r="J25" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K25">
         <v>3000</v>
       </c>
       <c r="L25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M25" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -2862,7 +2855,7 @@
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E26">
         <v>9000</v>
@@ -2871,7 +2864,7 @@
         <v>22</v>
       </c>
       <c r="G26" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>21</v>
@@ -2880,16 +2873,16 @@
         <v>1</v>
       </c>
       <c r="J26" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K26">
         <v>3000</v>
       </c>
       <c r="L26" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M26" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -2900,7 +2893,7 @@
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E27">
         <v>9140</v>
@@ -2909,7 +2902,7 @@
         <v>22</v>
       </c>
       <c r="G27" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>21</v>
@@ -2918,16 +2911,16 @@
         <v>1</v>
       </c>
       <c r="J27" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K27">
         <v>2400</v>
       </c>
       <c r="L27" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M27" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -2938,7 +2931,7 @@
         <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E28">
         <v>9340</v>
@@ -2947,7 +2940,7 @@
         <v>22</v>
       </c>
       <c r="G28" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>21</v>
@@ -2956,16 +2949,16 @@
         <v>1</v>
       </c>
       <c r="J28" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K28">
         <v>2400</v>
       </c>
       <c r="L28" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M28" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -2976,7 +2969,7 @@
         <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E29">
         <v>8540</v>
@@ -2985,7 +2978,7 @@
         <v>22</v>
       </c>
       <c r="G29" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>21</v>
@@ -2994,16 +2987,16 @@
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K29">
         <v>1800</v>
       </c>
       <c r="L29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M29" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -3014,7 +3007,7 @@
         <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E30">
         <v>8620</v>
@@ -3023,7 +3016,7 @@
         <v>22</v>
       </c>
       <c r="G30" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>21</v>
@@ -3032,16 +3025,16 @@
         <v>1</v>
       </c>
       <c r="J30" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K30">
         <v>3000</v>
       </c>
       <c r="L30" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M30" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -3052,7 +3045,7 @@
         <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E31">
         <v>8430</v>
@@ -3061,7 +3054,7 @@
         <v>22</v>
       </c>
       <c r="G31" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>21</v>
@@ -3070,16 +3063,16 @@
         <v>1</v>
       </c>
       <c r="J31" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K31">
         <v>1800</v>
       </c>
       <c r="L31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M31" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -3090,7 +3083,7 @@
         <v>8</v>
       </c>
       <c r="C32" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E32">
         <v>2920</v>
@@ -3099,7 +3092,7 @@
         <v>22</v>
       </c>
       <c r="G32" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>21</v>
@@ -3108,16 +3101,16 @@
         <v>1</v>
       </c>
       <c r="J32" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K32">
         <v>1800</v>
       </c>
       <c r="L32" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M32" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -3128,7 +3121,7 @@
         <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E33">
         <v>5500</v>
@@ -3137,7 +3130,7 @@
         <v>22</v>
       </c>
       <c r="G33" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>21</v>
@@ -3146,16 +3139,16 @@
         <v>1</v>
       </c>
       <c r="J33" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K33">
         <v>3000</v>
       </c>
       <c r="L33" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M33" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -3166,7 +3159,7 @@
         <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E34">
         <v>2000</v>
@@ -3175,7 +3168,7 @@
         <v>22</v>
       </c>
       <c r="G34" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>21</v>
@@ -3184,16 +3177,16 @@
         <v>1</v>
       </c>
       <c r="J34" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K34">
         <v>2400</v>
       </c>
       <c r="L34" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M34" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -3204,7 +3197,7 @@
         <v>8</v>
       </c>
       <c r="C35" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E35">
         <v>1348</v>
@@ -3213,7 +3206,7 @@
         <v>22</v>
       </c>
       <c r="G35" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>21</v>
@@ -3222,16 +3215,16 @@
         <v>1</v>
       </c>
       <c r="J35" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K35">
         <v>3000</v>
       </c>
       <c r="L35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M35" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -3242,7 +3235,7 @@
         <v>8</v>
       </c>
       <c r="C36" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E36">
         <v>8400</v>
@@ -3251,7 +3244,7 @@
         <v>22</v>
       </c>
       <c r="G36" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>21</v>
@@ -3260,16 +3253,16 @@
         <v>1</v>
       </c>
       <c r="J36" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K36">
         <v>2400</v>
       </c>
       <c r="L36" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M36" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -3280,7 +3273,7 @@
         <v>8</v>
       </c>
       <c r="C37" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E37">
         <v>1348</v>
@@ -3289,7 +3282,7 @@
         <v>22</v>
       </c>
       <c r="G37" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>21</v>
@@ -3298,16 +3291,16 @@
         <v>1</v>
       </c>
       <c r="J37" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K37">
         <v>2400</v>
       </c>
       <c r="L37" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M37" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -3318,7 +3311,7 @@
         <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E38">
         <v>7130</v>
@@ -3327,7 +3320,7 @@
         <v>22</v>
       </c>
       <c r="G38" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>21</v>
@@ -3336,16 +3329,16 @@
         <v>1</v>
       </c>
       <c r="J38" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K38">
         <v>2400</v>
       </c>
       <c r="L38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M38" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -3356,7 +3349,7 @@
         <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E39">
         <v>1140</v>
@@ -3365,7 +3358,7 @@
         <v>22</v>
       </c>
       <c r="G39" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>21</v>
@@ -3374,16 +3367,16 @@
         <v>1</v>
       </c>
       <c r="J39" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K39">
         <v>3000</v>
       </c>
       <c r="L39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M39" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -3394,7 +3387,7 @@
         <v>8</v>
       </c>
       <c r="C40" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E40">
         <v>2840</v>
@@ -3403,7 +3396,7 @@
         <v>22</v>
       </c>
       <c r="G40" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>21</v>
@@ -3412,16 +3405,16 @@
         <v>1</v>
       </c>
       <c r="J40" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K40">
         <v>3000</v>
       </c>
       <c r="L40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M40" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -3432,7 +3425,7 @@
         <v>8</v>
       </c>
       <c r="C41" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E41">
         <v>1348</v>
@@ -3441,7 +3434,7 @@
         <v>22</v>
       </c>
       <c r="G41" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>21</v>
@@ -3450,16 +3443,16 @@
         <v>1</v>
       </c>
       <c r="J41" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K41">
         <v>3000</v>
       </c>
       <c r="L41" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M41" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
@@ -3470,7 +3463,7 @@
         <v>8</v>
       </c>
       <c r="C42" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E42">
         <v>2550</v>
@@ -3479,7 +3472,7 @@
         <v>22</v>
       </c>
       <c r="G42" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>21</v>
@@ -3488,16 +3481,16 @@
         <v>1</v>
       </c>
       <c r="J42" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K42">
         <v>1800</v>
       </c>
       <c r="L42" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M42" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -3508,7 +3501,7 @@
         <v>8</v>
       </c>
       <c r="C43" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E43">
         <v>4000</v>
@@ -3517,7 +3510,7 @@
         <v>22</v>
       </c>
       <c r="G43" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>21</v>
@@ -3526,16 +3519,16 @@
         <v>1</v>
       </c>
       <c r="J43" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K43">
         <v>1800</v>
       </c>
       <c r="L43" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M43" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -3546,7 +3539,7 @@
         <v>8</v>
       </c>
       <c r="C44" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E44">
         <v>2570</v>
@@ -3555,7 +3548,7 @@
         <v>22</v>
       </c>
       <c r="G44" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>21</v>
@@ -3564,16 +3557,16 @@
         <v>1</v>
       </c>
       <c r="J44" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K44">
         <v>2400</v>
       </c>
       <c r="L44" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M44" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
@@ -3584,7 +3577,7 @@
         <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E45">
         <v>1082</v>
@@ -3593,7 +3586,7 @@
         <v>22</v>
       </c>
       <c r="G45" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>21</v>
@@ -3602,16 +3595,16 @@
         <v>1</v>
       </c>
       <c r="J45" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K45">
         <v>2280</v>
       </c>
       <c r="L45" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M45" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
@@ -3622,7 +3615,7 @@
         <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E46">
         <v>2800</v>
@@ -3631,7 +3624,7 @@
         <v>22</v>
       </c>
       <c r="G46" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>21</v>
@@ -3640,16 +3633,16 @@
         <v>1</v>
       </c>
       <c r="J46" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K46">
         <v>2400</v>
       </c>
       <c r="L46" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M46" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -3660,7 +3653,7 @@
         <v>8</v>
       </c>
       <c r="C47" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E47">
         <v>5300</v>
@@ -3669,7 +3662,7 @@
         <v>22</v>
       </c>
       <c r="G47" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H47" s="2" t="s">
         <v>21</v>
@@ -3678,16 +3671,16 @@
         <v>1</v>
       </c>
       <c r="J47" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K47">
         <v>2400</v>
       </c>
       <c r="L47" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M47" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
@@ -3698,7 +3691,7 @@
         <v>8</v>
       </c>
       <c r="C48" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E48">
         <v>3500</v>
@@ -3707,7 +3700,7 @@
         <v>22</v>
       </c>
       <c r="G48" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H48" s="2" t="s">
         <v>21</v>
@@ -3716,16 +3709,16 @@
         <v>1</v>
       </c>
       <c r="J48" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K48">
         <v>2400</v>
       </c>
       <c r="L48" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M48" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
@@ -3736,7 +3729,7 @@
         <v>8</v>
       </c>
       <c r="C49" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E49">
         <v>5380</v>
@@ -3745,7 +3738,7 @@
         <v>22</v>
       </c>
       <c r="G49" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H49" s="2" t="s">
         <v>21</v>
@@ -3754,16 +3747,16 @@
         <v>1</v>
       </c>
       <c r="J49" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K49">
         <v>1800</v>
       </c>
       <c r="L49" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M49" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
@@ -3774,7 +3767,7 @@
         <v>8</v>
       </c>
       <c r="C50" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E50">
         <v>2570</v>
@@ -3783,7 +3776,7 @@
         <v>22</v>
       </c>
       <c r="G50" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H50" s="2" t="s">
         <v>21</v>
@@ -3792,16 +3785,16 @@
         <v>1</v>
       </c>
       <c r="J50" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K50">
         <v>1800</v>
       </c>
       <c r="L50" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M50" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
@@ -3812,7 +3805,7 @@
         <v>8</v>
       </c>
       <c r="C51" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E51">
         <v>1982</v>
@@ -3821,7 +3814,7 @@
         <v>22</v>
       </c>
       <c r="G51" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H51" s="2" t="s">
         <v>21</v>
@@ -3830,16 +3823,16 @@
         <v>1</v>
       </c>
       <c r="J51" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K51">
         <v>1800</v>
       </c>
       <c r="L51" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M51" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
@@ -3850,7 +3843,7 @@
         <v>8</v>
       </c>
       <c r="C52" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E52">
         <v>6800</v>
@@ -3859,7 +3852,7 @@
         <v>22</v>
       </c>
       <c r="G52" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H52" s="2" t="s">
         <v>21</v>
@@ -3868,16 +3861,16 @@
         <v>1</v>
       </c>
       <c r="J52" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K52">
         <v>2400</v>
       </c>
       <c r="L52" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M52" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
@@ -3888,7 +3881,7 @@
         <v>8</v>
       </c>
       <c r="C53" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E53">
         <v>8400</v>
@@ -3897,7 +3890,7 @@
         <v>22</v>
       </c>
       <c r="G53" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H53" s="2" t="s">
         <v>21</v>
@@ -3906,16 +3899,16 @@
         <v>1</v>
       </c>
       <c r="J53" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K53">
         <v>2400</v>
       </c>
       <c r="L53" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M53" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
@@ -3926,7 +3919,7 @@
         <v>8</v>
       </c>
       <c r="C54" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E54">
         <v>4500</v>
@@ -3935,7 +3928,7 @@
         <v>22</v>
       </c>
       <c r="G54" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H54" s="2" t="s">
         <v>21</v>
@@ -3944,16 +3937,16 @@
         <v>1</v>
       </c>
       <c r="J54" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K54">
         <v>3000</v>
       </c>
       <c r="L54" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M54" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
@@ -3964,7 +3957,7 @@
         <v>8</v>
       </c>
       <c r="C55" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E55">
         <v>1348</v>
@@ -3973,7 +3966,7 @@
         <v>22</v>
       </c>
       <c r="G55" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>21</v>
@@ -3982,16 +3975,16 @@
         <v>1</v>
       </c>
       <c r="J55" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K55">
         <v>4920</v>
       </c>
       <c r="L55" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M55" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
@@ -4002,7 +3995,7 @@
         <v>8</v>
       </c>
       <c r="C56" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E56">
         <v>7130</v>
@@ -4011,7 +4004,7 @@
         <v>22</v>
       </c>
       <c r="G56" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H56" s="2" t="s">
         <v>21</v>
@@ -4020,16 +4013,16 @@
         <v>1</v>
       </c>
       <c r="J56" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K56">
         <v>2400</v>
       </c>
       <c r="L56" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M56" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
@@ -4040,7 +4033,7 @@
         <v>8</v>
       </c>
       <c r="C57" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E57">
         <v>1348</v>
@@ -4049,7 +4042,7 @@
         <v>22</v>
       </c>
       <c r="G57" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H57" s="2" t="s">
         <v>21</v>
@@ -4058,16 +4051,16 @@
         <v>1</v>
       </c>
       <c r="J57" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K57">
         <v>2400</v>
       </c>
       <c r="L57" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M57" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -4078,7 +4071,7 @@
         <v>8</v>
       </c>
       <c r="C58" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E58">
         <v>3500</v>
@@ -4087,7 +4080,7 @@
         <v>22</v>
       </c>
       <c r="G58" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>21</v>
@@ -4096,16 +4089,16 @@
         <v>1</v>
       </c>
       <c r="J58" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K58">
         <v>2400</v>
       </c>
       <c r="L58" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M58" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
@@ -4116,7 +4109,7 @@
         <v>8</v>
       </c>
       <c r="C59" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E59">
         <v>2000</v>
@@ -4125,7 +4118,7 @@
         <v>22</v>
       </c>
       <c r="G59" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>21</v>
@@ -4134,16 +4127,16 @@
         <v>1</v>
       </c>
       <c r="J59" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K59">
         <v>2400</v>
       </c>
       <c r="L59" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M59" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
@@ -4154,7 +4147,7 @@
         <v>8</v>
       </c>
       <c r="C60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E60">
         <v>8400</v>
@@ -4163,7 +4156,7 @@
         <v>22</v>
       </c>
       <c r="G60" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H60" s="2" t="s">
         <v>21</v>
@@ -4172,16 +4165,16 @@
         <v>1</v>
       </c>
       <c r="J60" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K60">
         <v>2280</v>
       </c>
       <c r="L60" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M60" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
@@ -4192,7 +4185,7 @@
         <v>8</v>
       </c>
       <c r="C61" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E61">
         <v>2060</v>
@@ -4201,7 +4194,7 @@
         <v>22</v>
       </c>
       <c r="G61" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H61" s="2" t="s">
         <v>21</v>
@@ -4210,16 +4203,16 @@
         <v>1</v>
       </c>
       <c r="J61" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K61">
         <v>1800</v>
       </c>
       <c r="L61" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M61" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
@@ -4230,7 +4223,7 @@
         <v>8</v>
       </c>
       <c r="C62" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E62">
         <v>2640</v>
@@ -4239,7 +4232,7 @@
         <v>22</v>
       </c>
       <c r="G62" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H62" s="2" t="s">
         <v>21</v>
@@ -4248,16 +4241,16 @@
         <v>1</v>
       </c>
       <c r="J62" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K62">
         <v>3360</v>
       </c>
       <c r="L62" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M62" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
@@ -4268,7 +4261,7 @@
         <v>8</v>
       </c>
       <c r="C63" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E63">
         <v>3511</v>
@@ -4277,7 +4270,7 @@
         <v>22</v>
       </c>
       <c r="G63" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H63" s="2" t="s">
         <v>21</v>
@@ -4286,16 +4279,16 @@
         <v>1</v>
       </c>
       <c r="J63" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K63">
         <v>2400</v>
       </c>
       <c r="L63" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M63" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
@@ -4306,7 +4299,7 @@
         <v>8</v>
       </c>
       <c r="C64" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E64">
         <v>8400</v>
@@ -4315,7 +4308,7 @@
         <v>22</v>
       </c>
       <c r="G64" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H64" s="2" t="s">
         <v>21</v>
@@ -4324,16 +4317,16 @@
         <v>1</v>
       </c>
       <c r="J64" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K64">
         <v>2400</v>
       </c>
       <c r="L64" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M64" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
@@ -4344,7 +4337,7 @@
         <v>8</v>
       </c>
       <c r="C65" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E65">
         <v>3511</v>
@@ -4353,7 +4346,7 @@
         <v>22</v>
       </c>
       <c r="G65" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H65" s="2" t="s">
         <v>21</v>
@@ -4362,16 +4355,16 @@
         <v>1</v>
       </c>
       <c r="J65" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K65">
         <v>2400</v>
       </c>
       <c r="L65" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M65" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
@@ -4382,7 +4375,7 @@
         <v>8</v>
       </c>
       <c r="C66" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E66">
         <v>1800</v>
@@ -4391,7 +4384,7 @@
         <v>22</v>
       </c>
       <c r="G66" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H66" s="2" t="s">
         <v>21</v>
@@ -4400,16 +4393,16 @@
         <v>1</v>
       </c>
       <c r="J66" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K66">
         <v>2400</v>
       </c>
       <c r="L66" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M66" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
@@ -4420,7 +4413,7 @@
         <v>8</v>
       </c>
       <c r="C67" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E67">
         <v>2500</v>
@@ -4429,7 +4422,7 @@
         <v>22</v>
       </c>
       <c r="G67" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H67" s="2" t="s">
         <v>21</v>
@@ -4438,16 +4431,16 @@
         <v>1</v>
       </c>
       <c r="J67" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K67">
         <v>1800</v>
       </c>
       <c r="L67" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M67" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
@@ -4458,7 +4451,7 @@
         <v>8</v>
       </c>
       <c r="C68" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E68">
         <v>2840</v>
@@ -4467,7 +4460,7 @@
         <v>22</v>
       </c>
       <c r="G68" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H68" s="2" t="s">
         <v>21</v>
@@ -4476,16 +4469,16 @@
         <v>1</v>
       </c>
       <c r="J68" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K68">
         <v>2400</v>
       </c>
       <c r="L68" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M68" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
@@ -4496,7 +4489,7 @@
         <v>8</v>
       </c>
       <c r="C69" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E69">
         <v>2660</v>
@@ -4505,7 +4498,7 @@
         <v>22</v>
       </c>
       <c r="G69" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H69" s="2" t="s">
         <v>21</v>
@@ -4514,16 +4507,16 @@
         <v>1</v>
       </c>
       <c r="J69" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K69">
         <v>2280</v>
       </c>
       <c r="L69" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M69" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
@@ -4534,7 +4527,7 @@
         <v>8</v>
       </c>
       <c r="C70" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E70">
         <v>4681</v>
@@ -4543,7 +4536,7 @@
         <v>22</v>
       </c>
       <c r="G70" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H70" s="2" t="s">
         <v>21</v>
@@ -4552,16 +4545,16 @@
         <v>1</v>
       </c>
       <c r="J70" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K70">
         <v>1800</v>
       </c>
       <c r="L70" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M70" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
@@ -4572,7 +4565,7 @@
         <v>8</v>
       </c>
       <c r="C71" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E71">
         <v>5350</v>
@@ -4581,7 +4574,7 @@
         <v>22</v>
       </c>
       <c r="G71" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H71" s="2" t="s">
         <v>21</v>
@@ -4590,16 +4583,16 @@
         <v>1</v>
       </c>
       <c r="J71" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K71">
         <v>1800</v>
       </c>
       <c r="L71" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M71" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
@@ -4610,7 +4603,7 @@
         <v>8</v>
       </c>
       <c r="C72" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E72">
         <v>3500</v>
@@ -4619,7 +4612,7 @@
         <v>22</v>
       </c>
       <c r="G72" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H72" s="2" t="s">
         <v>21</v>
@@ -4628,16 +4621,16 @@
         <v>1</v>
       </c>
       <c r="J72" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K72">
         <v>1800</v>
       </c>
       <c r="L72" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M72" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
@@ -4648,7 +4641,7 @@
         <v>8</v>
       </c>
       <c r="C73" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E73">
         <v>2600</v>
@@ -4657,7 +4650,7 @@
         <v>22</v>
       </c>
       <c r="G73" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H73" s="2" t="s">
         <v>21</v>
@@ -4666,16 +4659,16 @@
         <v>1</v>
       </c>
       <c r="J73" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K73">
         <v>2400</v>
       </c>
       <c r="L73" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M73" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
@@ -4686,7 +4679,7 @@
         <v>8</v>
       </c>
       <c r="C74" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E74">
         <v>9150</v>
@@ -4695,7 +4688,7 @@
         <v>22</v>
       </c>
       <c r="G74" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H74" s="2" t="s">
         <v>21</v>
@@ -4704,16 +4697,16 @@
         <v>1</v>
       </c>
       <c r="J74" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K74">
         <v>1800</v>
       </c>
       <c r="L74" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M74" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
@@ -4724,7 +4717,7 @@
         <v>8</v>
       </c>
       <c r="C75" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E75">
         <v>1800</v>
@@ -4733,7 +4726,7 @@
         <v>22</v>
       </c>
       <c r="G75" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H75" s="2" t="s">
         <v>21</v>
@@ -4742,16 +4735,16 @@
         <v>1</v>
       </c>
       <c r="J75" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K75">
         <v>2400</v>
       </c>
       <c r="L75" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M75" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
@@ -4762,7 +4755,7 @@
         <v>8</v>
       </c>
       <c r="C76" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E76">
         <v>1348</v>
@@ -4771,7 +4764,7 @@
         <v>22</v>
       </c>
       <c r="G76" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H76" s="2" t="s">
         <v>21</v>
@@ -4780,16 +4773,16 @@
         <v>1</v>
       </c>
       <c r="J76" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K76">
         <v>1800</v>
       </c>
       <c r="L76" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M76" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
@@ -4800,7 +4793,7 @@
         <v>8</v>
       </c>
       <c r="C77" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E77">
         <v>7130</v>
@@ -4809,7 +4802,7 @@
         <v>22</v>
       </c>
       <c r="G77" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H77" s="2" t="s">
         <v>21</v>
@@ -4818,16 +4811,16 @@
         <v>1</v>
       </c>
       <c r="J77" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K77">
         <v>1800</v>
       </c>
       <c r="L77" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M77" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
@@ -4838,7 +4831,7 @@
         <v>8</v>
       </c>
       <c r="C78" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E78">
         <v>1020</v>
@@ -4847,7 +4840,7 @@
         <v>22</v>
       </c>
       <c r="G78" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H78" s="2" t="s">
         <v>21</v>
@@ -4856,16 +4849,16 @@
         <v>1</v>
       </c>
       <c r="J78" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K78">
         <v>1800</v>
       </c>
       <c r="L78" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M78" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
@@ -4876,7 +4869,7 @@
         <v>8</v>
       </c>
       <c r="C79" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E79">
         <v>7100</v>
@@ -4885,7 +4878,7 @@
         <v>22</v>
       </c>
       <c r="G79" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>21</v>
@@ -4894,16 +4887,16 @@
         <v>1</v>
       </c>
       <c r="J79" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K79">
         <v>1800</v>
       </c>
       <c r="L79" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M79" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
@@ -4914,7 +4907,7 @@
         <v>8</v>
       </c>
       <c r="C80" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E80">
         <v>2845</v>
@@ -4923,7 +4916,7 @@
         <v>22</v>
       </c>
       <c r="G80" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H80" s="2" t="s">
         <v>21</v>
@@ -4932,16 +4925,16 @@
         <v>1</v>
       </c>
       <c r="J80" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K80">
         <v>1800</v>
       </c>
       <c r="L80" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M80" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
@@ -4952,7 +4945,7 @@
         <v>8</v>
       </c>
       <c r="C81" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E81">
         <v>5523</v>
@@ -4961,7 +4954,7 @@
         <v>22</v>
       </c>
       <c r="G81" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H81" s="2" t="s">
         <v>21</v>
@@ -4970,16 +4963,16 @@
         <v>1</v>
       </c>
       <c r="J81" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K81">
         <v>3000</v>
       </c>
       <c r="L81" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M81" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
@@ -4996,7 +4989,7 @@
         <v>22</v>
       </c>
       <c r="G82" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H82" s="2" t="s">
         <v>21</v>
@@ -5005,16 +4998,16 @@
         <v>1</v>
       </c>
       <c r="J82" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K82">
         <v>1800</v>
       </c>
       <c r="L82" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M82" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
@@ -5031,7 +5024,7 @@
         <v>22</v>
       </c>
       <c r="G83" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H83" s="2" t="s">
         <v>21</v>
@@ -5040,16 +5033,16 @@
         <v>1</v>
       </c>
       <c r="J83" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K83">
         <v>1800</v>
       </c>
       <c r="L83" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M83" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
@@ -5066,7 +5059,7 @@
         <v>22</v>
       </c>
       <c r="G84" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H84" s="2" t="s">
         <v>21</v>
@@ -5075,16 +5068,16 @@
         <v>1</v>
       </c>
       <c r="J84" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K84">
         <v>3000</v>
       </c>
       <c r="L84" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M84" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -5100,50 +5093,50 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="55.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="62.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="4" max="4" width="55.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="62.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B1" t="s">
         <v>180</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>181</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>182</v>
       </c>
-      <c r="D1" t="s">
-        <v>183</v>
-      </c>
       <c r="E1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F1" t="s">
         <v>188</v>
-      </c>
-      <c r="F1" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B2" t="s">
         <v>184</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>185</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>186</v>
       </c>
-      <c r="D2" t="s">
-        <v>187</v>
-      </c>
       <c r="E2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -5161,60 +5154,60 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C1" t="s">
         <v>193</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>194</v>
       </c>
-      <c r="D1" t="s">
-        <v>195</v>
-      </c>
       <c r="E1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G1" t="s">
         <v>201</v>
       </c>
-      <c r="G1" t="s">
-        <v>202</v>
-      </c>
       <c r="H1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I1" t="s">
         <v>205</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>206</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>207</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>208</v>
       </c>
-      <c r="L1" t="s">
-        <v>209</v>
-      </c>
       <c r="M1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B2">
         <v>7</v>
@@ -5226,13 +5219,13 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F2" t="s">
+        <v>202</v>
+      </c>
+      <c r="G2" t="s">
         <v>203</v>
-      </c>
-      <c r="G2" t="s">
-        <v>204</v>
       </c>
       <c r="H2" t="s">
         <v>6</v>
@@ -5247,10 +5240,10 @@
         <v>102</v>
       </c>
       <c r="L2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="M2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -5262,14 +5255,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" bestFit="true" customWidth="true" width="34.140625" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="35.7109375" collapsed="false"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="35.42578125" collapsed="false"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="36.140625" collapsed="false"/>
+    <col min="2" max="3" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -5277,69 +5270,69 @@
         <v>68</v>
       </c>
       <c r="B1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C1" t="s">
         <v>321</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" t="s">
         <v>323</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>324</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>325</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>326</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>327</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>328</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>329</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" t="s">
         <v>331</v>
       </c>
-      <c r="M1" t="s">
-        <v>332</v>
-      </c>
       <c r="N1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C2" t="s">
         <v>333</v>
       </c>
-      <c r="C2" t="s">
-        <v>334</v>
-      </c>
       <c r="D2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I2">
         <v>4</v>
@@ -5354,10 +5347,10 @@
         <v>0</v>
       </c>
       <c r="M2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="N2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -5376,24 +5369,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -5454,7 +5447,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>80</v>
@@ -5518,9 +5511,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="96.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="1" max="1" width="96" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -5536,10 +5529,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" t="s">
         <v>165</v>
-      </c>
-      <c r="B2" t="s">
-        <v>166</v>
       </c>
       <c r="C2" t="s">
         <v>59</v>
@@ -5547,13 +5540,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" t="s">
         <v>196</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>197</v>
-      </c>
-      <c r="C3" t="s">
-        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -5572,8 +5565,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -5632,11 +5625,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="23.0" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.140625" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.42578125" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.0" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="19.42578125" collapsed="false"/>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -5653,7 +5646,7 @@
         <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -5670,7 +5663,7 @@
         <v>8870</v>
       </c>
       <c r="E2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -5687,7 +5680,7 @@
         <v>8870</v>
       </c>
       <c r="E3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -5704,7 +5697,7 @@
         <v>8870</v>
       </c>
       <c r="E4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -5736,13 +5729,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="2" max="4" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="1" max="1" width="23" customWidth="1" collapsed="1"/>
+    <col min="2" max="4" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="34.42578125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="30.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -6438,10 +6431,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="35.140625" collapsed="true"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="35.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -6496,10 +6489,10 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -6536,7 +6529,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -6554,18 +6547,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="29.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="60.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="25.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="27.85546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="26.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="22.0" collapsed="false"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="60.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="25.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="27.85546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="26.28515625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -6632,16 +6625,16 @@
         <v>102</v>
       </c>
       <c r="I2" t="s">
+        <v>280</v>
+      </c>
+      <c r="J2" t="s">
+        <v>279</v>
+      </c>
+      <c r="K2" t="s">
+        <v>278</v>
+      </c>
+      <c r="L2" t="s">
         <v>281</v>
-      </c>
-      <c r="J2" t="s">
-        <v>280</v>
-      </c>
-      <c r="K2" t="s">
-        <v>279</v>
-      </c>
-      <c r="L2" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -6670,16 +6663,16 @@
         <v>102</v>
       </c>
       <c r="I3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -6708,16 +6701,16 @@
         <v>102</v>
       </c>
       <c r="I4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -6746,16 +6739,16 @@
         <v>102</v>
       </c>
       <c r="I5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -6784,16 +6777,16 @@
         <v>102</v>
       </c>
       <c r="I6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -6822,16 +6815,16 @@
         <v>102</v>
       </c>
       <c r="I7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -6860,16 +6853,16 @@
         <v>102</v>
       </c>
       <c r="I8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -6898,16 +6891,16 @@
         <v>102</v>
       </c>
       <c r="I9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -6936,16 +6929,16 @@
         <v>102</v>
       </c>
       <c r="I10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -6974,16 +6967,16 @@
         <v>102</v>
       </c>
       <c r="I11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J11" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L11" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -7012,16 +7005,16 @@
         <v>102</v>
       </c>
       <c r="I12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -7050,16 +7043,16 @@
         <v>102</v>
       </c>
       <c r="I13" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J13" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L13" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -7088,16 +7081,16 @@
         <v>102</v>
       </c>
       <c r="I14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -7126,16 +7119,16 @@
         <v>102</v>
       </c>
       <c r="I15" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K15" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L15" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -7164,16 +7157,16 @@
         <v>102</v>
       </c>
       <c r="I16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J16" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K16" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L16" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -7202,16 +7195,16 @@
         <v>102</v>
       </c>
       <c r="I17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K17" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L17" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -7240,16 +7233,16 @@
         <v>102</v>
       </c>
       <c r="I18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -7278,16 +7271,16 @@
         <v>102</v>
       </c>
       <c r="I19" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J19" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K19" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L19" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -7316,16 +7309,16 @@
         <v>102</v>
       </c>
       <c r="I20" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J20" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K20" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L20" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -7354,16 +7347,16 @@
         <v>102</v>
       </c>
       <c r="I21" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J21" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K21" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L21" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
automation excel sheet updated
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
+++ b/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
@@ -29,7 +29,7 @@
   <calcPr calcId="0"/>
   <oleSize ref="A1:D13"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -1026,19 +1026,20 @@
     <t>EventID</t>
   </si>
   <si>
-    <t>00U3B000001VIRSUA4</t>
-  </si>
-  <si>
     <t>2017-11-24T07:00:00.000Z</t>
   </si>
   <si>
     <t>2017-11-243T08:00:00.000Z</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1425,9 +1426,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="26.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1471,7 +1472,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1513,8 +1514,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1575,7 +1576,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -1603,10 +1604,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1723,11 +1724,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1864,18 +1865,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="45.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="36.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="30.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="45.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="36.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -5086,10 +5087,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="55.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="62.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="55.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="62.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -5147,15 +5148,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -5255,16 +5256,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="47.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="47.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.85546875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -5289,16 +5290,16 @@
         <v>325</v>
       </c>
       <c r="B2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C2" t="s">
         <v>330</v>
-      </c>
-      <c r="C2" t="s">
-        <v>331</v>
       </c>
       <c r="D2" t="s">
         <v>327</v>
       </c>
       <c r="E2" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -5316,24 +5317,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -5458,9 +5459,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="96" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="96.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -5512,8 +5513,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -5572,11 +5573,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -5676,13 +5677,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" customWidth="1" collapsed="1"/>
-    <col min="2" max="4" width="24.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="34.42578125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="30.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="2" max="4" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="30.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -6378,10 +6379,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="35.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="35.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -6494,18 +6495,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="60.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="25.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="27.85546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="26.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="29.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="60.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
RTO dispatch process updated
RTO dispatch process updated
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
+++ b/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="5640"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="5640" firstSheet="13" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="User_Details" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1332" uniqueCount="322">
   <si>
     <t>UserName</t>
   </si>
@@ -1000,6 +1000,12 @@
   </si>
   <si>
     <t>servicemax1</t>
+  </si>
+  <si>
+    <t>Service Team</t>
+  </si>
+  <si>
+    <t>a1y3B000000HhoA</t>
   </si>
 </sst>
 </file>
@@ -1386,7 +1392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -5103,10 +5109,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5121,7 +5127,7 @@
     <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>189</v>
       </c>
@@ -5161,8 +5167,11 @@
       <c r="M1" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>190</v>
       </c>
@@ -5201,6 +5210,9 @@
       </c>
       <c r="M2" t="s">
         <v>210</v>
+      </c>
+      <c r="N2" t="s">
+        <v>321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RTO with SLA,Preferred Tech and PST,PET
RTO with SLA,Preferred Tech and PST,PET
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
+++ b/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="368">
   <si>
     <t>UserName</t>
   </si>
@@ -1143,6 +1143,12 @@
   </si>
   <si>
     <t>2017-12-07T07:04:00.000Z</t>
+  </si>
+  <si>
+    <t>Preferred Technician</t>
+  </si>
+  <si>
+    <t>a1u3B000000MMMSQA4</t>
   </si>
 </sst>
 </file>
@@ -6935,10 +6941,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6956,7 +6962,7 @@
     <col min="16" max="16" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>185</v>
       </c>
@@ -7011,8 +7017,11 @@
       <c r="R1" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>186</v>
       </c>
@@ -7066,6 +7075,9 @@
       </c>
       <c r="R2" t="s">
         <v>365</v>
+      </c>
+      <c r="S2" t="s">
+        <v>367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated datacreation tc to create appointment type and windows
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
+++ b/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\auto\sahi_pro\userdata\scripts\Sahi_Project\svmx\test_lab\test_cases\optimax\op_excleData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11760" windowHeight="4650" firstSheet="19" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11760" windowHeight="4815" firstSheet="22" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="User_Details" sheetId="1" r:id="rId1"/>
@@ -34,10 +29,13 @@
     <sheet name="Rules" sheetId="21" r:id="rId20"/>
     <sheet name="RTO_DispatchProcess" sheetId="22" r:id="rId21"/>
     <sheet name="TestAppts" sheetId="28" r:id="rId22"/>
+    <sheet name="AppointmentType" sheetId="30" r:id="rId23"/>
+    <sheet name="AppointmentWindow" sheetId="31" r:id="rId24"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:J14"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -45,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="387">
   <si>
     <t>UserName</t>
   </si>
@@ -1149,12 +1147,70 @@
   </si>
   <si>
     <t>a1u3B000000MMMSQA4</t>
+  </si>
+  <si>
+    <t>Appointment Type Name</t>
+  </si>
+  <si>
+    <t>Appointment Type Id</t>
+  </si>
+  <si>
+    <t>Time Window</t>
+  </si>
+  <si>
+    <t>AutoType</t>
+  </si>
+  <si>
+    <t>AutoMorning</t>
+  </si>
+  <si>
+    <t>AutoAfternoon</t>
+  </si>
+  <si>
+    <t>AutoEvening</t>
+  </si>
+  <si>
+    <t>a183B000000fmeOQAQ</t>
+  </si>
+  <si>
+    <t>a183B000000fn96QAA</t>
+  </si>
+  <si>
+    <t>a183B000000fn97QAA</t>
+  </si>
+  <si>
+    <t>a183B000000fn98QAA</t>
+  </si>
+  <si>
+    <t>a183B000000fn9kQAA</t>
+  </si>
+  <si>
+    <t>a183B000000fn9pQAA</t>
+  </si>
+  <si>
+    <t>a183B000000fn9qQAA</t>
+  </si>
+  <si>
+    <t>a183B000000fn9rQAA</t>
+  </si>
+  <si>
+    <t>a183B000000fn9zQAA</t>
+  </si>
+  <si>
+    <t>a183B000000fnA4QAI</t>
+  </si>
+  <si>
+    <t>a183B000000fnA5QAI</t>
+  </si>
+  <si>
+    <t>a183B000000fnA6QAI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1205,7 +1261,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1214,6 +1270,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1537,9 +1594,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="26.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1584,13 +1641,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" customWidth="1" collapsed="1"/>
-    <col min="2" max="4" width="24.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="34.42578125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="30.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="2" max="4" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="30.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -2286,10 +2343,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="35.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="35.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2402,18 +2459,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="60.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="25.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="27.85546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="26.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="29.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="60.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -3229,7 +3286,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -3271,8 +3328,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3333,7 +3390,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -3361,10 +3418,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3481,11 +3538,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3622,18 +3679,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="45.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="36.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="30.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="45.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="36.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -6888,10 +6945,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="55.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="56.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="62.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="55.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="56.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="62.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -6943,23 +7000,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="27.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="27.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -7089,19 +7146,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -7177,7 +7237,7 @@
         <v>46</v>
       </c>
       <c r="K2" t="s">
-        <v>355</v>
+        <v>383</v>
       </c>
       <c r="L2">
         <v>1000</v>
@@ -7187,6 +7247,117 @@
       </c>
       <c r="N2" t="s">
         <v>361</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>371</v>
+      </c>
+      <c r="B2" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>373</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D3" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>374</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D4" t="s">
+        <v>386</v>
       </c>
     </row>
   </sheetData>
@@ -7307,9 +7478,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -7347,9 +7518,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -7389,24 +7560,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -7531,9 +7702,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="96" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="96.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -7585,8 +7756,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -7645,11 +7816,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Pre release org details
Pre release org details
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
+++ b/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
@@ -3,8 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\auto\sahi_pro\userdata\scripts\Sahi_Project\svmx\test_lab\test_cases\optimax\op_excleData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11760" windowHeight="4815" firstSheet="22" activeTab="23"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11760" windowHeight="4815"/>
   </bookViews>
   <sheets>
     <sheet name="User_Details" sheetId="1" r:id="rId1"/>
@@ -33,9 +38,8 @@
     <sheet name="AppointmentWindow" sheetId="31" r:id="rId24"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:J14"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -43,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="378">
   <si>
     <t>UserName</t>
   </si>
@@ -999,12 +1003,6 @@
     <t>AM Load Testing</t>
   </si>
   <si>
-    <t>reena.jethmalani@svmx-cct5.org.cct5part1</t>
-  </si>
-  <si>
-    <t>salesforce@5</t>
-  </si>
-  <si>
     <t>Event Type</t>
   </si>
   <si>
@@ -1110,9 +1108,6 @@
     <t>Penalty</t>
   </si>
   <si>
-    <t>a183B000000e4O0</t>
-  </si>
-  <si>
     <t>EcoTerritoryNew</t>
   </si>
   <si>
@@ -1170,30 +1165,6 @@
     <t>AutoEvening</t>
   </si>
   <si>
-    <t>a183B000000fmeOQAQ</t>
-  </si>
-  <si>
-    <t>a183B000000fn96QAA</t>
-  </si>
-  <si>
-    <t>a183B000000fn97QAA</t>
-  </si>
-  <si>
-    <t>a183B000000fn98QAA</t>
-  </si>
-  <si>
-    <t>a183B000000fn9kQAA</t>
-  </si>
-  <si>
-    <t>a183B000000fn9pQAA</t>
-  </si>
-  <si>
-    <t>a183B000000fn9qQAA</t>
-  </si>
-  <si>
-    <t>a183B000000fn9rQAA</t>
-  </si>
-  <si>
     <t>a183B000000fn9zQAA</t>
   </si>
   <si>
@@ -1204,13 +1175,18 @@
   </si>
   <si>
     <t>a183B000000fnA6QAI</t>
+  </si>
+  <si>
+    <t>syed.abuthahir@optimax.com</t>
+  </si>
+  <si>
+    <t>servicemax2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1588,15 +1564,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="34.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="26.5703125" collapsed="true"/>
+    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1612,10 +1588,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>318</v>
+        <v>376</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>319</v>
+        <v>377</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -1624,7 +1600,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId2" display="salesforce@5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId3"/>
@@ -1641,13 +1617,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="2" max="4" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="1" max="1" width="23" customWidth="1" collapsed="1"/>
+    <col min="2" max="4" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="34.42578125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="30.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -2343,10 +2319,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="35.140625" collapsed="true"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="35.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2459,18 +2435,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="29.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="60.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="25.5703125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="27.85546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="26.28515625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="60.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="25.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="27.85546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="26.28515625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="22" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -3286,7 +3262,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -3328,8 +3304,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3390,7 +3366,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -3418,10 +3394,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="27.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3538,11 +3514,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3679,18 +3655,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="45.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="36.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="30.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="25.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="45.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="36.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="30.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="19" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -6903,33 +6879,33 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C1" t="s">
         <v>320</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>321</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>322</v>
-      </c>
-      <c r="D1" t="s">
-        <v>323</v>
-      </c>
-      <c r="E1" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>323</v>
+      </c>
+      <c r="B2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" t="s">
         <v>325</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>326</v>
-      </c>
-      <c r="C2" t="s">
-        <v>327</v>
-      </c>
-      <c r="D2" t="s">
-        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -6945,10 +6921,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="55.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="56.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="62.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="4" max="4" width="55.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="56.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="62.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -6973,10 +6949,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C2" t="s">
         <v>180</v>
@@ -6985,7 +6961,7 @@
         <v>181</v>
       </c>
       <c r="E2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F2" t="s">
         <v>184</v>
@@ -7006,17 +6982,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="27.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="27.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -7066,16 +7042,16 @@
         <v>315</v>
       </c>
       <c r="P1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="Q1" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="R1" t="s">
+        <v>361</v>
+      </c>
+      <c r="S1" t="s">
         <v>363</v>
-      </c>
-      <c r="R1" t="s">
-        <v>364</v>
-      </c>
-      <c r="S1" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -7125,16 +7101,16 @@
         <v>20</v>
       </c>
       <c r="P2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="Q2" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="R2" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="S2" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -7152,16 +7128,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="21.42578125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -7193,19 +7169,19 @@
         <v>205</v>
       </c>
       <c r="J1" t="s">
+        <v>356</v>
+      </c>
+      <c r="K1" t="s">
+        <v>351</v>
+      </c>
+      <c r="L1" t="s">
+        <v>352</v>
+      </c>
+      <c r="M1" t="s">
+        <v>357</v>
+      </c>
+      <c r="N1" t="s">
         <v>359</v>
-      </c>
-      <c r="K1" t="s">
-        <v>353</v>
-      </c>
-      <c r="L1" t="s">
-        <v>354</v>
-      </c>
-      <c r="M1" t="s">
-        <v>360</v>
-      </c>
-      <c r="N1" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -7237,7 +7213,7 @@
         <v>46</v>
       </c>
       <c r="K2" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="L2">
         <v>1000</v>
@@ -7246,7 +7222,7 @@
         <v>1</v>
       </c>
       <c r="N2" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -7256,7 +7232,7 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -7264,29 +7240,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>368</v>
       </c>
-      <c r="B1" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>371</v>
-      </c>
       <c r="B2" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:5" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>372</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7296,23 +7270,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D1" t="s">
         <v>84</v>
@@ -7320,7 +7294,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B2" s="6">
         <v>0.33333333333333331</v>
@@ -7329,12 +7303,12 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D2" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B3" s="6">
         <v>0.5</v>
@@ -7343,12 +7317,12 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="D3" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B4" s="6">
         <v>0.625</v>
@@ -7357,7 +7331,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="D4" t="s">
-        <v>386</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>
@@ -7380,69 +7354,69 @@
         <v>68</v>
       </c>
       <c r="B1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>330</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" t="s">
         <v>331</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>332</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>333</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>334</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>335</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>336</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>338</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" t="s">
         <v>339</v>
-      </c>
-      <c r="M1" t="s">
-        <v>340</v>
-      </c>
-      <c r="N1" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C2" t="s">
         <v>342</v>
       </c>
-      <c r="B2" t="s">
-        <v>343</v>
-      </c>
-      <c r="C2" t="s">
-        <v>344</v>
-      </c>
       <c r="D2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="F2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="I2">
         <v>4</v>
@@ -7457,10 +7431,10 @@
         <v>0</v>
       </c>
       <c r="M2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="N2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -7478,9 +7452,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -7496,13 +7470,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C2" t="s">
         <v>348</v>
-      </c>
-      <c r="B2" t="s">
-        <v>349</v>
-      </c>
-      <c r="C2" t="s">
-        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -7518,9 +7492,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -7536,13 +7510,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B2" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C2" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
   </sheetData>
@@ -7560,24 +7534,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -7702,9 +7676,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="96.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="1" max="1" width="96" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -7756,8 +7730,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -7816,11 +7790,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Pre release dispatch process update
Pre release dispatch process update
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
+++ b/svmx/test_lab/test_cases/optimax/op_excleData/automation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11760" windowHeight="4815"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11760" windowHeight="4815" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="User_Details" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="381">
   <si>
     <t>UserName</t>
   </si>
@@ -1181,6 +1181,15 @@
   </si>
   <si>
     <t>servicemax2</t>
+  </si>
+  <si>
+    <t>SY UK Valid Territory</t>
+  </si>
+  <si>
+    <t>a1u1g000000CsruAAC</t>
+  </si>
+  <si>
+    <t>a2Y1g000000CpgIEAS</t>
   </si>
 </sst>
 </file>
@@ -1564,7 +1573,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -7668,10 +7677,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7694,23 +7703,34 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>317</v>
+        <v>378</v>
       </c>
       <c r="B2" t="s">
-        <v>316</v>
+        <v>379</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>380</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>317</v>
+      </c>
+      <c r="B3" t="s">
+        <v>316</v>
+      </c>
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>190</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>191</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>192</v>
       </c>
     </row>

</xml_diff>